<commit_message>
New words and remove beep
</commit_message>
<xml_diff>
--- a/code/shabdakala/resource/sbwords.xlsx
+++ b/code/shabdakala/resource/sbwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/github/shabdakala/shabdakala/code/shabdakala/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F54C13-0FDC-E748-8222-46672311602D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24367EE-5B6C-4642-8CB0-5C60A74DA2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1540" yWindow="880" windowWidth="28040" windowHeight="17440" xr2:uid="{9F74AEE5-EB85-4044-AC84-8761A591B5C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="447">
   <si>
     <t>word0</t>
   </si>
@@ -260,9 +260,6 @@
     <t>संग्रहालय</t>
   </si>
   <si>
-    <t>कारावास</t>
-  </si>
-  <si>
     <t>आगा खान पॅलेस</t>
   </si>
   <si>
@@ -1170,6 +1167,213 @@
   </si>
   <si>
     <t>चीनचे प्राचीन शोध</t>
+  </si>
+  <si>
+    <t>स्थानबद्ध</t>
+  </si>
+  <si>
+    <t>मशाल</t>
+  </si>
+  <si>
+    <t>इंजिन</t>
+  </si>
+  <si>
+    <t>कमळ</t>
+  </si>
+  <si>
+    <t>घड्याळ</t>
+  </si>
+  <si>
+    <t>महाराष्ट्रातील पक्षांची निवडणूक चिन्हे</t>
+  </si>
+  <si>
+    <t>झोप</t>
+  </si>
+  <si>
+    <t>ठेच</t>
+  </si>
+  <si>
+    <t>बस</t>
+  </si>
+  <si>
+    <t>वाट</t>
+  </si>
+  <si>
+    <t>ही “लागते” :-)</t>
+  </si>
+  <si>
+    <t>संधी</t>
+  </si>
+  <si>
+    <t>जागा</t>
+  </si>
+  <si>
+    <t>ही “मिळते” :-)</t>
+  </si>
+  <si>
+    <t>तलफ</t>
+  </si>
+  <si>
+    <t>मंदी</t>
+  </si>
+  <si>
+    <t>जाग</t>
+  </si>
+  <si>
+    <t>शिंक</t>
+  </si>
+  <si>
+    <t>बहार</t>
+  </si>
+  <si>
+    <t>नंद</t>
+  </si>
+  <si>
+    <t>शिव</t>
+  </si>
+  <si>
+    <t>चार</t>
+  </si>
+  <si>
+    <t>दोन</t>
+  </si>
+  <si>
+    <t>तीन</t>
+  </si>
+  <si>
+    <t>पाच</t>
+  </si>
+  <si>
+    <t>सात</t>
+  </si>
+  <si>
+    <t>पहिल्या ४ मूळ संख्या</t>
+  </si>
+  <si>
+    <t>किरण</t>
+  </si>
+  <si>
+    <t>सुहास</t>
+  </si>
+  <si>
+    <t>चारु</t>
+  </si>
+  <si>
+    <t>शीतल</t>
+  </si>
+  <si>
+    <t>मराठी “यूनिसेक्स्” नावं</t>
+  </si>
+  <si>
+    <t>नंदा</t>
+  </si>
+  <si>
+    <t>नाथा</t>
+  </si>
+  <si>
+    <t>लखू</t>
+  </si>
+  <si>
+    <t>गजा</t>
+  </si>
+  <si>
+    <t>केदार</t>
+  </si>
+  <si>
+    <t>सारंग</t>
+  </si>
+  <si>
+    <t>कल्याण</t>
+  </si>
+  <si>
+    <t>मूळ</t>
+  </si>
+  <si>
+    <t>स्वाती</t>
+  </si>
+  <si>
+    <t>हस्त</t>
+  </si>
+  <si>
+    <t>चित्रा</t>
+  </si>
+  <si>
+    <t>नक्षत्रं</t>
+  </si>
+  <si>
+    <t>नंदी</t>
+  </si>
+  <si>
+    <t>रेडा</t>
+  </si>
+  <si>
+    <t>उंदीर</t>
+  </si>
+  <si>
+    <t>गरुड</t>
+  </si>
+  <si>
+    <t>भर</t>
+  </si>
+  <si>
+    <t>ओढ</t>
+  </si>
+  <si>
+    <t>ठेव</t>
+  </si>
+  <si>
+    <t>नामरुपे आणि क्रियेची आज्ञार्थ रुपे</t>
+  </si>
+  <si>
+    <t>उत्प्रेक्षा</t>
+  </si>
+  <si>
+    <t>यमक</t>
+  </si>
+  <si>
+    <t>रूपक</t>
+  </si>
+  <si>
+    <t>उपमा</t>
+  </si>
+  <si>
+    <t>'सदा' हा उपसर्ग लावून अर्थपूर्ण शब्द</t>
+  </si>
+  <si>
+    <t>नोकरी</t>
+  </si>
+  <si>
+    <t>सागरा धरणी</t>
+  </si>
+  <si>
+    <t xml:space="preserve">व्यक्ती आणि वल्ली' मधील काही व्यक्तिरेखा </t>
+  </si>
+  <si>
+    <t>आसावरी</t>
+  </si>
+  <si>
+    <t xml:space="preserve">काही देवांची वाहने </t>
+  </si>
+  <si>
+    <t>मराठी भाषालंकार</t>
+  </si>
+  <si>
+    <t>maths</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>काही राग</t>
+  </si>
+  <si>
+    <t>astro</t>
+  </si>
+  <si>
+    <t>mythology</t>
+  </si>
+  <si>
+    <t>ही “येते” :-)</t>
   </si>
 </sst>
 </file>
@@ -1688,7 +1892,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1696,6 +1900,7 @@
     <xf numFmtId="15" fontId="18" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1741,7 +1946,29 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2083,10 +2310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1707B-2FB7-B84C-9F84-E9F074F3056C}">
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2127,13 +2354,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>355</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>356</v>
       </c>
       <c r="L1" s="4">
         <v>45626</v>
@@ -2141,25 +2368,25 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
         <v>107</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>109</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>110</v>
       </c>
-      <c r="E2" t="s">
-        <v>111</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H2">
         <f>INT(J2/3)</f>
@@ -2174,7 +2401,7 @@
       </c>
       <c r="L2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45629</v>
+        <v>45631</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2191,13 +2418,13 @@
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="1">INT(J3/3)</f>
@@ -2215,25 +2442,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
         <v>144</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>145</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>146</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>147</v>
       </c>
-      <c r="E4" t="s">
-        <v>148</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
@@ -2251,25 +2478,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B5" t="s">
         <v>268</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>269</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>270</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>271</v>
       </c>
-      <c r="E5" t="s">
-        <v>272</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -2287,25 +2514,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>84</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>85</v>
       </c>
-      <c r="E6" t="s">
-        <v>86</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
@@ -2323,25 +2550,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
         <v>122</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>123</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>124</v>
       </c>
-      <c r="E7" t="s">
-        <v>125</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
@@ -2359,25 +2586,25 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" t="s">
         <v>347</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>348</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>349</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>350</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>351</v>
       </c>
-      <c r="F8" t="s">
-        <v>352</v>
-      </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -2394,32 +2621,32 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>336</v>
+      </c>
+      <c r="B9" t="s">
         <v>337</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>338</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>339</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>340</v>
       </c>
-      <c r="E9" t="s">
-        <v>341</v>
-      </c>
       <c r="F9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I9" s="3">
-        <f t="shared" ref="I9:I71" si="3">$L$1+H9</f>
+        <f t="shared" ref="I9:I84" si="3">$L$1+H9</f>
         <v>45628</v>
       </c>
       <c r="J9">
@@ -2429,25 +2656,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>341</v>
+      </c>
+      <c r="B10" t="s">
         <v>342</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>343</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>344</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>345</v>
       </c>
-      <c r="E10" t="s">
-        <v>346</v>
-      </c>
       <c r="F10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
@@ -2464,25 +2691,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D11" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E11" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
@@ -2499,28 +2726,28 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12" t="s">
         <v>361</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>368</v>
+      </c>
+      <c r="D12" t="s">
         <v>362</v>
       </c>
-      <c r="C12" t="s">
-        <v>369</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>363</v>
       </c>
-      <c r="E12" t="s">
-        <v>364</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H12:H74" si="5">INT(J12/3)</f>
+        <f t="shared" ref="H12:H87" si="5">INT(J12/3)</f>
         <v>3</v>
       </c>
       <c r="I12" s="3">
@@ -2528,31 +2755,31 @@
         <v>45629</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J74" si="6">J11+1</f>
+        <f t="shared" ref="J12:J87" si="6">J11+1</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" t="s">
         <v>365</v>
       </c>
-      <c r="B13" t="s">
-        <v>238</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>366</v>
       </c>
-      <c r="D13" t="s">
-        <v>367</v>
-      </c>
       <c r="E13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
@@ -2569,25 +2796,25 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s">
         <v>139</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>140</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>141</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>142</v>
       </c>
-      <c r="E14" t="s">
-        <v>143</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H14">
         <f t="shared" si="5"/>
@@ -2604,25 +2831,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="s">
         <v>97</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>98</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>100</v>
       </c>
-      <c r="E15" t="s">
-        <v>101</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H15">
         <f t="shared" si="5"/>
@@ -2651,13 +2878,13 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="H16">
         <f t="shared" si="5"/>
@@ -2686,10 +2913,10 @@
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>53</v>
@@ -2709,25 +2936,25 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
         <v>126</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>127</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>128</v>
       </c>
-      <c r="E18" t="s">
-        <v>129</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H18">
         <f t="shared" si="5"/>
@@ -2759,7 +2986,7 @@
         <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>12</v>
@@ -2779,25 +3006,25 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B20" t="s">
         <v>165</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>166</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>167</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>168</v>
       </c>
-      <c r="E20" t="s">
-        <v>169</v>
-      </c>
       <c r="F20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H20">
         <f t="shared" si="5"/>
@@ -2814,25 +3041,25 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" t="s">
         <v>109</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>110</v>
       </c>
-      <c r="E21" t="s">
-        <v>111</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H21">
         <f t="shared" si="5"/>
@@ -2849,25 +3076,25 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" t="s">
         <v>144</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>145</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>146</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>147</v>
       </c>
-      <c r="E22" t="s">
-        <v>148</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H22">
         <f t="shared" ref="H22:H23" si="7">INT(J22/3)</f>
@@ -2899,17 +3126,17 @@
         <v>48</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H23">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="H23:H86" si="9">INT(J23/3)</f>
         <v>7</v>
       </c>
       <c r="I23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="I23:I86" si="10">$L$1+H23</f>
         <v>45633</v>
       </c>
       <c r="J23">
@@ -2934,17 +3161,17 @@
         <v>41</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45633</v>
       </c>
       <c r="J24">
@@ -2954,32 +3181,32 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>379</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>380</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>381</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>382</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>94</v>
+        <v>383</v>
+      </c>
+      <c r="F25" t="s">
+        <v>414</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
       <c r="H25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="I25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45633</v>
       </c>
       <c r="J25">
@@ -2989,32 +3216,32 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>263</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>264</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
-        <v>265</v>
+        <v>135</v>
       </c>
       <c r="D26" t="s">
-        <v>266</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s">
-        <v>267</v>
+        <v>137</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="H26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45634</v>
       </c>
       <c r="J26">
@@ -3024,32 +3251,32 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>262</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>264</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>265</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>266</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="H27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="I27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45634</v>
       </c>
       <c r="J27">
@@ -3059,32 +3286,32 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>422</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>423</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>424</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>425</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>94</v>
+        <v>439</v>
+      </c>
+      <c r="F28" t="s">
+        <v>414</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>150</v>
+        <v>445</v>
       </c>
       <c r="H28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="I28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45634</v>
       </c>
       <c r="J28">
@@ -3094,32 +3321,32 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>277</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>279</v>
+        <v>103</v>
       </c>
       <c r="D29" t="s">
-        <v>280</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>281</v>
+        <v>105</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="H29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="I29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45635</v>
       </c>
       <c r="J29">
@@ -3129,32 +3356,32 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="E30" t="s">
-        <v>372</v>
+        <v>115</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="H30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="I30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45635</v>
       </c>
       <c r="J30">
@@ -3164,32 +3391,32 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>276</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>277</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="D31" t="s">
-        <v>38</v>
+        <v>279</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>280</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>353</v>
+        <v>93</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="I31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45635</v>
       </c>
       <c r="J31">
@@ -3199,32 +3426,32 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>121</v>
+        <v>371</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>152</v>
+        <v>54</v>
       </c>
       <c r="H32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="I32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45636</v>
       </c>
       <c r="J32">
@@ -3234,32 +3461,32 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>214</v>
+        <v>384</v>
       </c>
       <c r="B33" t="s">
-        <v>215</v>
+        <v>385</v>
       </c>
       <c r="C33" t="s">
-        <v>216</v>
+        <v>386</v>
       </c>
       <c r="D33" t="s">
-        <v>217</v>
+        <v>387</v>
       </c>
       <c r="E33" t="s">
-        <v>218</v>
+        <v>388</v>
       </c>
       <c r="F33" t="s">
-        <v>262</v>
+        <v>414</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>154</v>
+        <v>286</v>
       </c>
       <c r="H33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="I33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45636</v>
       </c>
       <c r="J33">
@@ -3269,32 +3496,32 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="E34" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>94</v>
+        <v>352</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="H34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="I34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45636</v>
       </c>
       <c r="J34">
@@ -3304,32 +3531,32 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>205</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="D35" t="s">
-        <v>207</v>
+        <v>119</v>
       </c>
       <c r="E35" t="s">
-        <v>208</v>
-      </c>
-      <c r="F35" t="s">
-        <v>262</v>
+        <v>120</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="H35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="I35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45637</v>
       </c>
       <c r="J35">
@@ -3339,32 +3566,32 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>213</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>214</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>215</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>216</v>
       </c>
       <c r="E36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>94</v>
+        <v>217</v>
+      </c>
+      <c r="F36" t="s">
+        <v>261</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
       <c r="H36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="I36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45637</v>
       </c>
       <c r="J36">
@@ -3374,32 +3601,32 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>199</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>201</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>202</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>203</v>
-      </c>
-      <c r="F37" t="s">
-        <v>262</v>
+        <v>90</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45637</v>
       </c>
       <c r="J37">
@@ -3408,33 +3635,33 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>42.195</v>
+      <c r="A38" t="s">
+        <v>436</v>
       </c>
       <c r="B38" t="s">
-        <v>130</v>
+        <v>389</v>
       </c>
       <c r="C38" t="s">
-        <v>131</v>
+        <v>390</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>435</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>94</v>
+        <v>391</v>
+      </c>
+      <c r="F38" t="s">
+        <v>414</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>153</v>
+        <v>286</v>
       </c>
       <c r="H38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45638</v>
       </c>
       <c r="J38">
@@ -3444,32 +3671,32 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>204</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>205</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>206</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>353</v>
+        <v>207</v>
+      </c>
+      <c r="F39" t="s">
+        <v>261</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="H39">
-        <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
       <c r="I39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45638</v>
       </c>
       <c r="J39">
@@ -3479,32 +3706,32 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>177</v>
+        <v>74</v>
       </c>
       <c r="D40" t="s">
-        <v>178</v>
+        <v>378</v>
       </c>
       <c r="E40" t="s">
-        <v>179</v>
-      </c>
-      <c r="F40" t="s">
-        <v>195</v>
+        <v>75</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>198</v>
+        <v>54</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45638</v>
       </c>
       <c r="J40">
@@ -3514,32 +3741,32 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="C41" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="D41" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="F41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>288</v>
+        <v>95</v>
       </c>
       <c r="H41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45639</v>
       </c>
       <c r="J41">
@@ -3549,32 +3776,32 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>243</v>
+        <v>426</v>
       </c>
       <c r="B42" t="s">
-        <v>244</v>
+        <v>427</v>
       </c>
       <c r="C42" t="s">
-        <v>245</v>
+        <v>428</v>
       </c>
       <c r="D42" t="s">
-        <v>246</v>
+        <v>386</v>
       </c>
       <c r="E42" t="s">
-        <v>247</v>
+        <v>429</v>
       </c>
       <c r="F42" t="s">
-        <v>262</v>
+        <v>414</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>150</v>
+        <v>286</v>
       </c>
       <c r="H42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45639</v>
       </c>
       <c r="J42">
@@ -3583,33 +3810,33 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>35</v>
+      <c r="A43" s="2">
+        <v>42.195</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="E43" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>353</v>
+        <v>93</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>55</v>
+        <v>152</v>
       </c>
       <c r="H43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45639</v>
       </c>
       <c r="J43">
@@ -3619,32 +3846,32 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>219</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>220</v>
+        <v>44</v>
       </c>
       <c r="D44" t="s">
-        <v>221</v>
+        <v>45</v>
       </c>
       <c r="E44" t="s">
-        <v>222</v>
-      </c>
-      <c r="F44" t="s">
-        <v>262</v>
+        <v>46</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>287</v>
+        <v>12</v>
       </c>
       <c r="H44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45640</v>
       </c>
       <c r="J44">
@@ -3654,32 +3881,32 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>322</v>
+        <v>174</v>
       </c>
       <c r="B45" t="s">
-        <v>323</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
-        <v>324</v>
+        <v>176</v>
       </c>
       <c r="D45" t="s">
-        <v>325</v>
+        <v>177</v>
       </c>
       <c r="E45" t="s">
-        <v>330</v>
+        <v>178</v>
       </c>
       <c r="F45" t="s">
-        <v>331</v>
+        <v>194</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>149</v>
+        <v>197</v>
       </c>
       <c r="H45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45640</v>
       </c>
       <c r="J45">
@@ -3689,32 +3916,32 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>160</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>223</v>
       </c>
       <c r="C46" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="D46" t="s">
-        <v>163</v>
+        <v>225</v>
       </c>
       <c r="E46" t="s">
-        <v>164</v>
+        <v>226</v>
       </c>
       <c r="F46" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>197</v>
+        <v>287</v>
       </c>
       <c r="H46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45640</v>
       </c>
       <c r="J46">
@@ -3723,33 +3950,33 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>353</v>
+      <c r="A47" t="s">
+        <v>392</v>
+      </c>
+      <c r="B47" t="s">
+        <v>393</v>
+      </c>
+      <c r="C47" t="s">
+        <v>394</v>
+      </c>
+      <c r="D47" t="s">
+        <v>395</v>
+      </c>
+      <c r="E47" t="s">
+        <v>446</v>
+      </c>
+      <c r="F47" t="s">
+        <v>414</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>12</v>
+        <v>286</v>
       </c>
       <c r="H47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45641</v>
       </c>
       <c r="J47">
@@ -3759,32 +3986,32 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="B48" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="C48" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="D48" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="E48" t="s">
+        <v>246</v>
+      </c>
+      <c r="F48" t="s">
         <v>261</v>
       </c>
-      <c r="F48" t="s">
-        <v>262</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45641</v>
       </c>
       <c r="J48">
@@ -3794,32 +4021,32 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>290</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>291</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>292</v>
+        <v>51</v>
       </c>
       <c r="D49" t="s">
-        <v>293</v>
+        <v>50</v>
       </c>
       <c r="E49" t="s">
-        <v>330</v>
-      </c>
-      <c r="F49" t="s">
-        <v>331</v>
+        <v>37</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>149</v>
+        <v>55</v>
       </c>
       <c r="H49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45641</v>
       </c>
       <c r="J49">
@@ -3829,32 +4056,32 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>305</v>
+        <v>56</v>
       </c>
       <c r="B50" t="s">
-        <v>306</v>
+        <v>218</v>
       </c>
       <c r="C50" t="s">
-        <v>307</v>
+        <v>219</v>
       </c>
       <c r="D50" t="s">
-        <v>308</v>
+        <v>220</v>
       </c>
       <c r="E50" t="s">
-        <v>309</v>
+        <v>221</v>
       </c>
       <c r="F50" t="s">
-        <v>331</v>
+        <v>261</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>53</v>
+        <v>286</v>
       </c>
       <c r="H50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45642</v>
       </c>
       <c r="J50">
@@ -3864,32 +4091,32 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>301</v>
+        <v>321</v>
       </c>
       <c r="B51" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
       <c r="C51" t="s">
-        <v>303</v>
+        <v>323</v>
       </c>
       <c r="D51" t="s">
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="E51" t="s">
+        <v>329</v>
+      </c>
+      <c r="F51" t="s">
         <v>330</v>
       </c>
-      <c r="F51" t="s">
-        <v>331</v>
-      </c>
       <c r="G51" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45642</v>
       </c>
       <c r="J51">
@@ -3899,32 +4126,32 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>332</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
-        <v>333</v>
+        <v>160</v>
       </c>
       <c r="C52" t="s">
-        <v>334</v>
+        <v>161</v>
       </c>
       <c r="D52" t="s">
-        <v>335</v>
+        <v>162</v>
       </c>
       <c r="E52" t="s">
-        <v>336</v>
+        <v>163</v>
       </c>
       <c r="F52" t="s">
-        <v>331</v>
+        <v>194</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="H52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45642</v>
       </c>
       <c r="J52">
@@ -3934,32 +4161,32 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>396</v>
       </c>
       <c r="B53" t="s">
-        <v>294</v>
+        <v>397</v>
       </c>
       <c r="C53" t="s">
-        <v>295</v>
+        <v>398</v>
       </c>
       <c r="D53" t="s">
-        <v>296</v>
+        <v>399</v>
       </c>
       <c r="E53" t="s">
-        <v>330</v>
+        <v>434</v>
       </c>
       <c r="F53" t="s">
-        <v>331</v>
+        <v>414</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>149</v>
+        <v>286</v>
       </c>
       <c r="H53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45643</v>
       </c>
       <c r="J53">
@@ -3969,32 +4196,32 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>233</v>
+        <v>417</v>
       </c>
       <c r="B54" t="s">
-        <v>234</v>
+        <v>418</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>419</v>
       </c>
       <c r="D54" t="s">
-        <v>236</v>
+        <v>420</v>
       </c>
       <c r="E54" t="s">
-        <v>237</v>
+        <v>421</v>
       </c>
       <c r="F54" t="s">
-        <v>262</v>
+        <v>414</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>149</v>
+        <v>444</v>
       </c>
       <c r="H54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="I54" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45643</v>
       </c>
       <c r="J54">
@@ -4003,33 +4230,33 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>326</v>
-      </c>
-      <c r="B55" t="s">
-        <v>327</v>
-      </c>
-      <c r="C55" t="s">
-        <v>328</v>
-      </c>
-      <c r="D55" t="s">
-        <v>329</v>
-      </c>
-      <c r="E55" t="s">
-        <v>330</v>
-      </c>
-      <c r="F55" t="s">
-        <v>331</v>
+      <c r="A55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>149</v>
+        <v>12</v>
       </c>
       <c r="H55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45643</v>
       </c>
       <c r="J55">
@@ -4039,32 +4266,32 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>256</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>257</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>258</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
       <c r="E56" t="s">
-        <v>174</v>
+        <v>260</v>
       </c>
       <c r="F56" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45644</v>
       </c>
       <c r="J56">
@@ -4074,32 +4301,32 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>180</v>
+        <v>430</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>431</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>432</v>
       </c>
       <c r="D57" t="s">
-        <v>183</v>
+        <v>433</v>
       </c>
       <c r="E57" t="s">
-        <v>184</v>
+        <v>440</v>
       </c>
       <c r="F57" t="s">
-        <v>195</v>
+        <v>414</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>149</v>
+        <v>286</v>
       </c>
       <c r="H57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="I57" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45644</v>
       </c>
       <c r="J57">
@@ -4109,32 +4336,32 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>209</v>
+        <v>289</v>
       </c>
       <c r="B58" t="s">
-        <v>210</v>
+        <v>290</v>
       </c>
       <c r="C58" t="s">
-        <v>211</v>
+        <v>291</v>
       </c>
       <c r="D58" t="s">
-        <v>212</v>
+        <v>292</v>
       </c>
       <c r="E58" t="s">
-        <v>213</v>
+        <v>329</v>
       </c>
       <c r="F58" t="s">
-        <v>262</v>
+        <v>330</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45644</v>
       </c>
       <c r="J58">
@@ -4144,32 +4371,32 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="B59" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="C59" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="D59" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="E59" t="s">
+        <v>308</v>
+      </c>
+      <c r="F59" t="s">
         <v>330</v>
       </c>
-      <c r="F59" t="s">
-        <v>331</v>
-      </c>
       <c r="G59" s="1" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="H59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="I59" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45645</v>
       </c>
       <c r="J59">
@@ -4179,32 +4406,32 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>301</v>
       </c>
       <c r="C60" t="s">
-        <v>32</v>
+        <v>302</v>
       </c>
       <c r="D60" t="s">
-        <v>33</v>
+        <v>303</v>
       </c>
       <c r="E60" t="s">
-        <v>34</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>353</v>
+        <v>329</v>
+      </c>
+      <c r="F60" t="s">
+        <v>330</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="H60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45645</v>
       </c>
       <c r="J60">
@@ -4214,32 +4441,32 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>190</v>
+        <v>331</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>332</v>
       </c>
       <c r="C61" t="s">
-        <v>192</v>
+        <v>333</v>
       </c>
       <c r="D61" t="s">
-        <v>193</v>
+        <v>334</v>
       </c>
       <c r="E61" t="s">
-        <v>194</v>
+        <v>335</v>
       </c>
       <c r="F61" t="s">
-        <v>195</v>
+        <v>330</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="H61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45645</v>
       </c>
       <c r="J61">
@@ -4252,29 +4479,29 @@
         <v>56</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>293</v>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
+        <v>294</v>
       </c>
       <c r="D62" t="s">
-        <v>59</v>
+        <v>295</v>
       </c>
       <c r="E62" t="s">
-        <v>60</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>94</v>
+        <v>329</v>
+      </c>
+      <c r="F62" t="s">
+        <v>330</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>95</v>
+        <v>148</v>
       </c>
       <c r="H62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="I62" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45646</v>
       </c>
       <c r="J62">
@@ -4284,32 +4511,32 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>238</v>
+        <v>400</v>
       </c>
       <c r="B63" t="s">
-        <v>239</v>
+        <v>401</v>
       </c>
       <c r="C63" t="s">
-        <v>240</v>
+        <v>402</v>
       </c>
       <c r="D63" t="s">
-        <v>241</v>
+        <v>403</v>
       </c>
       <c r="E63" t="s">
-        <v>242</v>
+        <v>404</v>
       </c>
       <c r="F63" t="s">
-        <v>262</v>
+        <v>414</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>289</v>
+        <v>441</v>
       </c>
       <c r="H63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="I63" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45646</v>
       </c>
       <c r="J63">
@@ -4319,32 +4546,32 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="B64" t="s">
-        <v>186</v>
+        <v>233</v>
       </c>
       <c r="C64" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="D64" t="s">
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="E64" t="s">
-        <v>189</v>
+        <v>236</v>
       </c>
       <c r="F64" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="H64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45646</v>
       </c>
       <c r="J64">
@@ -4354,32 +4581,32 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>282</v>
+        <v>325</v>
       </c>
       <c r="B65" t="s">
-        <v>283</v>
+        <v>326</v>
       </c>
       <c r="C65" t="s">
-        <v>284</v>
+        <v>327</v>
       </c>
       <c r="D65" t="s">
-        <v>285</v>
+        <v>328</v>
       </c>
       <c r="E65" t="s">
-        <v>286</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>94</v>
+        <v>329</v>
+      </c>
+      <c r="F65" t="s">
+        <v>330</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="H65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="I65" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45647</v>
       </c>
       <c r="J65">
@@ -4389,32 +4616,32 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>248</v>
+        <v>169</v>
       </c>
       <c r="B66" t="s">
-        <v>249</v>
+        <v>170</v>
       </c>
       <c r="C66" t="s">
-        <v>250</v>
+        <v>171</v>
       </c>
       <c r="D66" t="s">
-        <v>251</v>
+        <v>172</v>
       </c>
       <c r="E66" t="s">
-        <v>252</v>
+        <v>173</v>
       </c>
       <c r="F66" t="s">
-        <v>262</v>
+        <v>194</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="H66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="I66" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45647</v>
       </c>
       <c r="J66">
@@ -4424,32 +4651,32 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>318</v>
+        <v>179</v>
       </c>
       <c r="B67" t="s">
-        <v>319</v>
+        <v>180</v>
       </c>
       <c r="C67" t="s">
-        <v>320</v>
+        <v>181</v>
       </c>
       <c r="D67" t="s">
-        <v>321</v>
+        <v>182</v>
       </c>
       <c r="E67" t="s">
-        <v>330</v>
+        <v>183</v>
       </c>
       <c r="F67" t="s">
-        <v>331</v>
+        <v>194</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="I67" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45647</v>
       </c>
       <c r="J67">
@@ -4459,32 +4686,32 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>373</v>
+        <v>208</v>
       </c>
       <c r="B68" t="s">
-        <v>374</v>
+        <v>209</v>
       </c>
       <c r="C68" t="s">
-        <v>297</v>
+        <v>210</v>
       </c>
       <c r="D68" t="s">
-        <v>298</v>
+        <v>211</v>
       </c>
       <c r="E68" t="s">
-        <v>330</v>
+        <v>212</v>
       </c>
       <c r="F68" t="s">
-        <v>331</v>
+        <v>261</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="I68" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45648</v>
       </c>
       <c r="J68">
@@ -4494,32 +4721,32 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>273</v>
+        <v>313</v>
       </c>
       <c r="B69" t="s">
-        <v>274</v>
+        <v>314</v>
       </c>
       <c r="C69" t="s">
-        <v>275</v>
+        <v>315</v>
       </c>
       <c r="D69" t="s">
-        <v>255</v>
+        <v>316</v>
       </c>
       <c r="E69" t="s">
-        <v>276</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>94</v>
+        <v>329</v>
+      </c>
+      <c r="F69" t="s">
+        <v>330</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="H69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="I69" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45648</v>
       </c>
       <c r="J69">
@@ -4529,32 +4756,32 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>214</v>
+        <v>405</v>
       </c>
       <c r="B70" t="s">
-        <v>253</v>
+        <v>406</v>
       </c>
       <c r="C70" t="s">
-        <v>254</v>
+        <v>407</v>
       </c>
       <c r="D70" t="s">
-        <v>255</v>
+        <v>408</v>
       </c>
       <c r="E70" t="s">
-        <v>256</v>
+        <v>409</v>
       </c>
       <c r="F70" t="s">
-        <v>262</v>
+        <v>414</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>152</v>
+        <v>286</v>
       </c>
       <c r="H70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="I70" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45648</v>
       </c>
       <c r="J70">
@@ -4564,32 +4791,32 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>299</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>375</v>
+        <v>31</v>
       </c>
       <c r="C71" t="s">
-        <v>300</v>
+        <v>32</v>
       </c>
       <c r="D71" t="s">
-        <v>376</v>
+        <v>33</v>
       </c>
       <c r="E71" t="s">
-        <v>330</v>
-      </c>
-      <c r="F71" t="s">
-        <v>331</v>
+        <v>34</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>149</v>
+        <v>54</v>
       </c>
       <c r="H71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="I71" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="10"/>
         <v>45649</v>
       </c>
       <c r="J71">
@@ -4599,32 +4826,32 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>310</v>
+        <v>189</v>
       </c>
       <c r="B72" t="s">
-        <v>311</v>
+        <v>190</v>
       </c>
       <c r="C72" t="s">
-        <v>312</v>
+        <v>191</v>
       </c>
       <c r="D72" t="s">
-        <v>313</v>
+        <v>192</v>
       </c>
       <c r="E72" t="s">
-        <v>330</v>
+        <v>193</v>
       </c>
       <c r="F72" t="s">
-        <v>331</v>
+        <v>194</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="H72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="I72" s="3">
-        <f t="shared" ref="I72:I75" si="9">$L$1+H72</f>
+        <f t="shared" si="10"/>
         <v>45649</v>
       </c>
       <c r="J72">
@@ -4634,32 +4861,32 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>228</v>
+        <v>56</v>
       </c>
       <c r="B73" t="s">
-        <v>229</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
-        <v>230</v>
+        <v>58</v>
       </c>
       <c r="D73" t="s">
-        <v>231</v>
+        <v>59</v>
       </c>
       <c r="E73" t="s">
-        <v>232</v>
-      </c>
-      <c r="F73" t="s">
-        <v>262</v>
+        <v>60</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="H73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="I73" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45649</v>
       </c>
       <c r="J73">
@@ -4669,32 +4896,32 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>237</v>
       </c>
       <c r="B74" t="s">
-        <v>156</v>
+        <v>238</v>
       </c>
       <c r="C74" t="s">
-        <v>157</v>
+        <v>239</v>
       </c>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>240</v>
       </c>
       <c r="E74" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
       <c r="F74" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>196</v>
+        <v>288</v>
       </c>
       <c r="H74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="I74" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>45650</v>
       </c>
       <c r="J74">
@@ -4704,46 +4931,509 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>184</v>
+      </c>
+      <c r="B75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" t="s">
+        <v>186</v>
+      </c>
+      <c r="D75" t="s">
+        <v>187</v>
+      </c>
+      <c r="E75" t="s">
+        <v>188</v>
+      </c>
+      <c r="F75" t="s">
+        <v>194</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="shared" si="10"/>
+        <v>45650</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="6"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>410</v>
+      </c>
+      <c r="B76" t="s">
+        <v>411</v>
+      </c>
+      <c r="C76" t="s">
+        <v>412</v>
+      </c>
+      <c r="D76" t="s">
+        <v>413</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="F76" t="s">
+        <v>414</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="shared" si="10"/>
+        <v>45650</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="6"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>281</v>
+      </c>
+      <c r="B77" t="s">
+        <v>282</v>
+      </c>
+      <c r="C77" t="s">
+        <v>283</v>
+      </c>
+      <c r="D77" t="s">
+        <v>284</v>
+      </c>
+      <c r="E77" t="s">
+        <v>285</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="I77" s="3">
+        <f t="shared" si="10"/>
+        <v>45651</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>247</v>
+      </c>
+      <c r="B78" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" t="s">
+        <v>249</v>
+      </c>
+      <c r="D78" t="s">
+        <v>250</v>
+      </c>
+      <c r="E78" t="s">
+        <v>251</v>
+      </c>
+      <c r="F78" t="s">
+        <v>261</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="I78" s="3">
+        <f t="shared" si="10"/>
+        <v>45651</v>
+      </c>
+      <c r="J78">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" t="s">
+        <v>319</v>
+      </c>
+      <c r="D79" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" t="s">
+        <v>329</v>
+      </c>
+      <c r="F79" t="s">
+        <v>330</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="I79" s="3">
+        <f t="shared" si="10"/>
+        <v>45651</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="6"/>
         <v>77</v>
       </c>
-      <c r="B75" t="s">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>372</v>
+      </c>
+      <c r="B80" t="s">
+        <v>373</v>
+      </c>
+      <c r="C80" t="s">
+        <v>296</v>
+      </c>
+      <c r="D80" t="s">
+        <v>297</v>
+      </c>
+      <c r="E80" t="s">
+        <v>329</v>
+      </c>
+      <c r="F80" t="s">
+        <v>330</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="I80" s="3">
+        <f t="shared" si="10"/>
+        <v>45652</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="6"/>
         <v>78</v>
       </c>
-      <c r="C75" t="s">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>414</v>
+      </c>
+      <c r="B81" t="s">
+        <v>438</v>
+      </c>
+      <c r="C81" t="s">
+        <v>415</v>
+      </c>
+      <c r="D81" t="s">
+        <v>416</v>
+      </c>
+      <c r="E81" t="s">
+        <v>443</v>
+      </c>
+      <c r="F81" t="s">
+        <v>414</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="I81" s="3">
+        <f t="shared" si="10"/>
+        <v>45652</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
-      <c r="D75" t="s">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>272</v>
+      </c>
+      <c r="B82" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82" t="s">
+        <v>274</v>
+      </c>
+      <c r="D82" t="s">
+        <v>254</v>
+      </c>
+      <c r="E82" t="s">
+        <v>275</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="I82" s="3">
+        <f t="shared" si="10"/>
+        <v>45652</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="6"/>
         <v>80</v>
       </c>
-      <c r="E75" t="s">
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>213</v>
+      </c>
+      <c r="B83" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" t="s">
+        <v>253</v>
+      </c>
+      <c r="D83" t="s">
+        <v>254</v>
+      </c>
+      <c r="E83" t="s">
+        <v>255</v>
+      </c>
+      <c r="F83" t="s">
+        <v>261</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="I83" s="3">
+        <f t="shared" si="10"/>
+        <v>45653</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="6"/>
         <v>81</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H75">
-        <f t="shared" ref="H75" si="10">INT(J75/3)</f>
-        <v>24</v>
-      </c>
-      <c r="I75" s="3">
-        <f t="shared" si="9"/>
-        <v>45650</v>
-      </c>
-      <c r="J75">
-        <f t="shared" ref="J75" si="11">J74+1</f>
-        <v>73</v>
-      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>298</v>
+      </c>
+      <c r="B84" t="s">
+        <v>374</v>
+      </c>
+      <c r="C84" t="s">
+        <v>299</v>
+      </c>
+      <c r="D84" t="s">
+        <v>375</v>
+      </c>
+      <c r="E84" t="s">
+        <v>329</v>
+      </c>
+      <c r="F84" t="s">
+        <v>330</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="I84" s="3">
+        <f t="shared" si="10"/>
+        <v>45653</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="6"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>309</v>
+      </c>
+      <c r="B85" t="s">
+        <v>310</v>
+      </c>
+      <c r="C85" t="s">
+        <v>311</v>
+      </c>
+      <c r="D85" t="s">
+        <v>312</v>
+      </c>
+      <c r="E85" t="s">
+        <v>329</v>
+      </c>
+      <c r="F85" t="s">
+        <v>330</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="9"/>
+        <v>27</v>
+      </c>
+      <c r="I85" s="3">
+        <f t="shared" si="10"/>
+        <v>45653</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="6"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>227</v>
+      </c>
+      <c r="B86" t="s">
+        <v>228</v>
+      </c>
+      <c r="C86" t="s">
+        <v>229</v>
+      </c>
+      <c r="D86" t="s">
+        <v>230</v>
+      </c>
+      <c r="E86" t="s">
+        <v>231</v>
+      </c>
+      <c r="F86" t="s">
+        <v>261</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="I86" s="3">
+        <f t="shared" si="10"/>
+        <v>45654</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="6"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" t="s">
+        <v>156</v>
+      </c>
+      <c r="D87" t="s">
+        <v>157</v>
+      </c>
+      <c r="E87" t="s">
+        <v>158</v>
+      </c>
+      <c r="F87" t="s">
+        <v>194</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H87">
+        <f t="shared" ref="H87:H88" si="11">INT(J87/3)</f>
+        <v>28</v>
+      </c>
+      <c r="I87" s="3">
+        <f t="shared" ref="I87:I88" si="12">$L$1+H87</f>
+        <v>45654</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>76</v>
+      </c>
+      <c r="B88" t="s">
+        <v>77</v>
+      </c>
+      <c r="C88" t="s">
+        <v>78</v>
+      </c>
+      <c r="D88" t="s">
+        <v>79</v>
+      </c>
+      <c r="E88" t="s">
+        <v>80</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="11"/>
+        <v>28</v>
+      </c>
+      <c r="I88" s="3">
+        <f t="shared" si="12"/>
+        <v>45654</v>
+      </c>
+      <c r="J88">
+        <f t="shared" ref="J88" si="13">J87+1</f>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F89" s="1"/>
+      <c r="G89" s="1"/>
+      <c r="I89" s="3"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H78">
-    <sortCondition ref="H8:H78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:H91">
+    <sortCondition ref="H8:H91"/>
   </sortState>
-  <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="I99:I1048576 I1:I89">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
       <formula>$L$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="equal">
+      <formula>$L$2+1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Corrected a few words
</commit_message>
<xml_diff>
--- a/code/shabdakala/resource/sbwords.xlsx
+++ b/code/shabdakala/resource/sbwords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/github/shabdakala/shabdakala/code/shabdakala/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD68B72C-FD4A-144E-BDA5-D17FB9AFD52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB145A-9BAA-C64C-85BA-EDF72D9798A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9F74AEE5-EB85-4044-AC84-8761A591B5C1}"/>
   </bookViews>
@@ -146,9 +146,6 @@
     <t>मुंबई</t>
   </si>
   <si>
-    <t>दोरी</t>
-  </si>
-  <si>
     <t xml:space="preserve"> सुळका</t>
   </si>
   <si>
@@ -407,9 +404,6 @@
     <t xml:space="preserve"> अथेन्स</t>
   </si>
   <si>
-    <t xml:space="preserve"> धावक</t>
-  </si>
-  <si>
     <t>कीपटूम</t>
   </si>
   <si>
@@ -686,9 +680,6 @@
     <t>अमूल</t>
   </si>
   <si>
-    <t>कात्रज</t>
-  </si>
-  <si>
     <t>म्हैस</t>
   </si>
   <si>
@@ -2022,6 +2013,15 @@
   </si>
   <si>
     <t>रस्ता</t>
+  </si>
+  <si>
+    <t>केनिया</t>
+  </si>
+  <si>
+    <t>दोर</t>
+  </si>
+  <si>
+    <t>गवळी</t>
   </si>
 </sst>
 </file>
@@ -2948,8 +2948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1707B-2FB7-B84C-9F84-E9F074F3056C}">
   <dimension ref="A1:L135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2990,13 +2990,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="L1" s="4">
         <v>45625</v>
@@ -3004,25 +3004,25 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
         <v>101</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>103</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>104</v>
       </c>
-      <c r="E2" t="s">
-        <v>105</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H2">
         <f>INT(J2/3)</f>
@@ -3037,30 +3037,30 @@
       </c>
       <c r="L2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45638</v>
+        <v>45640</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H11" si="1">INT(J3/3)</f>
@@ -3078,25 +3078,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
         <v>137</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>138</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>139</v>
       </c>
-      <c r="D4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" t="s">
-        <v>141</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H4">
         <f t="shared" si="1"/>
@@ -3114,25 +3114,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D5" t="s">
         <v>261</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>262</v>
       </c>
-      <c r="C5" t="s">
-        <v>263</v>
-      </c>
-      <c r="D5" t="s">
-        <v>264</v>
-      </c>
-      <c r="E5" t="s">
-        <v>265</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
@@ -3150,25 +3150,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
         <v>76</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>77</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>78</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>79</v>
       </c>
-      <c r="E6" t="s">
-        <v>80</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
@@ -3186,25 +3186,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
         <v>115</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>116</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>117</v>
       </c>
-      <c r="E7" t="s">
-        <v>118</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
@@ -3222,25 +3222,25 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D8" t="s">
         <v>340</v>
       </c>
-      <c r="B8" t="s">
+      <c r="E8" t="s">
         <v>341</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>342</v>
       </c>
-      <c r="D8" t="s">
-        <v>343</v>
-      </c>
-      <c r="E8" t="s">
-        <v>344</v>
-      </c>
-      <c r="F8" t="s">
-        <v>345</v>
-      </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
@@ -3257,25 +3257,25 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D9" t="s">
         <v>330</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>331</v>
       </c>
-      <c r="C9" t="s">
-        <v>332</v>
-      </c>
-      <c r="D9" t="s">
-        <v>333</v>
-      </c>
-      <c r="E9" t="s">
-        <v>334</v>
-      </c>
       <c r="F9" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
@@ -3292,25 +3292,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" t="s">
+        <v>334</v>
+      </c>
+      <c r="D10" t="s">
         <v>335</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>336</v>
       </c>
-      <c r="C10" t="s">
-        <v>337</v>
-      </c>
-      <c r="D10" t="s">
-        <v>338</v>
-      </c>
-      <c r="E10" t="s">
-        <v>339</v>
-      </c>
       <c r="F10" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
@@ -3327,25 +3327,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B11" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C11" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D11" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="E11" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
@@ -3362,25 +3362,25 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12" t="s">
+        <v>353</v>
+      </c>
+      <c r="E12" t="s">
         <v>354</v>
       </c>
-      <c r="B12" t="s">
-        <v>355</v>
-      </c>
-      <c r="C12" t="s">
-        <v>362</v>
-      </c>
-      <c r="D12" t="s">
-        <v>356</v>
-      </c>
-      <c r="E12" t="s">
-        <v>357</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H12">
         <f t="shared" ref="H12:H21" si="5">INT(J12/3)</f>
@@ -3397,25 +3397,25 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C13" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D13" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E13" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H13">
         <f t="shared" si="5"/>
@@ -3432,25 +3432,25 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
         <v>132</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>133</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>134</v>
       </c>
-      <c r="D14" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" t="s">
-        <v>136</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14">
         <f t="shared" si="5"/>
@@ -3467,25 +3467,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>92</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>93</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>94</v>
       </c>
-      <c r="E15" t="s">
-        <v>95</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H15">
         <f t="shared" si="5"/>
@@ -3502,25 +3502,25 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="H16">
         <f t="shared" si="5"/>
@@ -3546,16 +3546,16 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17">
         <f t="shared" si="5"/>
@@ -3572,25 +3572,25 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" t="s">
         <v>119</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>120</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>121</v>
       </c>
-      <c r="E18" t="s">
-        <v>122</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H18">
         <f t="shared" si="5"/>
@@ -3622,7 +3622,7 @@
         <v>13</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>8</v>
@@ -3642,25 +3642,25 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
         <v>158</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>159</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>160</v>
       </c>
-      <c r="D20" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" t="s">
-        <v>162</v>
-      </c>
       <c r="F20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H20">
         <f t="shared" si="5"/>
@@ -3677,25 +3677,25 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
         <v>103</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>104</v>
       </c>
-      <c r="E21" t="s">
-        <v>105</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H21">
         <f t="shared" si="5"/>
@@ -3712,25 +3712,25 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" t="s">
         <v>137</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>138</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>139</v>
       </c>
-      <c r="D22" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" t="s">
-        <v>141</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H22">
         <f t="shared" ref="H22" si="7">INT(J22/3)</f>
@@ -3756,13 +3756,13 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
         <v>42</v>
       </c>
-      <c r="E23" t="s">
-        <v>43</v>
-      </c>
       <c r="F23" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>8</v>
@@ -3797,10 +3797,10 @@
         <v>36</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H24">
         <f t="shared" si="9"/>
@@ -3817,25 +3817,25 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>370</v>
+      </c>
+      <c r="B25" t="s">
+        <v>371</v>
+      </c>
+      <c r="C25" t="s">
+        <v>372</v>
+      </c>
+      <c r="D25" t="s">
         <v>373</v>
       </c>
-      <c r="B25" t="s">
+      <c r="E25" t="s">
         <v>374</v>
       </c>
-      <c r="C25" t="s">
-        <v>375</v>
-      </c>
-      <c r="D25" t="s">
-        <v>376</v>
-      </c>
-      <c r="E25" t="s">
-        <v>377</v>
-      </c>
       <c r="F25" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H25">
         <f t="shared" si="9"/>
@@ -3852,25 +3852,25 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
         <v>127</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>128</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>129</v>
       </c>
-      <c r="D26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" t="s">
-        <v>131</v>
-      </c>
       <c r="F26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H26">
         <f t="shared" si="9"/>
@@ -3887,22 +3887,22 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>253</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C27" t="s">
+        <v>255</v>
+      </c>
+      <c r="D27" t="s">
         <v>256</v>
       </c>
-      <c r="B27" t="s">
+      <c r="E27" t="s">
         <v>257</v>
       </c>
-      <c r="C27" t="s">
-        <v>258</v>
-      </c>
-      <c r="D27" t="s">
-        <v>259</v>
-      </c>
-      <c r="E27" t="s">
-        <v>260</v>
-      </c>
       <c r="F27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>8</v>
@@ -3922,25 +3922,25 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>413</v>
+      </c>
+      <c r="B28" t="s">
+        <v>414</v>
+      </c>
+      <c r="C28" t="s">
+        <v>415</v>
+      </c>
+      <c r="D28" t="s">
         <v>416</v>
       </c>
-      <c r="B28" t="s">
-        <v>417</v>
-      </c>
-      <c r="C28" t="s">
-        <v>418</v>
-      </c>
-      <c r="D28" t="s">
-        <v>419</v>
-      </c>
       <c r="E28" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="F28" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="H28">
         <f t="shared" ref="H28:H91" si="11">INT(J28/3)</f>
@@ -3957,25 +3957,25 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" t="s">
         <v>96</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>97</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>98</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>99</v>
       </c>
-      <c r="E29" t="s">
-        <v>100</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H29">
         <f t="shared" si="11"/>
@@ -3992,25 +3992,25 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
         <v>106</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>107</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>108</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>109</v>
       </c>
-      <c r="E30" t="s">
-        <v>110</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H30">
         <f t="shared" si="11"/>
@@ -4027,22 +4027,22 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>267</v>
+      </c>
+      <c r="B31" t="s">
+        <v>268</v>
+      </c>
+      <c r="C31" t="s">
+        <v>269</v>
+      </c>
+      <c r="D31" t="s">
         <v>270</v>
       </c>
-      <c r="B31" t="s">
+      <c r="E31" t="s">
         <v>271</v>
       </c>
-      <c r="C31" t="s">
-        <v>272</v>
-      </c>
-      <c r="D31" t="s">
-        <v>273</v>
-      </c>
-      <c r="E31" t="s">
-        <v>274</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>8</v>
@@ -4062,22 +4062,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>522</v>
+      </c>
+      <c r="B32" t="s">
+        <v>523</v>
+      </c>
+      <c r="C32" t="s">
+        <v>524</v>
+      </c>
+      <c r="D32" t="s">
         <v>525</v>
       </c>
-      <c r="B32" t="s">
+      <c r="E32" t="s">
         <v>526</v>
       </c>
-      <c r="C32" t="s">
-        <v>527</v>
-      </c>
-      <c r="D32" t="s">
-        <v>528</v>
-      </c>
-      <c r="E32" t="s">
-        <v>529</v>
-      </c>
       <c r="F32" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H32">
         <f t="shared" si="11"/>
@@ -4094,22 +4094,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B33" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C33" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D33" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E33" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F33" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H33">
         <f t="shared" si="11"/>
@@ -4126,22 +4126,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B34" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C34" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F34" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H34">
         <f t="shared" si="11"/>
@@ -4158,25 +4158,25 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
         <v>63</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>64</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>65</v>
       </c>
-      <c r="D35" t="s">
-        <v>66</v>
-      </c>
       <c r="E35" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H35">
         <f t="shared" si="11"/>
@@ -4205,10 +4205,10 @@
         <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>8</v>
@@ -4228,25 +4228,25 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
         <v>111</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>112</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>113</v>
       </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
       <c r="E37" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H37">
         <f t="shared" si="11"/>
@@ -4263,22 +4263,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>655</v>
+      </c>
+      <c r="B38" t="s">
+        <v>519</v>
+      </c>
+      <c r="C38" t="s">
         <v>658</v>
       </c>
-      <c r="B38" t="s">
-        <v>522</v>
-      </c>
-      <c r="C38" t="s">
-        <v>661</v>
-      </c>
       <c r="D38" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E38" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F38" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H38">
         <f t="shared" si="11"/>
@@ -4295,22 +4295,22 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B39" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E39" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="F39" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H39">
         <f t="shared" si="11"/>
@@ -4327,25 +4327,25 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" t="s">
         <v>207</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>208</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>209</v>
       </c>
-      <c r="D40" t="s">
-        <v>210</v>
-      </c>
-      <c r="E40" t="s">
-        <v>211</v>
-      </c>
       <c r="F40" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H40">
         <f t="shared" si="11"/>
@@ -4362,25 +4362,25 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
         <v>81</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>83</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>84</v>
       </c>
-      <c r="E41" t="s">
-        <v>85</v>
-      </c>
       <c r="F41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H41">
         <f t="shared" si="11"/>
@@ -4397,22 +4397,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>592</v>
+      </c>
+      <c r="B42" t="s">
+        <v>593</v>
+      </c>
+      <c r="C42" t="s">
+        <v>656</v>
+      </c>
+      <c r="D42" t="s">
+        <v>594</v>
+      </c>
+      <c r="E42" t="s">
         <v>595</v>
       </c>
-      <c r="B42" t="s">
-        <v>596</v>
-      </c>
-      <c r="C42" t="s">
-        <v>659</v>
-      </c>
-      <c r="D42" t="s">
-        <v>597</v>
-      </c>
-      <c r="E42" t="s">
-        <v>598</v>
-      </c>
       <c r="F42" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H42">
         <f t="shared" si="11"/>
@@ -4429,22 +4429,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>604</v>
+      </c>
+      <c r="B43" t="s">
+        <v>605</v>
+      </c>
+      <c r="C43" t="s">
+        <v>606</v>
+      </c>
+      <c r="D43" t="s">
         <v>607</v>
       </c>
-      <c r="B43" t="s">
+      <c r="E43" t="s">
         <v>608</v>
       </c>
-      <c r="C43" t="s">
-        <v>609</v>
-      </c>
-      <c r="D43" t="s">
-        <v>610</v>
-      </c>
-      <c r="E43" t="s">
-        <v>611</v>
-      </c>
       <c r="F43" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H43">
         <f t="shared" si="11"/>
@@ -4461,25 +4461,25 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B44" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C44" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D44" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E44" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F44" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H44">
         <f t="shared" si="11"/>
@@ -4496,25 +4496,25 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45" t="s">
         <v>197</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>198</v>
       </c>
-      <c r="C45" t="s">
+      <c r="E45" t="s">
         <v>199</v>
       </c>
-      <c r="D45" t="s">
-        <v>200</v>
-      </c>
-      <c r="E45" t="s">
-        <v>201</v>
-      </c>
       <c r="F45" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H45">
         <f t="shared" si="11"/>
@@ -4531,22 +4531,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>538</v>
+      </c>
+      <c r="B46" t="s">
+        <v>539</v>
+      </c>
+      <c r="C46" t="s">
+        <v>540</v>
+      </c>
+      <c r="D46" t="s">
+        <v>659</v>
+      </c>
+      <c r="E46" t="s">
         <v>541</v>
       </c>
-      <c r="B46" t="s">
-        <v>542</v>
-      </c>
-      <c r="C46" t="s">
-        <v>543</v>
-      </c>
-      <c r="D46" t="s">
-        <v>662</v>
-      </c>
-      <c r="E46" t="s">
-        <v>544</v>
-      </c>
       <c r="F46" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H46">
         <f t="shared" si="11"/>
@@ -4563,22 +4563,22 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B47" t="s">
+        <v>542</v>
+      </c>
+      <c r="C47" t="s">
+        <v>543</v>
+      </c>
+      <c r="D47" t="s">
+        <v>544</v>
+      </c>
+      <c r="E47" t="s">
         <v>545</v>
       </c>
-      <c r="C47" t="s">
-        <v>546</v>
-      </c>
-      <c r="D47" t="s">
-        <v>547</v>
-      </c>
-      <c r="E47" t="s">
-        <v>548</v>
-      </c>
       <c r="F47" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H47">
         <f t="shared" si="11"/>
@@ -4595,22 +4595,22 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>546</v>
+      </c>
+      <c r="B48" t="s">
+        <v>547</v>
+      </c>
+      <c r="C48" t="s">
+        <v>548</v>
+      </c>
+      <c r="D48" t="s">
         <v>549</v>
       </c>
-      <c r="B48" t="s">
+      <c r="E48" t="s">
         <v>550</v>
       </c>
-      <c r="C48" t="s">
-        <v>551</v>
-      </c>
-      <c r="D48" t="s">
-        <v>552</v>
-      </c>
-      <c r="E48" t="s">
-        <v>553</v>
-      </c>
       <c r="F48" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H48">
         <f t="shared" si="11"/>
@@ -4627,25 +4627,25 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B49" t="s">
+        <v>191</v>
+      </c>
+      <c r="C49" t="s">
         <v>192</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>193</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>194</v>
       </c>
-      <c r="D49" t="s">
-        <v>195</v>
-      </c>
-      <c r="E49" t="s">
-        <v>196</v>
-      </c>
       <c r="F49" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H49">
         <f t="shared" si="11"/>
@@ -4662,25 +4662,25 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>417</v>
+      </c>
+      <c r="B50" t="s">
+        <v>418</v>
+      </c>
+      <c r="C50" t="s">
+        <v>419</v>
+      </c>
+      <c r="D50" t="s">
+        <v>377</v>
+      </c>
+      <c r="E50" t="s">
         <v>420</v>
       </c>
-      <c r="B50" t="s">
-        <v>421</v>
-      </c>
-      <c r="C50" t="s">
-        <v>422</v>
-      </c>
-      <c r="D50" t="s">
-        <v>380</v>
-      </c>
-      <c r="E50" t="s">
-        <v>423</v>
-      </c>
       <c r="F50" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H50">
         <f t="shared" si="11"/>
@@ -4700,22 +4700,22 @@
         <v>42.195</v>
       </c>
       <c r="B51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" t="s">
+        <v>660</v>
+      </c>
+      <c r="D51" t="s">
         <v>123</v>
       </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>124</v>
       </c>
-      <c r="D51" t="s">
-        <v>125</v>
-      </c>
-      <c r="E51" t="s">
-        <v>126</v>
-      </c>
       <c r="F51" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H51">
         <f t="shared" si="11"/>
@@ -4732,22 +4732,22 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>661</v>
+      </c>
+      <c r="B52" t="s">
         <v>37</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>38</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>39</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>40</v>
       </c>
-      <c r="E52" t="s">
-        <v>41</v>
-      </c>
       <c r="F52" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>8</v>
@@ -4767,25 +4767,25 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" t="s">
         <v>168</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>169</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>170</v>
       </c>
-      <c r="D53" t="s">
-        <v>171</v>
-      </c>
-      <c r="E53" t="s">
-        <v>172</v>
-      </c>
       <c r="F53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H53">
         <f t="shared" si="11"/>
@@ -4802,25 +4802,25 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>214</v>
+      </c>
+      <c r="B54" t="s">
+        <v>662</v>
+      </c>
+      <c r="C54" t="s">
+        <v>215</v>
+      </c>
+      <c r="D54" t="s">
         <v>216</v>
       </c>
-      <c r="B54" t="s">
+      <c r="E54" t="s">
         <v>217</v>
       </c>
-      <c r="C54" t="s">
-        <v>218</v>
-      </c>
-      <c r="D54" t="s">
-        <v>219</v>
-      </c>
-      <c r="E54" t="s">
-        <v>220</v>
-      </c>
       <c r="F54" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H54">
         <f t="shared" si="11"/>
@@ -4837,25 +4837,25 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>383</v>
+      </c>
+      <c r="B55" t="s">
+        <v>384</v>
+      </c>
+      <c r="C55" t="s">
+        <v>385</v>
+      </c>
+      <c r="D55" t="s">
         <v>386</v>
       </c>
-      <c r="B55" t="s">
-        <v>387</v>
-      </c>
-      <c r="C55" t="s">
-        <v>388</v>
-      </c>
-      <c r="D55" t="s">
-        <v>389</v>
-      </c>
       <c r="E55" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F55" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H55">
         <f t="shared" si="11"/>
@@ -4872,25 +4872,25 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>233</v>
+      </c>
+      <c r="B56" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" t="s">
+        <v>235</v>
+      </c>
+      <c r="D56" t="s">
         <v>236</v>
       </c>
-      <c r="B56" t="s">
+      <c r="E56" t="s">
         <v>237</v>
       </c>
-      <c r="C56" t="s">
-        <v>238</v>
-      </c>
-      <c r="D56" t="s">
-        <v>239</v>
-      </c>
-      <c r="E56" t="s">
-        <v>240</v>
-      </c>
       <c r="F56" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H56">
         <f t="shared" si="11"/>
@@ -4913,19 +4913,19 @@
         <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E57" t="s">
         <v>33</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H57">
         <f t="shared" si="11"/>
@@ -4942,22 +4942,22 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>474</v>
+      </c>
+      <c r="B58" t="s">
+        <v>475</v>
+      </c>
+      <c r="C58" t="s">
+        <v>476</v>
+      </c>
+      <c r="D58" t="s">
         <v>477</v>
       </c>
-      <c r="B58" t="s">
+      <c r="E58" t="s">
         <v>478</v>
       </c>
-      <c r="C58" t="s">
-        <v>479</v>
-      </c>
-      <c r="D58" t="s">
-        <v>480</v>
-      </c>
-      <c r="E58" t="s">
-        <v>481</v>
-      </c>
       <c r="F58" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H58">
         <f t="shared" si="11"/>
@@ -4974,22 +4974,22 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>479</v>
+      </c>
+      <c r="B59" t="s">
+        <v>480</v>
+      </c>
+      <c r="C59" t="s">
+        <v>481</v>
+      </c>
+      <c r="D59" t="s">
         <v>482</v>
       </c>
-      <c r="B59" t="s">
+      <c r="E59" t="s">
         <v>483</v>
       </c>
-      <c r="C59" t="s">
-        <v>484</v>
-      </c>
-      <c r="D59" t="s">
-        <v>485</v>
-      </c>
-      <c r="E59" t="s">
-        <v>486</v>
-      </c>
       <c r="F59" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H59">
         <f t="shared" si="11"/>
@@ -5006,22 +5006,22 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>484</v>
+      </c>
+      <c r="B60" t="s">
+        <v>485</v>
+      </c>
+      <c r="C60" t="s">
+        <v>486</v>
+      </c>
+      <c r="D60" t="s">
         <v>487</v>
       </c>
-      <c r="B60" t="s">
+      <c r="E60" t="s">
         <v>488</v>
       </c>
-      <c r="C60" t="s">
-        <v>489</v>
-      </c>
-      <c r="D60" t="s">
-        <v>490</v>
-      </c>
-      <c r="E60" t="s">
-        <v>491</v>
-      </c>
       <c r="F60" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H60">
         <f t="shared" si="11"/>
@@ -5038,25 +5038,25 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>375</v>
+      </c>
+      <c r="B61" t="s">
+        <v>376</v>
+      </c>
+      <c r="C61" t="s">
+        <v>377</v>
+      </c>
+      <c r="D61" t="s">
         <v>378</v>
       </c>
-      <c r="B61" t="s">
+      <c r="E61" t="s">
         <v>379</v>
       </c>
-      <c r="C61" t="s">
-        <v>380</v>
-      </c>
-      <c r="D61" t="s">
-        <v>381</v>
-      </c>
-      <c r="E61" t="s">
-        <v>382</v>
-      </c>
       <c r="F61" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H61">
         <f t="shared" si="11"/>
@@ -5073,25 +5073,25 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" t="s">
+        <v>211</v>
+      </c>
+      <c r="D62" t="s">
         <v>212</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E62" t="s">
         <v>213</v>
       </c>
-      <c r="D62" t="s">
-        <v>214</v>
-      </c>
-      <c r="E62" t="s">
-        <v>215</v>
-      </c>
       <c r="F62" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H62">
         <f t="shared" si="11"/>
@@ -5108,25 +5108,25 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>312</v>
+      </c>
+      <c r="B63" t="s">
+        <v>313</v>
+      </c>
+      <c r="C63" t="s">
+        <v>314</v>
+      </c>
+      <c r="D63" t="s">
         <v>315</v>
       </c>
-      <c r="B63" t="s">
-        <v>316</v>
-      </c>
-      <c r="C63" t="s">
-        <v>317</v>
-      </c>
-      <c r="D63" t="s">
-        <v>318</v>
-      </c>
       <c r="E63" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F63" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H63">
         <f t="shared" si="11"/>
@@ -5143,25 +5143,25 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>151</v>
+      </c>
+      <c r="B64" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" t="s">
         <v>153</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>154</v>
       </c>
-      <c r="C64" t="s">
+      <c r="E64" t="s">
         <v>155</v>
       </c>
-      <c r="D64" t="s">
-        <v>156</v>
-      </c>
-      <c r="E64" t="s">
-        <v>157</v>
-      </c>
       <c r="F64" t="s">
+        <v>186</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="H64">
         <f t="shared" si="11"/>
@@ -5178,25 +5178,25 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>387</v>
+      </c>
+      <c r="B65" t="s">
+        <v>388</v>
+      </c>
+      <c r="C65" t="s">
+        <v>389</v>
+      </c>
+      <c r="D65" t="s">
         <v>390</v>
       </c>
-      <c r="B65" t="s">
-        <v>391</v>
-      </c>
-      <c r="C65" t="s">
-        <v>392</v>
-      </c>
-      <c r="D65" t="s">
-        <v>393</v>
-      </c>
       <c r="E65" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F65" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H65">
         <f t="shared" si="11"/>
@@ -5213,25 +5213,25 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>408</v>
+      </c>
+      <c r="B66" t="s">
+        <v>409</v>
+      </c>
+      <c r="C66" t="s">
+        <v>410</v>
+      </c>
+      <c r="D66" t="s">
         <v>411</v>
       </c>
-      <c r="B66" t="s">
+      <c r="E66" t="s">
         <v>412</v>
       </c>
-      <c r="C66" t="s">
-        <v>413</v>
-      </c>
-      <c r="D66" t="s">
-        <v>414</v>
-      </c>
-      <c r="E66" t="s">
-        <v>415</v>
-      </c>
       <c r="F66" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="H66">
         <f t="shared" si="11"/>
@@ -5248,22 +5248,22 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>470</v>
+      </c>
+      <c r="B67" t="s">
+        <v>471</v>
+      </c>
+      <c r="C67" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" t="s">
+        <v>472</v>
+      </c>
+      <c r="E67" t="s">
         <v>473</v>
       </c>
-      <c r="B67" t="s">
-        <v>474</v>
-      </c>
-      <c r="C67" t="s">
-        <v>214</v>
-      </c>
-      <c r="D67" t="s">
-        <v>475</v>
-      </c>
-      <c r="E67" t="s">
-        <v>476</v>
-      </c>
       <c r="F67" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H67">
         <f t="shared" si="11"/>
@@ -5280,25 +5280,25 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>247</v>
+      </c>
+      <c r="B68" t="s">
+        <v>248</v>
+      </c>
+      <c r="C68" t="s">
+        <v>249</v>
+      </c>
+      <c r="D68" t="s">
         <v>250</v>
       </c>
-      <c r="B68" t="s">
+      <c r="E68" t="s">
         <v>251</v>
       </c>
-      <c r="C68" t="s">
+      <c r="F68" t="s">
         <v>252</v>
       </c>
-      <c r="D68" t="s">
-        <v>253</v>
-      </c>
-      <c r="E68" t="s">
-        <v>254</v>
-      </c>
-      <c r="F68" t="s">
-        <v>255</v>
-      </c>
       <c r="G68" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H68">
         <f t="shared" si="11"/>
@@ -5315,22 +5315,22 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B69" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C69" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D69" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E69" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="F69" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H69">
         <f t="shared" si="11"/>
@@ -5347,22 +5347,22 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>599</v>
+      </c>
+      <c r="B70" t="s">
+        <v>600</v>
+      </c>
+      <c r="C70" t="s">
+        <v>601</v>
+      </c>
+      <c r="D70" t="s">
         <v>602</v>
       </c>
-      <c r="B70" t="s">
+      <c r="E70" t="s">
         <v>603</v>
       </c>
-      <c r="C70" t="s">
-        <v>604</v>
-      </c>
-      <c r="D70" t="s">
-        <v>605</v>
-      </c>
-      <c r="E70" t="s">
-        <v>606</v>
-      </c>
       <c r="F70" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H70">
         <f t="shared" si="11"/>
@@ -5379,25 +5379,25 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>421</v>
+      </c>
+      <c r="B71" t="s">
+        <v>422</v>
+      </c>
+      <c r="C71" t="s">
+        <v>423</v>
+      </c>
+      <c r="D71" t="s">
         <v>424</v>
       </c>
-      <c r="B71" t="s">
-        <v>425</v>
-      </c>
-      <c r="C71" t="s">
-        <v>426</v>
-      </c>
-      <c r="D71" t="s">
-        <v>427</v>
-      </c>
       <c r="E71" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F71" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H71">
         <f t="shared" si="11"/>
@@ -5414,25 +5414,25 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>280</v>
+      </c>
+      <c r="B72" t="s">
+        <v>281</v>
+      </c>
+      <c r="C72" t="s">
+        <v>282</v>
+      </c>
+      <c r="D72" t="s">
         <v>283</v>
       </c>
-      <c r="B72" t="s">
-        <v>284</v>
-      </c>
-      <c r="C72" t="s">
-        <v>285</v>
-      </c>
-      <c r="D72" t="s">
-        <v>286</v>
-      </c>
       <c r="E72" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F72" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H72">
         <f t="shared" si="11"/>
@@ -5449,25 +5449,25 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>295</v>
+      </c>
+      <c r="B73" t="s">
+        <v>296</v>
+      </c>
+      <c r="C73" t="s">
+        <v>297</v>
+      </c>
+      <c r="D73" t="s">
         <v>298</v>
       </c>
-      <c r="B73" t="s">
+      <c r="E73" t="s">
         <v>299</v>
       </c>
-      <c r="C73" t="s">
-        <v>300</v>
-      </c>
-      <c r="D73" t="s">
-        <v>301</v>
-      </c>
-      <c r="E73" t="s">
-        <v>302</v>
-      </c>
       <c r="F73" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H73">
         <f t="shared" si="11"/>
@@ -5484,25 +5484,25 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" t="s">
+        <v>292</v>
+      </c>
+      <c r="C74" t="s">
+        <v>293</v>
+      </c>
+      <c r="D74" t="s">
         <v>294</v>
       </c>
-      <c r="B74" t="s">
-        <v>295</v>
-      </c>
-      <c r="C74" t="s">
-        <v>296</v>
-      </c>
-      <c r="D74" t="s">
-        <v>297</v>
-      </c>
       <c r="E74" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F74" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H74">
         <f t="shared" si="11"/>
@@ -5519,22 +5519,22 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B75" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C75" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D75" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E75" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="F75" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H75">
         <f t="shared" si="11"/>
@@ -5551,22 +5551,22 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B76" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="C76" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D76" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E76" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F76" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H76">
         <f t="shared" si="11"/>
@@ -5583,25 +5583,25 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>322</v>
+      </c>
+      <c r="B77" t="s">
+        <v>323</v>
+      </c>
+      <c r="C77" t="s">
+        <v>324</v>
+      </c>
+      <c r="D77" t="s">
         <v>325</v>
       </c>
-      <c r="B77" t="s">
+      <c r="E77" t="s">
         <v>326</v>
       </c>
-      <c r="C77" t="s">
-        <v>327</v>
-      </c>
-      <c r="D77" t="s">
-        <v>328</v>
-      </c>
-      <c r="E77" t="s">
-        <v>329</v>
-      </c>
       <c r="F77" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H77">
         <f t="shared" si="11"/>
@@ -5618,25 +5618,25 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B78" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C78" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D78" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E78" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F78" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H78">
         <f t="shared" si="11"/>
@@ -5653,22 +5653,22 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>460</v>
+      </c>
+      <c r="B79" t="s">
+        <v>461</v>
+      </c>
+      <c r="C79" t="s">
+        <v>462</v>
+      </c>
+      <c r="D79" t="s">
         <v>463</v>
       </c>
-      <c r="B79" t="s">
+      <c r="E79" t="s">
         <v>464</v>
       </c>
-      <c r="C79" t="s">
-        <v>465</v>
-      </c>
-      <c r="D79" t="s">
-        <v>466</v>
-      </c>
-      <c r="E79" t="s">
-        <v>467</v>
-      </c>
       <c r="F79" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H79">
         <f t="shared" si="11"/>
@@ -5685,22 +5685,22 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>465</v>
+      </c>
+      <c r="B80" t="s">
+        <v>466</v>
+      </c>
+      <c r="C80" t="s">
+        <v>467</v>
+      </c>
+      <c r="D80" t="s">
         <v>468</v>
       </c>
-      <c r="B80" t="s">
+      <c r="E80" t="s">
         <v>469</v>
       </c>
-      <c r="C80" t="s">
-        <v>470</v>
-      </c>
-      <c r="D80" t="s">
-        <v>471</v>
-      </c>
-      <c r="E80" t="s">
-        <v>472</v>
-      </c>
       <c r="F80" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H80">
         <f t="shared" si="11"/>
@@ -5717,25 +5717,25 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>391</v>
+      </c>
+      <c r="B81" t="s">
+        <v>392</v>
+      </c>
+      <c r="C81" t="s">
+        <v>393</v>
+      </c>
+      <c r="D81" t="s">
         <v>394</v>
       </c>
-      <c r="B81" t="s">
+      <c r="E81" t="s">
         <v>395</v>
       </c>
-      <c r="C81" t="s">
-        <v>396</v>
-      </c>
-      <c r="D81" t="s">
-        <v>397</v>
-      </c>
-      <c r="E81" t="s">
-        <v>398</v>
-      </c>
       <c r="F81" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="H81">
         <f t="shared" si="11"/>
@@ -5752,25 +5752,25 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>223</v>
+      </c>
+      <c r="B82" t="s">
+        <v>224</v>
+      </c>
+      <c r="C82" t="s">
+        <v>225</v>
+      </c>
+      <c r="D82" t="s">
         <v>226</v>
       </c>
-      <c r="B82" t="s">
+      <c r="E82" t="s">
         <v>227</v>
       </c>
-      <c r="C82" t="s">
-        <v>228</v>
-      </c>
-      <c r="D82" t="s">
-        <v>229</v>
-      </c>
-      <c r="E82" t="s">
-        <v>230</v>
-      </c>
       <c r="F82" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H82">
         <f t="shared" si="11"/>
@@ -5787,22 +5787,22 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>489</v>
+      </c>
+      <c r="B83" t="s">
+        <v>490</v>
+      </c>
+      <c r="C83" t="s">
+        <v>491</v>
+      </c>
+      <c r="D83" t="s">
         <v>492</v>
       </c>
-      <c r="B83" t="s">
+      <c r="E83" t="s">
         <v>493</v>
       </c>
-      <c r="C83" t="s">
-        <v>494</v>
-      </c>
-      <c r="D83" t="s">
-        <v>495</v>
-      </c>
-      <c r="E83" t="s">
-        <v>496</v>
-      </c>
       <c r="F83" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H83">
         <f t="shared" si="11"/>
@@ -5819,22 +5819,22 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>494</v>
+      </c>
+      <c r="B84" t="s">
+        <v>495</v>
+      </c>
+      <c r="C84" t="s">
+        <v>496</v>
+      </c>
+      <c r="D84" t="s">
         <v>497</v>
       </c>
-      <c r="B84" t="s">
+      <c r="E84" t="s">
         <v>498</v>
       </c>
-      <c r="C84" t="s">
-        <v>499</v>
-      </c>
-      <c r="D84" t="s">
-        <v>500</v>
-      </c>
-      <c r="E84" t="s">
-        <v>501</v>
-      </c>
       <c r="F84" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H84">
         <f t="shared" si="11"/>
@@ -5851,25 +5851,25 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>316</v>
+      </c>
+      <c r="B85" t="s">
+        <v>317</v>
+      </c>
+      <c r="C85" t="s">
+        <v>318</v>
+      </c>
+      <c r="D85" t="s">
         <v>319</v>
       </c>
-      <c r="B85" t="s">
+      <c r="E85" t="s">
         <v>320</v>
       </c>
-      <c r="C85" t="s">
+      <c r="F85" t="s">
         <v>321</v>
       </c>
-      <c r="D85" t="s">
-        <v>322</v>
-      </c>
-      <c r="E85" t="s">
-        <v>323</v>
-      </c>
-      <c r="F85" t="s">
-        <v>324</v>
-      </c>
       <c r="G85" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H85">
         <f t="shared" si="11"/>
@@ -5886,25 +5886,25 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>161</v>
+      </c>
+      <c r="B86" t="s">
+        <v>162</v>
+      </c>
+      <c r="C86" t="s">
         <v>163</v>
       </c>
-      <c r="B86" t="s">
+      <c r="D86" t="s">
         <v>164</v>
       </c>
-      <c r="C86" t="s">
+      <c r="E86" t="s">
         <v>165</v>
       </c>
-      <c r="D86" t="s">
-        <v>166</v>
-      </c>
-      <c r="E86" t="s">
-        <v>167</v>
-      </c>
       <c r="F86" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H86">
         <f t="shared" si="11"/>
@@ -5921,22 +5921,22 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>504</v>
+      </c>
+      <c r="B87" t="s">
+        <v>505</v>
+      </c>
+      <c r="C87" t="s">
+        <v>506</v>
+      </c>
+      <c r="D87" t="s">
         <v>507</v>
       </c>
-      <c r="B87" t="s">
+      <c r="E87" t="s">
         <v>508</v>
       </c>
-      <c r="C87" t="s">
-        <v>509</v>
-      </c>
-      <c r="D87" t="s">
-        <v>510</v>
-      </c>
-      <c r="E87" t="s">
-        <v>511</v>
-      </c>
       <c r="F87" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H87">
         <f t="shared" si="11"/>
@@ -5953,22 +5953,22 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>509</v>
+      </c>
+      <c r="B88" t="s">
+        <v>510</v>
+      </c>
+      <c r="C88" t="s">
+        <v>511</v>
+      </c>
+      <c r="D88" t="s">
         <v>512</v>
       </c>
-      <c r="B88" t="s">
+      <c r="E88" t="s">
         <v>513</v>
       </c>
-      <c r="C88" t="s">
-        <v>514</v>
-      </c>
-      <c r="D88" t="s">
-        <v>515</v>
-      </c>
-      <c r="E88" t="s">
-        <v>516</v>
-      </c>
       <c r="F88" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H88">
         <f t="shared" si="11"/>
@@ -5985,22 +5985,22 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>514</v>
+      </c>
+      <c r="B89" t="s">
+        <v>515</v>
+      </c>
+      <c r="C89" t="s">
+        <v>516</v>
+      </c>
+      <c r="D89" t="s">
         <v>517</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
         <v>518</v>
       </c>
-      <c r="C89" t="s">
-        <v>519</v>
-      </c>
-      <c r="D89" t="s">
-        <v>520</v>
-      </c>
-      <c r="E89" t="s">
-        <v>521</v>
-      </c>
       <c r="F89" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H89">
         <f t="shared" si="11"/>
@@ -6017,25 +6017,25 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" t="s">
         <v>173</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>174</v>
       </c>
-      <c r="C90" t="s">
+      <c r="E90" t="s">
         <v>175</v>
       </c>
-      <c r="D90" t="s">
-        <v>176</v>
-      </c>
-      <c r="E90" t="s">
-        <v>177</v>
-      </c>
       <c r="F90" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H90">
         <f t="shared" si="11"/>
@@ -6052,25 +6052,25 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>200</v>
+      </c>
+      <c r="B91" t="s">
+        <v>201</v>
+      </c>
+      <c r="C91" t="s">
         <v>202</v>
       </c>
-      <c r="B91" t="s">
+      <c r="D91" t="s">
         <v>203</v>
       </c>
-      <c r="C91" t="s">
+      <c r="E91" t="s">
         <v>204</v>
       </c>
-      <c r="D91" t="s">
-        <v>205</v>
-      </c>
-      <c r="E91" t="s">
-        <v>206</v>
-      </c>
       <c r="F91" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H91">
         <f t="shared" si="11"/>
@@ -6087,25 +6087,25 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>304</v>
+      </c>
+      <c r="B92" t="s">
+        <v>305</v>
+      </c>
+      <c r="C92" t="s">
+        <v>306</v>
+      </c>
+      <c r="D92" t="s">
         <v>307</v>
       </c>
-      <c r="B92" t="s">
-        <v>308</v>
-      </c>
-      <c r="C92" t="s">
-        <v>309</v>
-      </c>
-      <c r="D92" t="s">
-        <v>310</v>
-      </c>
       <c r="E92" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F92" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H92">
         <f t="shared" ref="H92:H135" si="13">INT(J92/3)</f>
@@ -6122,22 +6122,22 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B93" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C93" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D93" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E93" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F93" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H93">
         <f t="shared" si="13"/>
@@ -6154,22 +6154,22 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B94" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C94" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D94" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E94" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="F94" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H94">
         <f t="shared" si="13"/>
@@ -6186,22 +6186,22 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>588</v>
+      </c>
+      <c r="B95" t="s">
+        <v>589</v>
+      </c>
+      <c r="C95" t="s">
+        <v>590</v>
+      </c>
+      <c r="D95" t="s">
+        <v>153</v>
+      </c>
+      <c r="E95" t="s">
         <v>591</v>
       </c>
-      <c r="B95" t="s">
-        <v>592</v>
-      </c>
-      <c r="C95" t="s">
-        <v>593</v>
-      </c>
-      <c r="D95" t="s">
-        <v>155</v>
-      </c>
-      <c r="E95" t="s">
-        <v>594</v>
-      </c>
       <c r="F95" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H95">
         <f t="shared" si="13"/>
@@ -6218,25 +6218,25 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>397</v>
+      </c>
+      <c r="B96" t="s">
+        <v>398</v>
+      </c>
+      <c r="C96" t="s">
+        <v>399</v>
+      </c>
+      <c r="D96" t="s">
         <v>400</v>
       </c>
-      <c r="B96" t="s">
+      <c r="E96" t="s">
         <v>401</v>
       </c>
-      <c r="C96" t="s">
-        <v>402</v>
-      </c>
-      <c r="D96" t="s">
-        <v>403</v>
-      </c>
-      <c r="E96" t="s">
-        <v>404</v>
-      </c>
       <c r="F96" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H96">
         <f t="shared" si="13"/>
@@ -6268,10 +6268,10 @@
         <v>30</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H97">
         <f t="shared" si="13"/>
@@ -6288,25 +6288,25 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98" t="s">
         <v>67</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>68</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
+        <v>369</v>
+      </c>
+      <c r="E98" t="s">
         <v>69</v>
       </c>
-      <c r="D98" t="s">
-        <v>372</v>
-      </c>
-      <c r="E98" t="s">
-        <v>70</v>
-      </c>
       <c r="F98" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H98">
         <f t="shared" si="13"/>
@@ -6323,22 +6323,22 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B99" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C99" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D99" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E99" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F99" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H99">
         <f t="shared" si="13"/>
@@ -6355,22 +6355,22 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>553</v>
+      </c>
+      <c r="B100" t="s">
+        <v>554</v>
+      </c>
+      <c r="C100" t="s">
+        <v>555</v>
+      </c>
+      <c r="D100" t="s">
         <v>556</v>
       </c>
-      <c r="B100" t="s">
+      <c r="E100" t="s">
         <v>557</v>
       </c>
-      <c r="C100" t="s">
-        <v>558</v>
-      </c>
-      <c r="D100" t="s">
-        <v>559</v>
-      </c>
-      <c r="E100" t="s">
-        <v>560</v>
-      </c>
       <c r="F100" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H100">
         <f t="shared" si="13"/>
@@ -6387,22 +6387,22 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B101" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C101" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D101" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E101" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="F101" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H101">
         <f t="shared" si="13"/>
@@ -6419,22 +6419,22 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>561</v>
+      </c>
+      <c r="B102" t="s">
+        <v>562</v>
+      </c>
+      <c r="C102" t="s">
+        <v>563</v>
+      </c>
+      <c r="D102" t="s">
         <v>564</v>
       </c>
-      <c r="B102" t="s">
+      <c r="E102" t="s">
         <v>565</v>
       </c>
-      <c r="C102" t="s">
-        <v>566</v>
-      </c>
-      <c r="D102" t="s">
-        <v>567</v>
-      </c>
-      <c r="E102" t="s">
-        <v>568</v>
-      </c>
       <c r="F102" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H102">
         <f t="shared" si="13"/>
@@ -6451,22 +6451,22 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
+        <v>566</v>
+      </c>
+      <c r="B103" t="s">
+        <v>567</v>
+      </c>
+      <c r="C103" t="s">
+        <v>568</v>
+      </c>
+      <c r="D103" t="s">
         <v>569</v>
       </c>
-      <c r="B103" t="s">
+      <c r="E103" t="s">
         <v>570</v>
       </c>
-      <c r="C103" t="s">
-        <v>571</v>
-      </c>
-      <c r="D103" t="s">
-        <v>572</v>
-      </c>
-      <c r="E103" t="s">
-        <v>573</v>
-      </c>
       <c r="F103" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H103">
         <f t="shared" si="13"/>
@@ -6483,25 +6483,25 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>181</v>
+      </c>
+      <c r="B104" t="s">
+        <v>182</v>
+      </c>
+      <c r="C104" t="s">
         <v>183</v>
       </c>
-      <c r="B104" t="s">
+      <c r="D104" t="s">
         <v>184</v>
       </c>
-      <c r="C104" t="s">
+      <c r="E104" t="s">
         <v>185</v>
       </c>
-      <c r="D104" t="s">
+      <c r="F104" t="s">
         <v>186</v>
       </c>
-      <c r="E104" t="s">
+      <c r="G104" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="F104" t="s">
-        <v>188</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="H104">
         <f t="shared" si="13"/>
@@ -6518,25 +6518,25 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>50</v>
+      </c>
+      <c r="B105" t="s">
         <v>51</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>52</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>53</v>
       </c>
-      <c r="D105" t="s">
+      <c r="E105" t="s">
         <v>54</v>
       </c>
-      <c r="E105" t="s">
-        <v>55</v>
-      </c>
       <c r="F105" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G105" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="H105">
         <f t="shared" si="13"/>
@@ -6553,25 +6553,25 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>228</v>
+      </c>
+      <c r="B106" t="s">
+        <v>229</v>
+      </c>
+      <c r="C106" t="s">
+        <v>230</v>
+      </c>
+      <c r="D106" t="s">
         <v>231</v>
       </c>
-      <c r="B106" t="s">
+      <c r="E106" t="s">
         <v>232</v>
       </c>
-      <c r="C106" t="s">
-        <v>233</v>
-      </c>
-      <c r="D106" t="s">
-        <v>234</v>
-      </c>
-      <c r="E106" t="s">
-        <v>235</v>
-      </c>
       <c r="F106" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H106">
         <f t="shared" si="13"/>
@@ -6588,25 +6588,25 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>176</v>
+      </c>
+      <c r="B107" t="s">
+        <v>177</v>
+      </c>
+      <c r="C107" t="s">
         <v>178</v>
       </c>
-      <c r="B107" t="s">
+      <c r="D107" t="s">
         <v>179</v>
       </c>
-      <c r="C107" t="s">
+      <c r="E107" t="s">
         <v>180</v>
       </c>
-      <c r="D107" t="s">
-        <v>181</v>
-      </c>
-      <c r="E107" t="s">
-        <v>182</v>
-      </c>
       <c r="F107" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H107">
         <f t="shared" si="13"/>
@@ -6623,22 +6623,22 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>624</v>
+      </c>
+      <c r="B108" t="s">
+        <v>625</v>
+      </c>
+      <c r="C108" t="s">
+        <v>626</v>
+      </c>
+      <c r="D108" t="s">
         <v>627</v>
       </c>
-      <c r="B108" t="s">
+      <c r="E108" t="s">
         <v>628</v>
       </c>
-      <c r="C108" t="s">
-        <v>629</v>
-      </c>
-      <c r="D108" t="s">
-        <v>630</v>
-      </c>
-      <c r="E108" t="s">
-        <v>631</v>
-      </c>
       <c r="F108" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H108">
         <f t="shared" si="13"/>
@@ -6655,22 +6655,22 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>534</v>
+      </c>
+      <c r="B109" t="s">
+        <v>472</v>
+      </c>
+      <c r="C109" t="s">
+        <v>535</v>
+      </c>
+      <c r="D109" t="s">
+        <v>536</v>
+      </c>
+      <c r="E109" t="s">
         <v>537</v>
       </c>
-      <c r="B109" t="s">
-        <v>475</v>
-      </c>
-      <c r="C109" t="s">
-        <v>538</v>
-      </c>
-      <c r="D109" t="s">
-        <v>539</v>
-      </c>
-      <c r="E109" t="s">
-        <v>540</v>
-      </c>
       <c r="F109" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H109">
         <f t="shared" si="13"/>
@@ -6687,22 +6687,22 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
+        <v>629</v>
+      </c>
+      <c r="B110" t="s">
+        <v>630</v>
+      </c>
+      <c r="C110" t="s">
+        <v>631</v>
+      </c>
+      <c r="D110" t="s">
         <v>632</v>
       </c>
-      <c r="B110" t="s">
+      <c r="E110" t="s">
         <v>633</v>
       </c>
-      <c r="C110" t="s">
+      <c r="F110" t="s">
         <v>634</v>
-      </c>
-      <c r="D110" t="s">
-        <v>635</v>
-      </c>
-      <c r="E110" t="s">
-        <v>636</v>
-      </c>
-      <c r="F110" t="s">
-        <v>637</v>
       </c>
       <c r="H110">
         <f t="shared" si="13"/>
@@ -6719,25 +6719,25 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
+        <v>402</v>
+      </c>
+      <c r="B111" t="s">
+        <v>403</v>
+      </c>
+      <c r="C111" t="s">
+        <v>404</v>
+      </c>
+      <c r="D111" t="s">
         <v>405</v>
       </c>
-      <c r="B111" t="s">
-        <v>406</v>
-      </c>
-      <c r="C111" t="s">
-        <v>407</v>
-      </c>
-      <c r="D111" t="s">
-        <v>408</v>
-      </c>
       <c r="E111" s="7" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F111" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H111">
         <f t="shared" si="13"/>
@@ -6754,22 +6754,22 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B112" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C112" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D112" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E112" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="F112" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H112">
         <f t="shared" si="13"/>
@@ -6786,22 +6786,22 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>574</v>
+      </c>
+      <c r="B113" t="s">
+        <v>575</v>
+      </c>
+      <c r="C113" t="s">
+        <v>576</v>
+      </c>
+      <c r="D113" t="s">
         <v>577</v>
       </c>
-      <c r="B113" t="s">
+      <c r="E113" t="s">
         <v>578</v>
       </c>
-      <c r="C113" t="s">
-        <v>579</v>
-      </c>
-      <c r="D113" t="s">
-        <v>580</v>
-      </c>
-      <c r="E113" t="s">
-        <v>581</v>
-      </c>
       <c r="F113" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H113">
         <f t="shared" si="13"/>
@@ -6818,22 +6818,22 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>579</v>
+      </c>
+      <c r="B114" t="s">
+        <v>580</v>
+      </c>
+      <c r="C114" t="s">
+        <v>581</v>
+      </c>
+      <c r="D114" t="s">
         <v>582</v>
       </c>
-      <c r="B114" t="s">
-        <v>583</v>
-      </c>
-      <c r="C114" t="s">
-        <v>584</v>
-      </c>
-      <c r="D114" t="s">
-        <v>585</v>
-      </c>
       <c r="E114" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="F114" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H114">
         <f t="shared" si="13"/>
@@ -6850,22 +6850,22 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
+        <v>272</v>
+      </c>
+      <c r="B115" t="s">
+        <v>273</v>
+      </c>
+      <c r="C115" t="s">
+        <v>274</v>
+      </c>
+      <c r="D115" t="s">
         <v>275</v>
       </c>
-      <c r="B115" t="s">
+      <c r="E115" t="s">
         <v>276</v>
       </c>
-      <c r="C115" t="s">
-        <v>277</v>
-      </c>
-      <c r="D115" t="s">
-        <v>278</v>
-      </c>
-      <c r="E115" t="s">
-        <v>279</v>
-      </c>
       <c r="F115" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>8</v>
@@ -6885,22 +6885,22 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
+        <v>238</v>
+      </c>
+      <c r="B116" t="s">
+        <v>239</v>
+      </c>
+      <c r="C116" t="s">
+        <v>240</v>
+      </c>
+      <c r="D116" t="s">
         <v>241</v>
       </c>
-      <c r="B116" t="s">
+      <c r="E116" t="s">
         <v>242</v>
       </c>
-      <c r="C116" t="s">
-        <v>243</v>
-      </c>
-      <c r="D116" t="s">
-        <v>244</v>
-      </c>
-      <c r="E116" t="s">
-        <v>245</v>
-      </c>
       <c r="F116" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>8</v>
@@ -6920,25 +6920,25 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>308</v>
+      </c>
+      <c r="B117" t="s">
+        <v>309</v>
+      </c>
+      <c r="C117" t="s">
+        <v>310</v>
+      </c>
+      <c r="D117" t="s">
         <v>311</v>
       </c>
-      <c r="B117" t="s">
-        <v>312</v>
-      </c>
-      <c r="C117" t="s">
-        <v>313</v>
-      </c>
-      <c r="D117" t="s">
-        <v>314</v>
-      </c>
       <c r="E117" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F117" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H117">
         <f t="shared" si="13"/>
@@ -6955,22 +6955,22 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>609</v>
+      </c>
+      <c r="B118" t="s">
+        <v>610</v>
+      </c>
+      <c r="C118" t="s">
+        <v>611</v>
+      </c>
+      <c r="D118" t="s">
         <v>612</v>
       </c>
-      <c r="B118" t="s">
+      <c r="E118" t="s">
         <v>613</v>
       </c>
-      <c r="C118" t="s">
-        <v>614</v>
-      </c>
-      <c r="D118" t="s">
-        <v>615</v>
-      </c>
-      <c r="E118" t="s">
-        <v>616</v>
-      </c>
       <c r="F118" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H118">
         <f t="shared" si="13"/>
@@ -6987,22 +6987,22 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>614</v>
+      </c>
+      <c r="B119" t="s">
+        <v>615</v>
+      </c>
+      <c r="C119" t="s">
+        <v>616</v>
+      </c>
+      <c r="D119" t="s">
         <v>617</v>
       </c>
-      <c r="B119" t="s">
+      <c r="E119" t="s">
         <v>618</v>
       </c>
-      <c r="C119" t="s">
-        <v>619</v>
-      </c>
-      <c r="D119" t="s">
-        <v>620</v>
-      </c>
-      <c r="E119" t="s">
-        <v>621</v>
-      </c>
       <c r="F119" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H119">
         <f t="shared" si="13"/>
@@ -7019,25 +7019,25 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B120" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C120" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D120" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E120" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F120" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H120">
         <f t="shared" si="13"/>
@@ -7054,25 +7054,25 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="B121" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C121" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D121" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="E121" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F121" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H121">
         <f t="shared" si="13"/>
@@ -7089,25 +7089,25 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>263</v>
+      </c>
+      <c r="B122" t="s">
+        <v>264</v>
+      </c>
+      <c r="C122" t="s">
+        <v>265</v>
+      </c>
+      <c r="D122" t="s">
+        <v>245</v>
+      </c>
+      <c r="E122" t="s">
         <v>266</v>
       </c>
-      <c r="B122" t="s">
-        <v>267</v>
-      </c>
-      <c r="C122" t="s">
-        <v>268</v>
-      </c>
-      <c r="D122" t="s">
-        <v>248</v>
-      </c>
-      <c r="E122" t="s">
-        <v>269</v>
-      </c>
       <c r="F122" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H122">
         <f t="shared" si="13"/>
@@ -7124,25 +7124,25 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B123" t="s">
+        <v>243</v>
+      </c>
+      <c r="C123" t="s">
+        <v>244</v>
+      </c>
+      <c r="D123" t="s">
+        <v>245</v>
+      </c>
+      <c r="E123" t="s">
         <v>246</v>
       </c>
-      <c r="C123" t="s">
-        <v>247</v>
-      </c>
-      <c r="D123" t="s">
-        <v>248</v>
-      </c>
-      <c r="E123" t="s">
-        <v>249</v>
-      </c>
       <c r="F123" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H123">
         <f t="shared" si="13"/>
@@ -7159,22 +7159,22 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
+        <v>619</v>
+      </c>
+      <c r="B124" t="s">
+        <v>620</v>
+      </c>
+      <c r="C124" t="s">
+        <v>621</v>
+      </c>
+      <c r="D124" t="s">
         <v>622</v>
       </c>
-      <c r="B124" t="s">
+      <c r="E124" t="s">
         <v>623</v>
       </c>
-      <c r="C124" t="s">
-        <v>624</v>
-      </c>
-      <c r="D124" t="s">
-        <v>625</v>
-      </c>
-      <c r="E124" t="s">
-        <v>626</v>
-      </c>
       <c r="F124" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H124">
         <f t="shared" si="13"/>
@@ -7191,25 +7191,25 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B125" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C125" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D125" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E125" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F125" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H125">
         <f t="shared" si="13"/>
@@ -7226,25 +7226,25 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
+        <v>300</v>
+      </c>
+      <c r="B126" t="s">
+        <v>301</v>
+      </c>
+      <c r="C126" t="s">
+        <v>302</v>
+      </c>
+      <c r="D126" t="s">
         <v>303</v>
       </c>
-      <c r="B126" t="s">
-        <v>304</v>
-      </c>
-      <c r="C126" t="s">
-        <v>305</v>
-      </c>
-      <c r="D126" t="s">
-        <v>306</v>
-      </c>
       <c r="E126" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F126" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H126">
         <f t="shared" si="13"/>
@@ -7261,22 +7261,22 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>218</v>
+      </c>
+      <c r="B127" t="s">
+        <v>219</v>
+      </c>
+      <c r="C127" t="s">
+        <v>220</v>
+      </c>
+      <c r="D127" t="s">
         <v>221</v>
       </c>
-      <c r="B127" t="s">
+      <c r="E127" t="s">
         <v>222</v>
       </c>
-      <c r="C127" t="s">
-        <v>223</v>
-      </c>
-      <c r="D127" t="s">
-        <v>224</v>
-      </c>
-      <c r="E127" t="s">
-        <v>225</v>
-      </c>
       <c r="F127" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>8</v>
@@ -7296,25 +7296,25 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>146</v>
+      </c>
+      <c r="B128" t="s">
+        <v>147</v>
+      </c>
+      <c r="C128" t="s">
         <v>148</v>
       </c>
-      <c r="B128" t="s">
+      <c r="D128" t="s">
         <v>149</v>
       </c>
-      <c r="C128" t="s">
+      <c r="E128" t="s">
         <v>150</v>
       </c>
-      <c r="D128" t="s">
-        <v>151</v>
-      </c>
-      <c r="E128" t="s">
-        <v>152</v>
-      </c>
       <c r="F128" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H128">
         <f t="shared" si="13"/>
@@ -7331,25 +7331,25 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129" t="s">
         <v>71</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>72</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
         <v>73</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E129" t="s">
         <v>74</v>
       </c>
-      <c r="E129" t="s">
-        <v>75</v>
-      </c>
       <c r="F129" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H129">
         <f t="shared" si="13"/>
@@ -7366,25 +7366,25 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
+        <v>438</v>
+      </c>
+      <c r="B130" t="s">
+        <v>439</v>
+      </c>
+      <c r="C130" t="s">
+        <v>440</v>
+      </c>
+      <c r="D130" t="s">
         <v>441</v>
       </c>
-      <c r="B130" t="s">
+      <c r="E130" t="s">
         <v>442</v>
       </c>
-      <c r="C130" t="s">
+      <c r="F130" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="D130" t="s">
-        <v>444</v>
-      </c>
-      <c r="E130" t="s">
-        <v>445</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="G130" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H130">
         <f t="shared" si="13"/>
@@ -7401,25 +7401,25 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B131" t="s">
+        <v>444</v>
+      </c>
+      <c r="C131" t="s">
+        <v>445</v>
+      </c>
+      <c r="D131" t="s">
+        <v>446</v>
+      </c>
+      <c r="E131" t="s">
         <v>447</v>
       </c>
-      <c r="C131" t="s">
+      <c r="F131" t="s">
         <v>448</v>
       </c>
-      <c r="D131" t="s">
-        <v>449</v>
-      </c>
-      <c r="E131" t="s">
-        <v>450</v>
-      </c>
-      <c r="F131" t="s">
-        <v>451</v>
-      </c>
       <c r="G131" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H131">
         <f t="shared" si="13"/>
@@ -7436,25 +7436,25 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
+        <v>449</v>
+      </c>
+      <c r="B132" t="s">
+        <v>450</v>
+      </c>
+      <c r="C132" t="s">
+        <v>451</v>
+      </c>
+      <c r="D132" t="s">
         <v>452</v>
       </c>
-      <c r="B132" t="s">
+      <c r="E132" t="s">
         <v>453</v>
       </c>
-      <c r="C132" t="s">
-        <v>454</v>
-      </c>
-      <c r="D132" t="s">
-        <v>455</v>
-      </c>
-      <c r="E132" t="s">
-        <v>456</v>
-      </c>
       <c r="F132" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H132">
         <f t="shared" si="13"/>
@@ -7471,25 +7471,25 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
+        <v>454</v>
+      </c>
+      <c r="B133" t="s">
+        <v>455</v>
+      </c>
+      <c r="C133" t="s">
+        <v>456</v>
+      </c>
+      <c r="D133" t="s">
         <v>457</v>
       </c>
-      <c r="B133" t="s">
+      <c r="E133" t="s">
         <v>458</v>
       </c>
-      <c r="C133" t="s">
+      <c r="F133" t="s">
+        <v>443</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="D133" t="s">
-        <v>460</v>
-      </c>
-      <c r="E133" t="s">
-        <v>461</v>
-      </c>
-      <c r="F133" t="s">
-        <v>446</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>462</v>
       </c>
       <c r="H133">
         <f t="shared" si="13"/>
@@ -7506,22 +7506,22 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B134" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C134" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D134" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E134" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="F134" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H134">
         <f t="shared" si="13"/>
@@ -7538,22 +7538,22 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B135" t="s">
+        <v>640</v>
+      </c>
+      <c r="C135" t="s">
+        <v>641</v>
+      </c>
+      <c r="D135" t="s">
+        <v>642</v>
+      </c>
+      <c r="E135" t="s">
         <v>643</v>
       </c>
-      <c r="C135" t="s">
-        <v>644</v>
-      </c>
-      <c r="D135" t="s">
-        <v>645</v>
-      </c>
-      <c r="E135" t="s">
-        <v>646</v>
-      </c>
       <c r="F135" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="H135">
         <f t="shared" si="13"/>

</xml_diff>

<commit_message>
Add timer and words
</commit_message>
<xml_diff>
--- a/code/shabdakala/resource/sbwords.xlsx
+++ b/code/shabdakala/resource/sbwords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/github/shabdakala/shabdakala/code/shabdakala/resource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/shabdak_github/sbbd/shabdakala/code/shabdakala/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB0CC4-3365-794C-A317-3B6DEA471A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61C43C-072A-4245-A288-61F46AAE511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9F74AEE5-EB85-4044-AC84-8761A591B5C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1046">
   <si>
     <t>word0</t>
   </si>
@@ -1409,9 +1409,6 @@
     <t>माड</t>
   </si>
   <si>
-    <t>क्षितिज</t>
-  </si>
-  <si>
     <t>शिंपला</t>
   </si>
   <si>
@@ -1424,15 +1421,6 @@
     <t>मात</t>
   </si>
   <si>
-    <t>चाल</t>
-  </si>
-  <si>
-    <t>मारणे</t>
-  </si>
-  <si>
-    <t>बुद्धिबळाच्या चाली</t>
-  </si>
-  <si>
     <t>राणी</t>
   </si>
   <si>
@@ -3168,6 +3156,21 @@
   </si>
   <si>
     <t>सोमेश्वर</t>
+  </si>
+  <si>
+    <t>कॅसलिंग</t>
+  </si>
+  <si>
+    <t>लाटा</t>
+  </si>
+  <si>
+    <t>एन पासंट</t>
+  </si>
+  <si>
+    <t>चौसष्ट</t>
+  </si>
+  <si>
+    <t>अडीच</t>
   </si>
 </sst>
 </file>
@@ -4094,8 +4097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1707B-2FB7-B84C-9F84-E9F074F3056C}">
   <dimension ref="A1:L222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4183,7 +4186,7 @@
       </c>
       <c r="L2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45650</v>
+        <v>45651</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -4978,7 +4981,7 @@
         <v>370</v>
       </c>
       <c r="F25" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>185</v>
@@ -5083,7 +5086,7 @@
         <v>426</v>
       </c>
       <c r="F28" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>432</v>
@@ -5208,22 +5211,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>506</v>
+      </c>
+      <c r="B32" t="s">
+        <v>507</v>
+      </c>
+      <c r="C32" t="s">
+        <v>508</v>
+      </c>
+      <c r="D32" t="s">
+        <v>509</v>
+      </c>
+      <c r="E32" t="s">
         <v>510</v>
       </c>
-      <c r="B32" t="s">
-        <v>511</v>
-      </c>
-      <c r="C32" t="s">
-        <v>512</v>
-      </c>
-      <c r="D32" t="s">
-        <v>513</v>
-      </c>
-      <c r="E32" t="s">
-        <v>514</v>
-      </c>
       <c r="F32" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H32">
         <f t="shared" si="7"/>
@@ -5240,22 +5243,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B33" t="s">
         <v>371</v>
       </c>
       <c r="C33" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
       </c>
       <c r="E33" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F33" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H33">
         <f t="shared" si="7"/>
@@ -5272,22 +5275,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B34" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="C34" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
       </c>
       <c r="E34" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F34" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H34">
         <f t="shared" si="7"/>
@@ -5351,7 +5354,7 @@
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>339</v>
@@ -5386,7 +5389,7 @@
         <v>111</v>
       </c>
       <c r="E37" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>85</v>
@@ -5409,22 +5412,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B38" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C38" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D38" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E38" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F38" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H38">
         <f t="shared" si="7"/>
@@ -5441,22 +5444,22 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B39" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="E39" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="F39" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H39">
         <f t="shared" si="7"/>
@@ -5543,22 +5546,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B42" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C42" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D42" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="E42" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="F42" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H42">
         <f t="shared" si="7"/>
@@ -5575,22 +5578,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>588</v>
+      </c>
+      <c r="B43" t="s">
+        <v>589</v>
+      </c>
+      <c r="C43" t="s">
+        <v>590</v>
+      </c>
+      <c r="D43" t="s">
+        <v>591</v>
+      </c>
+      <c r="E43" t="s">
         <v>592</v>
       </c>
-      <c r="B43" t="s">
-        <v>593</v>
-      </c>
-      <c r="C43" t="s">
-        <v>594</v>
-      </c>
-      <c r="D43" t="s">
-        <v>595</v>
-      </c>
-      <c r="E43" t="s">
-        <v>596</v>
-      </c>
       <c r="F43" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H43">
         <f t="shared" si="7"/>
@@ -5622,7 +5625,7 @@
         <v>378</v>
       </c>
       <c r="F44" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>275</v>
@@ -5677,22 +5680,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B46" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C46" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D46" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="E46" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="F46" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H46">
         <f t="shared" si="7"/>
@@ -5712,19 +5715,19 @@
         <v>228</v>
       </c>
       <c r="B47" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C47" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D47" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="E47" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F47" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H47">
         <f t="shared" si="7"/>
@@ -5741,22 +5744,22 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>530</v>
+      </c>
+      <c r="B48" t="s">
+        <v>531</v>
+      </c>
+      <c r="C48" t="s">
+        <v>532</v>
+      </c>
+      <c r="D48" t="s">
+        <v>533</v>
+      </c>
+      <c r="E48" t="s">
         <v>534</v>
       </c>
-      <c r="B48" t="s">
-        <v>535</v>
-      </c>
-      <c r="C48" t="s">
-        <v>536</v>
-      </c>
-      <c r="D48" t="s">
-        <v>537</v>
-      </c>
-      <c r="E48" t="s">
-        <v>538</v>
-      </c>
       <c r="F48" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H48">
         <f t="shared" si="7"/>
@@ -5823,7 +5826,7 @@
         <v>416</v>
       </c>
       <c r="F50" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>275</v>
@@ -5849,7 +5852,7 @@
         <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D51" t="s">
         <v>121</v>
@@ -5878,7 +5881,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="B52" t="s">
         <v>36</v>
@@ -5951,7 +5954,7 @@
         <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="C54" t="s">
         <v>213</v>
@@ -5998,7 +6001,7 @@
         <v>433</v>
       </c>
       <c r="F55" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>275</v>
@@ -6021,19 +6024,19 @@
         <v>233</v>
       </c>
       <c r="B56" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="C56" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="D56" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="E56" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="F56" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H56">
         <f t="shared" si="7"/>
@@ -6056,7 +6059,7 @@
         <v>232</v>
       </c>
       <c r="C57" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="D57" t="s">
         <v>234</v>
@@ -6085,19 +6088,19 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>645</v>
+      </c>
+      <c r="B58" t="s">
+        <v>646</v>
+      </c>
+      <c r="C58" t="s">
+        <v>647</v>
+      </c>
+      <c r="D58" t="s">
+        <v>648</v>
+      </c>
+      <c r="E58" t="s">
         <v>649</v>
-      </c>
-      <c r="B58" t="s">
-        <v>650</v>
-      </c>
-      <c r="C58" t="s">
-        <v>651</v>
-      </c>
-      <c r="D58" t="s">
-        <v>652</v>
-      </c>
-      <c r="E58" t="s">
-        <v>653</v>
       </c>
       <c r="F58" t="s">
         <v>444</v>
@@ -6117,22 +6120,22 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B59" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C59" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D59" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="E59" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F59" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H59">
         <f t="shared" si="7"/>
@@ -6149,22 +6152,22 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B60" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C60" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D60" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="E60" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="F60" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H60">
         <f t="shared" ref="H60:H123" si="9">INT(J60/3)</f>
@@ -6181,22 +6184,22 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="B61" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C61" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D61" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E61" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F61" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H61">
         <f t="shared" si="9"/>
@@ -6213,22 +6216,22 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
       <c r="B62" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
       <c r="C62" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="D62" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
       <c r="E62" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F62" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H62">
         <f t="shared" si="9"/>
@@ -6245,19 +6248,19 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B63" t="s">
+        <v>640</v>
+      </c>
+      <c r="C63" t="s">
+        <v>641</v>
+      </c>
+      <c r="D63" t="s">
+        <v>642</v>
+      </c>
+      <c r="E63" t="s">
         <v>644</v>
-      </c>
-      <c r="C63" t="s">
-        <v>645</v>
-      </c>
-      <c r="D63" t="s">
-        <v>646</v>
-      </c>
-      <c r="E63" t="s">
-        <v>648</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>444</v>
@@ -6293,7 +6296,7 @@
         <v>375</v>
       </c>
       <c r="F64" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>275</v>
@@ -6433,7 +6436,7 @@
         <v>421</v>
       </c>
       <c r="F68" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>275</v>
@@ -6468,7 +6471,7 @@
         <v>408</v>
       </c>
       <c r="F69" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>431</v>
@@ -6488,22 +6491,22 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B70" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C70" t="s">
         <v>210</v>
       </c>
       <c r="D70" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E70" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="F70" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H70">
         <f t="shared" si="9"/>
@@ -6558,19 +6561,19 @@
         <v>213</v>
       </c>
       <c r="B72" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C72" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D72" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="E72" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="F72" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H72">
         <f t="shared" si="9"/>
@@ -6587,22 +6590,22 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>583</v>
+      </c>
+      <c r="B73" t="s">
+        <v>584</v>
+      </c>
+      <c r="C73" t="s">
+        <v>585</v>
+      </c>
+      <c r="D73" t="s">
+        <v>586</v>
+      </c>
+      <c r="E73" t="s">
         <v>587</v>
       </c>
-      <c r="B73" t="s">
-        <v>588</v>
-      </c>
-      <c r="C73" t="s">
-        <v>589</v>
-      </c>
-      <c r="D73" t="s">
-        <v>590</v>
-      </c>
-      <c r="E73" t="s">
-        <v>591</v>
-      </c>
       <c r="F73" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H73">
         <f t="shared" si="9"/>
@@ -6619,22 +6622,22 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>839</v>
+      </c>
+      <c r="B74" t="s">
+        <v>840</v>
+      </c>
+      <c r="C74" t="s">
+        <v>841</v>
+      </c>
+      <c r="D74" t="s">
+        <v>842</v>
+      </c>
+      <c r="E74" t="s">
         <v>843</v>
       </c>
-      <c r="B74" t="s">
-        <v>844</v>
-      </c>
-      <c r="C74" t="s">
-        <v>845</v>
-      </c>
-      <c r="D74" t="s">
-        <v>846</v>
-      </c>
-      <c r="E74" t="s">
-        <v>847</v>
-      </c>
       <c r="F74" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H74">
         <f t="shared" si="9"/>
@@ -6666,7 +6669,7 @@
         <v>427</v>
       </c>
       <c r="F75" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>275</v>
@@ -6791,22 +6794,22 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B79" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C79" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D79" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E79" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="F79" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H79">
         <f t="shared" si="9"/>
@@ -6823,22 +6826,22 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B80" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C80" t="s">
         <v>302</v>
       </c>
       <c r="D80" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="E80" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F80" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H80">
         <f t="shared" si="9"/>
@@ -6893,13 +6896,13 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="C82" t="s">
         <v>282</v>
       </c>
       <c r="D82" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="E82" t="s">
         <v>316</v>
@@ -6931,16 +6934,16 @@
         <v>457</v>
       </c>
       <c r="C83" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D83" t="s">
         <v>458</v>
       </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>459</v>
       </c>
-      <c r="E83" t="s">
-        <v>460</v>
-      </c>
       <c r="F83" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H83">
         <f t="shared" si="9"/>
@@ -6957,22 +6960,22 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>461</v>
+        <v>1045</v>
       </c>
       <c r="B84" t="s">
-        <v>462</v>
+        <v>1044</v>
       </c>
       <c r="C84" t="s">
-        <v>463</v>
+        <v>1041</v>
       </c>
       <c r="D84" t="s">
-        <v>464</v>
+        <v>1043</v>
       </c>
       <c r="E84" t="s">
-        <v>465</v>
+        <v>1039</v>
       </c>
       <c r="F84" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H84">
         <f t="shared" si="9"/>
@@ -7004,7 +7007,7 @@
         <v>391</v>
       </c>
       <c r="F85" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>428</v>
@@ -7059,22 +7062,22 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>473</v>
+      </c>
+      <c r="B87" t="s">
+        <v>474</v>
+      </c>
+      <c r="C87" t="s">
+        <v>475</v>
+      </c>
+      <c r="D87" t="s">
+        <v>476</v>
+      </c>
+      <c r="E87" t="s">
         <v>477</v>
       </c>
-      <c r="B87" t="s">
-        <v>478</v>
-      </c>
-      <c r="C87" t="s">
-        <v>479</v>
-      </c>
-      <c r="D87" t="s">
-        <v>480</v>
-      </c>
-      <c r="E87" t="s">
-        <v>481</v>
-      </c>
       <c r="F87" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H87">
         <f t="shared" si="9"/>
@@ -7091,22 +7094,22 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>478</v>
+      </c>
+      <c r="B88" t="s">
+        <v>479</v>
+      </c>
+      <c r="C88" t="s">
+        <v>480</v>
+      </c>
+      <c r="D88" t="s">
+        <v>481</v>
+      </c>
+      <c r="E88" t="s">
         <v>482</v>
       </c>
-      <c r="B88" t="s">
-        <v>483</v>
-      </c>
-      <c r="C88" t="s">
-        <v>484</v>
-      </c>
-      <c r="D88" t="s">
-        <v>485</v>
-      </c>
-      <c r="E88" t="s">
-        <v>486</v>
-      </c>
       <c r="F88" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H88">
         <f t="shared" si="9"/>
@@ -7193,22 +7196,22 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>488</v>
+      </c>
+      <c r="B91" t="s">
+        <v>489</v>
+      </c>
+      <c r="C91" t="s">
+        <v>490</v>
+      </c>
+      <c r="D91" t="s">
+        <v>491</v>
+      </c>
+      <c r="E91" t="s">
         <v>492</v>
       </c>
-      <c r="B91" t="s">
-        <v>493</v>
-      </c>
-      <c r="C91" t="s">
-        <v>494</v>
-      </c>
-      <c r="D91" t="s">
-        <v>495</v>
-      </c>
-      <c r="E91" t="s">
-        <v>496</v>
-      </c>
       <c r="F91" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H91">
         <f t="shared" si="9"/>
@@ -7225,22 +7228,22 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>493</v>
+      </c>
+      <c r="B92" t="s">
+        <v>494</v>
+      </c>
+      <c r="C92" t="s">
+        <v>495</v>
+      </c>
+      <c r="D92" t="s">
+        <v>496</v>
+      </c>
+      <c r="E92" t="s">
         <v>497</v>
       </c>
-      <c r="B92" t="s">
-        <v>498</v>
-      </c>
-      <c r="C92" t="s">
-        <v>499</v>
-      </c>
-      <c r="D92" t="s">
-        <v>500</v>
-      </c>
-      <c r="E92" t="s">
-        <v>501</v>
-      </c>
       <c r="F92" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H92">
         <f t="shared" si="9"/>
@@ -7257,22 +7260,22 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>498</v>
+      </c>
+      <c r="B93" t="s">
+        <v>499</v>
+      </c>
+      <c r="C93" t="s">
+        <v>500</v>
+      </c>
+      <c r="D93" t="s">
+        <v>501</v>
+      </c>
+      <c r="E93" t="s">
         <v>502</v>
       </c>
-      <c r="B93" t="s">
-        <v>503</v>
-      </c>
-      <c r="C93" t="s">
-        <v>504</v>
-      </c>
-      <c r="D93" t="s">
-        <v>505</v>
-      </c>
-      <c r="E93" t="s">
-        <v>506</v>
-      </c>
       <c r="F93" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H93">
         <f t="shared" si="9"/>
@@ -7394,22 +7397,22 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B97" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C97" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D97" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E97" t="s">
         <v>162</v>
       </c>
       <c r="F97" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H97">
         <f t="shared" si="9"/>
@@ -7429,19 +7432,19 @@
         <v>162</v>
       </c>
       <c r="B98" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C98" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D98" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E98" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F98" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H98">
         <f t="shared" si="9"/>
@@ -7458,22 +7461,22 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B99" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C99" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D99" t="s">
         <v>151</v>
       </c>
       <c r="E99" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F99" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H99">
         <f t="shared" si="9"/>
@@ -7505,7 +7508,7 @@
         <v>397</v>
       </c>
       <c r="F100" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>275</v>
@@ -7598,7 +7601,7 @@
         <v>411</v>
       </c>
       <c r="B103" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="C103" t="s">
         <v>410</v>
@@ -7607,10 +7610,10 @@
         <v>412</v>
       </c>
       <c r="E103" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="F103" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H103">
         <f t="shared" si="9"/>
@@ -7627,22 +7630,22 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
+        <v>537</v>
+      </c>
+      <c r="B104" t="s">
+        <v>538</v>
+      </c>
+      <c r="C104" t="s">
+        <v>539</v>
+      </c>
+      <c r="D104" t="s">
+        <v>540</v>
+      </c>
+      <c r="E104" t="s">
         <v>541</v>
       </c>
-      <c r="B104" t="s">
-        <v>542</v>
-      </c>
-      <c r="C104" t="s">
-        <v>543</v>
-      </c>
-      <c r="D104" t="s">
-        <v>544</v>
-      </c>
-      <c r="E104" t="s">
-        <v>545</v>
-      </c>
       <c r="F104" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H104">
         <f t="shared" si="9"/>
@@ -7659,22 +7662,22 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B105" t="s">
         <v>392</v>
       </c>
       <c r="C105" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D105" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="E105" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="F105" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H105">
         <f t="shared" si="9"/>
@@ -7691,22 +7694,22 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
+        <v>545</v>
+      </c>
+      <c r="B106" t="s">
+        <v>546</v>
+      </c>
+      <c r="C106" t="s">
+        <v>547</v>
+      </c>
+      <c r="D106" t="s">
+        <v>548</v>
+      </c>
+      <c r="E106" t="s">
         <v>549</v>
       </c>
-      <c r="B106" t="s">
-        <v>550</v>
-      </c>
-      <c r="C106" t="s">
-        <v>551</v>
-      </c>
-      <c r="D106" t="s">
-        <v>552</v>
-      </c>
-      <c r="E106" t="s">
-        <v>553</v>
-      </c>
       <c r="F106" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H106">
         <f t="shared" si="9"/>
@@ -7723,22 +7726,22 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>550</v>
+      </c>
+      <c r="B107" t="s">
+        <v>551</v>
+      </c>
+      <c r="C107" t="s">
+        <v>552</v>
+      </c>
+      <c r="D107" t="s">
+        <v>553</v>
+      </c>
+      <c r="E107" t="s">
         <v>554</v>
       </c>
-      <c r="B107" t="s">
-        <v>555</v>
-      </c>
-      <c r="C107" t="s">
-        <v>556</v>
-      </c>
-      <c r="D107" t="s">
-        <v>557</v>
-      </c>
-      <c r="E107" t="s">
-        <v>558</v>
-      </c>
       <c r="F107" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H107">
         <f t="shared" si="9"/>
@@ -7895,22 +7898,22 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>603</v>
+      </c>
+      <c r="B112" t="s">
+        <v>604</v>
+      </c>
+      <c r="C112" t="s">
+        <v>605</v>
+      </c>
+      <c r="D112" t="s">
+        <v>606</v>
+      </c>
+      <c r="E112" t="s">
         <v>607</v>
       </c>
-      <c r="B112" t="s">
-        <v>608</v>
-      </c>
-      <c r="C112" t="s">
-        <v>609</v>
-      </c>
-      <c r="D112" t="s">
-        <v>610</v>
-      </c>
-      <c r="E112" t="s">
-        <v>611</v>
-      </c>
       <c r="F112" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H112">
         <f t="shared" si="9"/>
@@ -7927,22 +7930,22 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B113" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C113" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D113" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="E113" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="F113" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H113">
         <f t="shared" si="9"/>
@@ -7959,22 +7962,22 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>608</v>
+      </c>
+      <c r="B114" t="s">
+        <v>609</v>
+      </c>
+      <c r="C114" t="s">
+        <v>610</v>
+      </c>
+      <c r="D114" t="s">
+        <v>611</v>
+      </c>
+      <c r="E114" t="s">
         <v>612</v>
       </c>
-      <c r="B114" t="s">
+      <c r="F114" t="s">
         <v>613</v>
-      </c>
-      <c r="C114" t="s">
-        <v>614</v>
-      </c>
-      <c r="D114" t="s">
-        <v>615</v>
-      </c>
-      <c r="E114" t="s">
-        <v>616</v>
-      </c>
-      <c r="F114" t="s">
-        <v>617</v>
       </c>
       <c r="H114">
         <f t="shared" si="9"/>
@@ -8006,7 +8009,7 @@
         <v>424</v>
       </c>
       <c r="F115" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>87</v>
@@ -8026,22 +8029,22 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B116" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C116" t="s">
         <v>412</v>
       </c>
       <c r="D116" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="E116" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F116" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H116">
         <f t="shared" si="9"/>
@@ -8058,22 +8061,22 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
+        <v>558</v>
+      </c>
+      <c r="B117" t="s">
+        <v>559</v>
+      </c>
+      <c r="C117" t="s">
+        <v>560</v>
+      </c>
+      <c r="D117" t="s">
+        <v>561</v>
+      </c>
+      <c r="E117" t="s">
         <v>562</v>
       </c>
-      <c r="B117" t="s">
-        <v>563</v>
-      </c>
-      <c r="C117" t="s">
-        <v>564</v>
-      </c>
-      <c r="D117" t="s">
-        <v>565</v>
-      </c>
-      <c r="E117" t="s">
-        <v>566</v>
-      </c>
       <c r="F117" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H117">
         <f t="shared" si="9"/>
@@ -8090,22 +8093,22 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B118" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C118" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D118" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="E118" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="F118" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H118">
         <f t="shared" si="9"/>
@@ -8227,22 +8230,22 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>593</v>
+      </c>
+      <c r="B122" t="s">
+        <v>594</v>
+      </c>
+      <c r="C122" t="s">
+        <v>595</v>
+      </c>
+      <c r="D122" t="s">
+        <v>596</v>
+      </c>
+      <c r="E122" t="s">
         <v>597</v>
       </c>
-      <c r="B122" t="s">
-        <v>598</v>
-      </c>
-      <c r="C122" t="s">
-        <v>599</v>
-      </c>
-      <c r="D122" t="s">
-        <v>600</v>
-      </c>
-      <c r="E122" t="s">
-        <v>601</v>
-      </c>
       <c r="F122" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H122">
         <f t="shared" si="9"/>
@@ -8294,7 +8297,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B124" t="s">
         <v>425</v>
@@ -8309,7 +8312,7 @@
         <v>430</v>
       </c>
       <c r="F124" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>429</v>
@@ -8399,22 +8402,22 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>598</v>
+      </c>
+      <c r="B127" t="s">
+        <v>599</v>
+      </c>
+      <c r="C127" t="s">
+        <v>600</v>
+      </c>
+      <c r="D127" t="s">
+        <v>601</v>
+      </c>
+      <c r="E127" t="s">
         <v>602</v>
       </c>
-      <c r="B127" t="s">
-        <v>603</v>
-      </c>
-      <c r="C127" t="s">
-        <v>604</v>
-      </c>
-      <c r="D127" t="s">
-        <v>605</v>
-      </c>
-      <c r="E127" t="s">
-        <v>606</v>
-      </c>
       <c r="F127" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H127">
         <f t="shared" si="12"/>
@@ -8746,22 +8749,22 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B137" t="s">
         <v>232</v>
       </c>
       <c r="C137" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D137" t="s">
         <v>231</v>
       </c>
       <c r="E137" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="F137" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H137">
         <f t="shared" si="12"/>
@@ -8790,7 +8793,7 @@
         <v>43</v>
       </c>
       <c r="E138" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>339</v>
@@ -8813,22 +8816,22 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>675</v>
+      </c>
+      <c r="B139" t="s">
+        <v>676</v>
+      </c>
+      <c r="C139" t="s">
+        <v>677</v>
+      </c>
+      <c r="D139" t="s">
+        <v>678</v>
+      </c>
+      <c r="E139" t="s">
         <v>679</v>
       </c>
-      <c r="B139" t="s">
-        <v>680</v>
-      </c>
-      <c r="C139" t="s">
-        <v>681</v>
-      </c>
-      <c r="D139" t="s">
-        <v>682</v>
-      </c>
-      <c r="E139" t="s">
-        <v>683</v>
-      </c>
       <c r="F139" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139">
@@ -8846,22 +8849,22 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>660</v>
+      </c>
+      <c r="B140" t="s">
+        <v>661</v>
+      </c>
+      <c r="C140" t="s">
+        <v>662</v>
+      </c>
+      <c r="D140" t="s">
+        <v>663</v>
+      </c>
+      <c r="E140" t="s">
         <v>664</v>
       </c>
-      <c r="B140" t="s">
-        <v>665</v>
-      </c>
-      <c r="C140" t="s">
-        <v>666</v>
-      </c>
-      <c r="D140" t="s">
-        <v>667</v>
-      </c>
-      <c r="E140" t="s">
-        <v>668</v>
-      </c>
       <c r="F140" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H140">
         <f t="shared" si="12"/>
@@ -8878,22 +8881,22 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
+        <v>665</v>
+      </c>
+      <c r="B141" t="s">
+        <v>666</v>
+      </c>
+      <c r="C141" t="s">
+        <v>667</v>
+      </c>
+      <c r="D141" t="s">
+        <v>668</v>
+      </c>
+      <c r="E141" t="s">
         <v>669</v>
       </c>
-      <c r="B141" t="s">
-        <v>670</v>
-      </c>
-      <c r="C141" t="s">
-        <v>671</v>
-      </c>
-      <c r="D141" t="s">
-        <v>672</v>
-      </c>
-      <c r="E141" t="s">
-        <v>673</v>
-      </c>
       <c r="F141" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H141">
         <f t="shared" si="12"/>
@@ -8910,22 +8913,22 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
+        <v>670</v>
+      </c>
+      <c r="B142" t="s">
+        <v>671</v>
+      </c>
+      <c r="C142" t="s">
+        <v>672</v>
+      </c>
+      <c r="D142" t="s">
+        <v>673</v>
+      </c>
+      <c r="E142" t="s">
         <v>674</v>
       </c>
-      <c r="B142" t="s">
-        <v>675</v>
-      </c>
-      <c r="C142" t="s">
-        <v>676</v>
-      </c>
-      <c r="D142" t="s">
-        <v>677</v>
-      </c>
-      <c r="E142" t="s">
-        <v>678</v>
-      </c>
       <c r="F142" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H142">
         <f t="shared" si="12"/>
@@ -8942,22 +8945,22 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
+        <v>680</v>
+      </c>
+      <c r="B143" t="s">
+        <v>681</v>
+      </c>
+      <c r="C143" t="s">
+        <v>682</v>
+      </c>
+      <c r="D143" t="s">
+        <v>683</v>
+      </c>
+      <c r="E143" t="s">
         <v>684</v>
       </c>
-      <c r="B143" t="s">
-        <v>685</v>
-      </c>
-      <c r="C143" t="s">
-        <v>686</v>
-      </c>
-      <c r="D143" t="s">
-        <v>687</v>
-      </c>
-      <c r="E143" t="s">
-        <v>688</v>
-      </c>
       <c r="F143" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H143">
         <f t="shared" si="12"/>
@@ -8974,22 +8977,22 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="B144" t="s">
         <v>228</v>
       </c>
       <c r="C144" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="D144" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="E144" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="F144" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H144">
         <f t="shared" si="12"/>
@@ -9006,22 +9009,22 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
+        <v>689</v>
+      </c>
+      <c r="B145" t="s">
+        <v>690</v>
+      </c>
+      <c r="C145" t="s">
+        <v>691</v>
+      </c>
+      <c r="D145" t="s">
+        <v>692</v>
+      </c>
+      <c r="E145" t="s">
         <v>693</v>
       </c>
-      <c r="B145" t="s">
-        <v>694</v>
-      </c>
-      <c r="C145" t="s">
-        <v>695</v>
-      </c>
-      <c r="D145" t="s">
-        <v>696</v>
-      </c>
-      <c r="E145" t="s">
-        <v>697</v>
-      </c>
       <c r="F145" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H145">
         <f t="shared" si="12"/>
@@ -9038,22 +9041,22 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
+        <v>694</v>
+      </c>
+      <c r="B146" t="s">
+        <v>695</v>
+      </c>
+      <c r="C146" t="s">
+        <v>696</v>
+      </c>
+      <c r="D146" t="s">
+        <v>697</v>
+      </c>
+      <c r="E146" t="s">
         <v>698</v>
       </c>
-      <c r="B146" t="s">
-        <v>699</v>
-      </c>
-      <c r="C146" t="s">
-        <v>700</v>
-      </c>
-      <c r="D146" t="s">
-        <v>701</v>
-      </c>
-      <c r="E146" t="s">
-        <v>702</v>
-      </c>
       <c r="F146" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H146">
         <f t="shared" si="12"/>
@@ -9070,22 +9073,22 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B147" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="C147" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="D147" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="E147" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="F147" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H147">
         <f t="shared" si="12"/>
@@ -9102,22 +9105,22 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
+        <v>703</v>
+      </c>
+      <c r="B148" t="s">
+        <v>704</v>
+      </c>
+      <c r="C148" t="s">
+        <v>705</v>
+      </c>
+      <c r="D148" t="s">
+        <v>706</v>
+      </c>
+      <c r="E148" t="s">
         <v>707</v>
       </c>
-      <c r="B148" t="s">
-        <v>708</v>
-      </c>
-      <c r="C148" t="s">
-        <v>709</v>
-      </c>
-      <c r="D148" t="s">
-        <v>710</v>
-      </c>
-      <c r="E148" t="s">
-        <v>711</v>
-      </c>
       <c r="F148" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H148">
         <f t="shared" si="12"/>
@@ -9134,22 +9137,22 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
+        <v>708</v>
+      </c>
+      <c r="B149" t="s">
+        <v>709</v>
+      </c>
+      <c r="C149" t="s">
+        <v>710</v>
+      </c>
+      <c r="D149" t="s">
+        <v>711</v>
+      </c>
+      <c r="E149" t="s">
         <v>712</v>
       </c>
-      <c r="B149" t="s">
-        <v>713</v>
-      </c>
-      <c r="C149" t="s">
-        <v>714</v>
-      </c>
-      <c r="D149" t="s">
-        <v>715</v>
-      </c>
-      <c r="E149" t="s">
-        <v>716</v>
-      </c>
       <c r="F149" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H149">
         <f t="shared" si="12"/>
@@ -9166,22 +9169,22 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
+        <v>713</v>
+      </c>
+      <c r="B150" t="s">
+        <v>714</v>
+      </c>
+      <c r="C150" t="s">
+        <v>715</v>
+      </c>
+      <c r="D150" t="s">
+        <v>716</v>
+      </c>
+      <c r="E150" t="s">
         <v>717</v>
       </c>
-      <c r="B150" t="s">
-        <v>718</v>
-      </c>
-      <c r="C150" t="s">
-        <v>719</v>
-      </c>
-      <c r="D150" t="s">
-        <v>720</v>
-      </c>
-      <c r="E150" t="s">
-        <v>721</v>
-      </c>
       <c r="F150" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H150">
         <f t="shared" si="12"/>
@@ -9198,22 +9201,22 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>718</v>
+      </c>
+      <c r="B151" t="s">
+        <v>719</v>
+      </c>
+      <c r="C151" t="s">
+        <v>720</v>
+      </c>
+      <c r="D151" t="s">
+        <v>721</v>
+      </c>
+      <c r="E151" t="s">
         <v>722</v>
       </c>
-      <c r="B151" t="s">
-        <v>723</v>
-      </c>
-      <c r="C151" t="s">
-        <v>724</v>
-      </c>
-      <c r="D151" t="s">
-        <v>725</v>
-      </c>
-      <c r="E151" t="s">
-        <v>726</v>
-      </c>
       <c r="F151" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H151">
         <f t="shared" si="12"/>
@@ -9230,22 +9233,22 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
+        <v>723</v>
+      </c>
+      <c r="B152" t="s">
+        <v>724</v>
+      </c>
+      <c r="C152" t="s">
+        <v>725</v>
+      </c>
+      <c r="D152" t="s">
+        <v>726</v>
+      </c>
+      <c r="E152" t="s">
         <v>727</v>
       </c>
-      <c r="B152" t="s">
-        <v>728</v>
-      </c>
-      <c r="C152" t="s">
-        <v>729</v>
-      </c>
-      <c r="D152" t="s">
-        <v>730</v>
-      </c>
-      <c r="E152" t="s">
-        <v>731</v>
-      </c>
       <c r="F152" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H152">
         <f t="shared" si="12"/>
@@ -9262,22 +9265,22 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B153" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="C153" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="D153" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="E153" t="s">
         <v>246</v>
       </c>
       <c r="F153" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H153">
         <f t="shared" si="12"/>
@@ -9294,22 +9297,22 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B154" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C154" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D154" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="E154" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="F154" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H154">
         <f t="shared" si="12"/>
@@ -9326,22 +9329,22 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
+        <v>736</v>
+      </c>
+      <c r="B155" t="s">
+        <v>737</v>
+      </c>
+      <c r="C155" t="s">
+        <v>738</v>
+      </c>
+      <c r="D155" t="s">
+        <v>739</v>
+      </c>
+      <c r="E155" t="s">
         <v>740</v>
       </c>
-      <c r="B155" t="s">
-        <v>741</v>
-      </c>
-      <c r="C155" t="s">
-        <v>742</v>
-      </c>
-      <c r="D155" t="s">
-        <v>743</v>
-      </c>
-      <c r="E155" t="s">
-        <v>744</v>
-      </c>
       <c r="F155" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H155">
         <f t="shared" si="12"/>
@@ -9358,22 +9361,22 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
+        <v>741</v>
+      </c>
+      <c r="B156" t="s">
+        <v>742</v>
+      </c>
+      <c r="C156" t="s">
+        <v>743</v>
+      </c>
+      <c r="D156" t="s">
+        <v>744</v>
+      </c>
+      <c r="E156" t="s">
         <v>745</v>
       </c>
-      <c r="B156" t="s">
-        <v>746</v>
-      </c>
-      <c r="C156" t="s">
-        <v>747</v>
-      </c>
-      <c r="D156" t="s">
-        <v>748</v>
-      </c>
-      <c r="E156" t="s">
-        <v>749</v>
-      </c>
       <c r="F156" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H156">
         <f t="shared" si="12"/>
@@ -9390,22 +9393,22 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>746</v>
+      </c>
+      <c r="B157" t="s">
+        <v>747</v>
+      </c>
+      <c r="C157" t="s">
+        <v>748</v>
+      </c>
+      <c r="D157" t="s">
+        <v>749</v>
+      </c>
+      <c r="E157" t="s">
         <v>750</v>
       </c>
-      <c r="B157" t="s">
-        <v>751</v>
-      </c>
-      <c r="C157" t="s">
-        <v>752</v>
-      </c>
-      <c r="D157" t="s">
-        <v>753</v>
-      </c>
-      <c r="E157" t="s">
-        <v>754</v>
-      </c>
       <c r="F157" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H157">
         <f t="shared" si="12"/>
@@ -9422,22 +9425,22 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
+        <v>751</v>
+      </c>
+      <c r="B158" t="s">
+        <v>752</v>
+      </c>
+      <c r="C158" t="s">
+        <v>753</v>
+      </c>
+      <c r="D158" t="s">
+        <v>754</v>
+      </c>
+      <c r="E158" t="s">
         <v>755</v>
       </c>
-      <c r="B158" t="s">
-        <v>756</v>
-      </c>
-      <c r="C158" t="s">
-        <v>757</v>
-      </c>
-      <c r="D158" t="s">
-        <v>758</v>
-      </c>
-      <c r="E158" t="s">
-        <v>759</v>
-      </c>
       <c r="F158" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H158">
         <f t="shared" si="12"/>
@@ -9454,22 +9457,22 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B159" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C159" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D159" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E159" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="F159" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H159">
         <f t="shared" si="12"/>
@@ -9486,22 +9489,22 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
+        <v>760</v>
+      </c>
+      <c r="B160" t="s">
+        <v>761</v>
+      </c>
+      <c r="C160" t="s">
+        <v>762</v>
+      </c>
+      <c r="D160" t="s">
+        <v>763</v>
+      </c>
+      <c r="E160" t="s">
         <v>764</v>
       </c>
-      <c r="B160" t="s">
-        <v>765</v>
-      </c>
-      <c r="C160" t="s">
-        <v>766</v>
-      </c>
-      <c r="D160" t="s">
-        <v>767</v>
-      </c>
-      <c r="E160" t="s">
-        <v>768</v>
-      </c>
       <c r="F160" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H160">
         <f t="shared" si="12"/>
@@ -9518,22 +9521,22 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
+        <v>765</v>
+      </c>
+      <c r="B161" t="s">
+        <v>766</v>
+      </c>
+      <c r="C161" t="s">
+        <v>767</v>
+      </c>
+      <c r="D161" t="s">
+        <v>768</v>
+      </c>
+      <c r="E161" t="s">
         <v>769</v>
       </c>
-      <c r="B161" t="s">
-        <v>770</v>
-      </c>
-      <c r="C161" t="s">
-        <v>771</v>
-      </c>
-      <c r="D161" t="s">
-        <v>772</v>
-      </c>
-      <c r="E161" t="s">
-        <v>773</v>
-      </c>
       <c r="F161" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H161">
         <f t="shared" si="12"/>
@@ -9550,22 +9553,22 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
+        <v>770</v>
+      </c>
+      <c r="B162" t="s">
+        <v>771</v>
+      </c>
+      <c r="C162" t="s">
+        <v>772</v>
+      </c>
+      <c r="D162" t="s">
+        <v>773</v>
+      </c>
+      <c r="E162" t="s">
         <v>774</v>
       </c>
-      <c r="B162" t="s">
-        <v>775</v>
-      </c>
-      <c r="C162" t="s">
-        <v>776</v>
-      </c>
-      <c r="D162" t="s">
-        <v>777</v>
-      </c>
-      <c r="E162" t="s">
-        <v>778</v>
-      </c>
       <c r="F162" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H162">
         <f t="shared" si="12"/>
@@ -9582,22 +9585,22 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
       <c r="B163" t="s">
-        <v>780</v>
+        <v>776</v>
       </c>
       <c r="C163" t="s">
         <v>291</v>
       </c>
       <c r="D163" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
       <c r="E163" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="F163" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H163">
         <f t="shared" si="12"/>
@@ -9614,22 +9617,22 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
+        <v>760</v>
+      </c>
+      <c r="B164" t="s">
+        <v>761</v>
+      </c>
+      <c r="C164" t="s">
+        <v>762</v>
+      </c>
+      <c r="D164" t="s">
+        <v>763</v>
+      </c>
+      <c r="E164" t="s">
         <v>764</v>
       </c>
-      <c r="B164" t="s">
-        <v>765</v>
-      </c>
-      <c r="C164" t="s">
-        <v>766</v>
-      </c>
-      <c r="D164" t="s">
-        <v>767</v>
-      </c>
-      <c r="E164" t="s">
-        <v>768</v>
-      </c>
       <c r="F164" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H164">
         <f t="shared" si="12"/>
@@ -9646,22 +9649,22 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
+        <v>779</v>
+      </c>
+      <c r="B165" t="s">
+        <v>780</v>
+      </c>
+      <c r="C165" t="s">
+        <v>781</v>
+      </c>
+      <c r="D165" t="s">
+        <v>782</v>
+      </c>
+      <c r="E165" t="s">
         <v>783</v>
       </c>
-      <c r="B165" t="s">
-        <v>784</v>
-      </c>
-      <c r="C165" t="s">
-        <v>785</v>
-      </c>
-      <c r="D165" t="s">
-        <v>786</v>
-      </c>
-      <c r="E165" t="s">
-        <v>787</v>
-      </c>
       <c r="F165" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H165">
         <f t="shared" si="12"/>
@@ -9678,22 +9681,22 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B166" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="C166" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="D166" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="E166" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="F166" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H166">
         <f t="shared" si="12"/>
@@ -9710,22 +9713,22 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
+        <v>788</v>
+      </c>
+      <c r="B167" t="s">
+        <v>789</v>
+      </c>
+      <c r="C167" t="s">
+        <v>790</v>
+      </c>
+      <c r="D167" t="s">
+        <v>791</v>
+      </c>
+      <c r="E167" t="s">
         <v>792</v>
       </c>
-      <c r="B167" t="s">
-        <v>793</v>
-      </c>
-      <c r="C167" t="s">
-        <v>794</v>
-      </c>
-      <c r="D167" t="s">
-        <v>795</v>
-      </c>
-      <c r="E167" t="s">
-        <v>796</v>
-      </c>
       <c r="F167" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H167">
         <f t="shared" si="12"/>
@@ -9742,22 +9745,22 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
+        <v>793</v>
+      </c>
+      <c r="B168" t="s">
+        <v>794</v>
+      </c>
+      <c r="C168" t="s">
+        <v>795</v>
+      </c>
+      <c r="D168" t="s">
+        <v>796</v>
+      </c>
+      <c r="E168" t="s">
         <v>797</v>
       </c>
-      <c r="B168" t="s">
-        <v>798</v>
-      </c>
-      <c r="C168" t="s">
-        <v>799</v>
-      </c>
-      <c r="D168" t="s">
-        <v>800</v>
-      </c>
-      <c r="E168" t="s">
-        <v>801</v>
-      </c>
       <c r="F168" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H168">
         <f t="shared" si="12"/>
@@ -9774,22 +9777,22 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>802</v>
+        <v>798</v>
       </c>
       <c r="B169" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="C169" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="D169" t="s">
-        <v>804</v>
+        <v>800</v>
       </c>
       <c r="E169" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="F169" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H169">
         <f t="shared" si="12"/>
@@ -9806,22 +9809,22 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
+        <v>802</v>
+      </c>
+      <c r="B170" t="s">
+        <v>803</v>
+      </c>
+      <c r="C170" t="s">
+        <v>804</v>
+      </c>
+      <c r="D170" t="s">
+        <v>805</v>
+      </c>
+      <c r="E170" t="s">
         <v>806</v>
       </c>
-      <c r="B170" t="s">
-        <v>807</v>
-      </c>
-      <c r="C170" t="s">
-        <v>808</v>
-      </c>
-      <c r="D170" t="s">
-        <v>809</v>
-      </c>
-      <c r="E170" t="s">
-        <v>810</v>
-      </c>
       <c r="F170" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H170">
         <f t="shared" si="12"/>
@@ -9838,22 +9841,22 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>807</v>
+      </c>
+      <c r="B171" t="s">
+        <v>808</v>
+      </c>
+      <c r="C171" t="s">
+        <v>809</v>
+      </c>
+      <c r="D171" t="s">
+        <v>810</v>
+      </c>
+      <c r="E171" t="s">
         <v>811</v>
       </c>
-      <c r="B171" t="s">
-        <v>812</v>
-      </c>
-      <c r="C171" t="s">
-        <v>813</v>
-      </c>
-      <c r="D171" t="s">
-        <v>814</v>
-      </c>
-      <c r="E171" t="s">
-        <v>815</v>
-      </c>
       <c r="F171" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H171">
         <f t="shared" si="12"/>
@@ -9873,19 +9876,19 @@
         <v>404</v>
       </c>
       <c r="B172" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="C172" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D172" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="E172" t="s">
         <v>103</v>
       </c>
       <c r="F172" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H172">
         <f t="shared" si="12"/>
@@ -9902,22 +9905,22 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>815</v>
+      </c>
+      <c r="B173" t="s">
+        <v>816</v>
+      </c>
+      <c r="C173" t="s">
+        <v>817</v>
+      </c>
+      <c r="D173" t="s">
+        <v>818</v>
+      </c>
+      <c r="E173" t="s">
         <v>819</v>
       </c>
-      <c r="B173" t="s">
-        <v>820</v>
-      </c>
-      <c r="C173" t="s">
-        <v>821</v>
-      </c>
-      <c r="D173" t="s">
-        <v>822</v>
-      </c>
-      <c r="E173" t="s">
-        <v>823</v>
-      </c>
       <c r="F173" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H173">
         <f t="shared" si="12"/>
@@ -9934,22 +9937,22 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
+        <v>820</v>
+      </c>
+      <c r="B174" t="s">
+        <v>821</v>
+      </c>
+      <c r="C174" t="s">
+        <v>822</v>
+      </c>
+      <c r="D174" t="s">
+        <v>823</v>
+      </c>
+      <c r="E174" t="s">
         <v>824</v>
       </c>
-      <c r="B174" t="s">
-        <v>825</v>
-      </c>
-      <c r="C174" t="s">
-        <v>826</v>
-      </c>
-      <c r="D174" t="s">
-        <v>827</v>
-      </c>
-      <c r="E174" t="s">
-        <v>828</v>
-      </c>
       <c r="F174" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H174">
         <f t="shared" si="12"/>
@@ -9966,22 +9969,22 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
+        <v>825</v>
+      </c>
+      <c r="B175" t="s">
+        <v>826</v>
+      </c>
+      <c r="C175" t="s">
+        <v>827</v>
+      </c>
+      <c r="D175" t="s">
+        <v>828</v>
+      </c>
+      <c r="E175" t="s">
         <v>829</v>
       </c>
-      <c r="B175" t="s">
-        <v>830</v>
-      </c>
-      <c r="C175" t="s">
-        <v>831</v>
-      </c>
-      <c r="D175" t="s">
-        <v>832</v>
-      </c>
-      <c r="E175" t="s">
-        <v>833</v>
-      </c>
       <c r="F175" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H175">
         <f t="shared" si="12"/>
@@ -9998,22 +10001,22 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B176" t="s">
         <v>299</v>
       </c>
       <c r="C176" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="D176" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="E176" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="F176" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H176">
         <f t="shared" si="12"/>
@@ -10030,22 +10033,22 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
+        <v>834</v>
+      </c>
+      <c r="B177" t="s">
+        <v>835</v>
+      </c>
+      <c r="C177" t="s">
+        <v>836</v>
+      </c>
+      <c r="D177" t="s">
+        <v>837</v>
+      </c>
+      <c r="E177" t="s">
         <v>838</v>
       </c>
-      <c r="B177" t="s">
-        <v>839</v>
-      </c>
-      <c r="C177" t="s">
-        <v>840</v>
-      </c>
-      <c r="D177" t="s">
-        <v>841</v>
-      </c>
-      <c r="E177" t="s">
-        <v>842</v>
-      </c>
       <c r="F177" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H177">
         <f t="shared" si="12"/>
@@ -10062,22 +10065,22 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="B178" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="C178" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="D178" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="E178" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F178" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H178">
         <f t="shared" si="12"/>
@@ -10094,22 +10097,22 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
+        <v>848</v>
+      </c>
+      <c r="B179" t="s">
+        <v>849</v>
+      </c>
+      <c r="C179" t="s">
+        <v>850</v>
+      </c>
+      <c r="D179" t="s">
+        <v>851</v>
+      </c>
+      <c r="E179" t="s">
         <v>852</v>
       </c>
-      <c r="B179" t="s">
-        <v>853</v>
-      </c>
-      <c r="C179" t="s">
-        <v>854</v>
-      </c>
-      <c r="D179" t="s">
-        <v>855</v>
-      </c>
-      <c r="E179" t="s">
-        <v>856</v>
-      </c>
       <c r="F179" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H179">
         <f t="shared" si="12"/>
@@ -10126,22 +10129,22 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
+        <v>853</v>
+      </c>
+      <c r="B180" t="s">
+        <v>854</v>
+      </c>
+      <c r="C180" t="s">
+        <v>855</v>
+      </c>
+      <c r="D180" t="s">
+        <v>856</v>
+      </c>
+      <c r="E180" t="s">
         <v>857</v>
       </c>
-      <c r="B180" t="s">
-        <v>858</v>
-      </c>
-      <c r="C180" t="s">
-        <v>859</v>
-      </c>
-      <c r="D180" t="s">
-        <v>860</v>
-      </c>
-      <c r="E180" t="s">
-        <v>861</v>
-      </c>
       <c r="F180" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H180">
         <f t="shared" si="12"/>
@@ -10158,22 +10161,22 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
+        <v>858</v>
+      </c>
+      <c r="B181" t="s">
+        <v>859</v>
+      </c>
+      <c r="C181" t="s">
+        <v>860</v>
+      </c>
+      <c r="D181" t="s">
+        <v>861</v>
+      </c>
+      <c r="E181" t="s">
         <v>862</v>
       </c>
-      <c r="B181" t="s">
-        <v>863</v>
-      </c>
-      <c r="C181" t="s">
-        <v>864</v>
-      </c>
-      <c r="D181" t="s">
-        <v>865</v>
-      </c>
-      <c r="E181" t="s">
-        <v>866</v>
-      </c>
       <c r="F181" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H181">
         <f t="shared" si="12"/>
@@ -10190,22 +10193,22 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B182" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="C182" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D182" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
       <c r="E182" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="F182" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H182">
         <f t="shared" si="12"/>
@@ -10222,22 +10225,22 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
+        <v>863</v>
+      </c>
+      <c r="B183" t="s">
+        <v>864</v>
+      </c>
+      <c r="C183" t="s">
+        <v>865</v>
+      </c>
+      <c r="D183" t="s">
+        <v>866</v>
+      </c>
+      <c r="E183" t="s">
         <v>867</v>
       </c>
-      <c r="B183" t="s">
-        <v>868</v>
-      </c>
-      <c r="C183" t="s">
-        <v>869</v>
-      </c>
-      <c r="D183" t="s">
-        <v>870</v>
-      </c>
-      <c r="E183" t="s">
-        <v>871</v>
-      </c>
       <c r="F183" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H183">
         <f t="shared" si="12"/>
@@ -10254,22 +10257,22 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
+        <v>868</v>
+      </c>
+      <c r="B184" t="s">
+        <v>869</v>
+      </c>
+      <c r="C184" t="s">
+        <v>870</v>
+      </c>
+      <c r="D184" t="s">
+        <v>871</v>
+      </c>
+      <c r="E184" t="s">
         <v>872</v>
       </c>
-      <c r="B184" t="s">
-        <v>873</v>
-      </c>
-      <c r="C184" t="s">
-        <v>874</v>
-      </c>
-      <c r="D184" t="s">
-        <v>875</v>
-      </c>
-      <c r="E184" t="s">
-        <v>876</v>
-      </c>
       <c r="F184" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H184">
         <f t="shared" si="12"/>
@@ -10286,22 +10289,22 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
+        <v>873</v>
+      </c>
+      <c r="B185" t="s">
+        <v>874</v>
+      </c>
+      <c r="C185" t="s">
+        <v>875</v>
+      </c>
+      <c r="D185" t="s">
+        <v>876</v>
+      </c>
+      <c r="E185" t="s">
         <v>877</v>
       </c>
-      <c r="B185" t="s">
-        <v>878</v>
-      </c>
-      <c r="C185" t="s">
-        <v>879</v>
-      </c>
-      <c r="D185" t="s">
-        <v>880</v>
-      </c>
-      <c r="E185" t="s">
-        <v>881</v>
-      </c>
       <c r="F185" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H185">
         <f t="shared" si="12"/>
@@ -10318,22 +10321,22 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>878</v>
+      </c>
+      <c r="B186" t="s">
+        <v>879</v>
+      </c>
+      <c r="C186" t="s">
+        <v>880</v>
+      </c>
+      <c r="D186" t="s">
+        <v>881</v>
+      </c>
+      <c r="E186" t="s">
         <v>882</v>
       </c>
-      <c r="B186" t="s">
-        <v>883</v>
-      </c>
-      <c r="C186" t="s">
-        <v>884</v>
-      </c>
-      <c r="D186" t="s">
-        <v>885</v>
-      </c>
-      <c r="E186" t="s">
-        <v>886</v>
-      </c>
       <c r="F186" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H186">
         <f t="shared" si="12"/>
@@ -10350,22 +10353,22 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
+        <v>883</v>
+      </c>
+      <c r="B187" t="s">
+        <v>884</v>
+      </c>
+      <c r="C187" t="s">
+        <v>885</v>
+      </c>
+      <c r="D187" t="s">
+        <v>886</v>
+      </c>
+      <c r="E187" t="s">
         <v>887</v>
       </c>
-      <c r="B187" t="s">
-        <v>888</v>
-      </c>
-      <c r="C187" t="s">
-        <v>889</v>
-      </c>
-      <c r="D187" t="s">
-        <v>890</v>
-      </c>
-      <c r="E187" t="s">
-        <v>891</v>
-      </c>
       <c r="F187" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H187">
         <f t="shared" si="12"/>
@@ -10382,22 +10385,22 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>888</v>
+      </c>
+      <c r="B188" t="s">
+        <v>889</v>
+      </c>
+      <c r="C188" t="s">
+        <v>890</v>
+      </c>
+      <c r="D188" t="s">
+        <v>891</v>
+      </c>
+      <c r="E188" t="s">
         <v>892</v>
       </c>
-      <c r="B188" t="s">
-        <v>893</v>
-      </c>
-      <c r="C188" t="s">
-        <v>894</v>
-      </c>
-      <c r="D188" t="s">
-        <v>895</v>
-      </c>
-      <c r="E188" t="s">
-        <v>896</v>
-      </c>
       <c r="F188" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H188">
         <f t="shared" ref="H188:H222" si="15">INT(J188/3)</f>
@@ -10414,22 +10417,22 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
       <c r="B189" t="s">
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
       <c r="D189" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="E189" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
       <c r="F189" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H189">
         <f t="shared" si="15"/>
@@ -10446,22 +10449,22 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
+        <v>897</v>
+      </c>
+      <c r="B190" t="s">
+        <v>898</v>
+      </c>
+      <c r="C190" t="s">
+        <v>899</v>
+      </c>
+      <c r="D190" t="s">
+        <v>900</v>
+      </c>
+      <c r="E190" t="s">
         <v>901</v>
       </c>
-      <c r="B190" t="s">
-        <v>902</v>
-      </c>
-      <c r="C190" t="s">
-        <v>903</v>
-      </c>
-      <c r="D190" t="s">
-        <v>904</v>
-      </c>
-      <c r="E190" t="s">
-        <v>905</v>
-      </c>
       <c r="F190" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H190">
         <f t="shared" si="15"/>
@@ -10478,22 +10481,22 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B191" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
       <c r="C191" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D191" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
       <c r="E191" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
       <c r="F191" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H191">
         <f t="shared" si="15"/>
@@ -10510,22 +10513,22 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>751</v>
+      </c>
+      <c r="B192" t="s">
+        <v>752</v>
+      </c>
+      <c r="C192" t="s">
+        <v>753</v>
+      </c>
+      <c r="D192" t="s">
+        <v>754</v>
+      </c>
+      <c r="E192" t="s">
         <v>755</v>
       </c>
-      <c r="B192" t="s">
-        <v>756</v>
-      </c>
-      <c r="C192" t="s">
-        <v>757</v>
-      </c>
-      <c r="D192" t="s">
-        <v>758</v>
-      </c>
-      <c r="E192" t="s">
-        <v>759</v>
-      </c>
       <c r="F192" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H192">
         <f t="shared" si="15"/>
@@ -10542,22 +10545,22 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>905</v>
+      </c>
+      <c r="B193" t="s">
+        <v>906</v>
+      </c>
+      <c r="C193" t="s">
+        <v>907</v>
+      </c>
+      <c r="D193" t="s">
+        <v>908</v>
+      </c>
+      <c r="E193" t="s">
         <v>909</v>
       </c>
-      <c r="B193" t="s">
-        <v>910</v>
-      </c>
-      <c r="C193" t="s">
-        <v>911</v>
-      </c>
-      <c r="D193" t="s">
-        <v>912</v>
-      </c>
-      <c r="E193" t="s">
-        <v>913</v>
-      </c>
       <c r="F193" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H193">
         <f t="shared" si="15"/>
@@ -10574,22 +10577,22 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>910</v>
+      </c>
+      <c r="B194" t="s">
+        <v>911</v>
+      </c>
+      <c r="C194" t="s">
+        <v>912</v>
+      </c>
+      <c r="D194" t="s">
+        <v>913</v>
+      </c>
+      <c r="E194" t="s">
         <v>914</v>
       </c>
-      <c r="B194" t="s">
-        <v>915</v>
-      </c>
-      <c r="C194" t="s">
-        <v>916</v>
-      </c>
-      <c r="D194" t="s">
-        <v>917</v>
-      </c>
-      <c r="E194" t="s">
-        <v>918</v>
-      </c>
       <c r="F194" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H194">
         <f t="shared" si="15"/>
@@ -10606,22 +10609,22 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="B195" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
       <c r="C195" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
       <c r="D195" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
       <c r="E195" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
       <c r="F195" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H195">
         <f t="shared" si="15"/>
@@ -10638,22 +10641,22 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>919</v>
+      </c>
+      <c r="B196" t="s">
+        <v>920</v>
+      </c>
+      <c r="C196" t="s">
+        <v>921</v>
+      </c>
+      <c r="D196" t="s">
+        <v>922</v>
+      </c>
+      <c r="E196" t="s">
         <v>923</v>
       </c>
-      <c r="B196" t="s">
-        <v>924</v>
-      </c>
-      <c r="C196" t="s">
-        <v>925</v>
-      </c>
-      <c r="D196" t="s">
-        <v>926</v>
-      </c>
-      <c r="E196" t="s">
-        <v>927</v>
-      </c>
       <c r="F196" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H196">
         <f t="shared" si="15"/>
@@ -10670,22 +10673,22 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>924</v>
+      </c>
+      <c r="B197" t="s">
+        <v>925</v>
+      </c>
+      <c r="C197" t="s">
+        <v>926</v>
+      </c>
+      <c r="D197" t="s">
+        <v>927</v>
+      </c>
+      <c r="E197" t="s">
         <v>928</v>
       </c>
-      <c r="B197" t="s">
-        <v>929</v>
-      </c>
-      <c r="C197" t="s">
-        <v>930</v>
-      </c>
-      <c r="D197" t="s">
-        <v>931</v>
-      </c>
-      <c r="E197" t="s">
-        <v>932</v>
-      </c>
       <c r="F197" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H197">
         <f t="shared" si="15"/>
@@ -10702,22 +10705,22 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
       <c r="B198" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="C198" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="D198" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
       <c r="E198" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="F198" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H198">
         <f t="shared" si="15"/>
@@ -10734,22 +10737,22 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B199" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C199" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D199" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="E199" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="F199" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H199">
         <f t="shared" si="15"/>
@@ -10766,22 +10769,22 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>935</v>
+      </c>
+      <c r="B200" t="s">
+        <v>936</v>
+      </c>
+      <c r="C200" t="s">
+        <v>937</v>
+      </c>
+      <c r="D200" t="s">
+        <v>938</v>
+      </c>
+      <c r="E200" t="s">
         <v>939</v>
       </c>
-      <c r="B200" t="s">
-        <v>940</v>
-      </c>
-      <c r="C200" t="s">
-        <v>941</v>
-      </c>
-      <c r="D200" t="s">
-        <v>942</v>
-      </c>
-      <c r="E200" t="s">
-        <v>943</v>
-      </c>
       <c r="F200" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H200">
         <f t="shared" si="15"/>
@@ -10798,22 +10801,22 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>940</v>
+      </c>
+      <c r="B201" t="s">
+        <v>941</v>
+      </c>
+      <c r="C201" t="s">
+        <v>942</v>
+      </c>
+      <c r="D201" t="s">
+        <v>943</v>
+      </c>
+      <c r="E201" t="s">
         <v>944</v>
       </c>
-      <c r="B201" t="s">
-        <v>945</v>
-      </c>
-      <c r="C201" t="s">
-        <v>946</v>
-      </c>
-      <c r="D201" t="s">
-        <v>947</v>
-      </c>
-      <c r="E201" t="s">
-        <v>948</v>
-      </c>
       <c r="F201" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H201">
         <f t="shared" si="15"/>
@@ -10830,22 +10833,22 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>945</v>
+      </c>
+      <c r="B202" t="s">
+        <v>946</v>
+      </c>
+      <c r="C202" t="s">
+        <v>947</v>
+      </c>
+      <c r="D202" t="s">
+        <v>948</v>
+      </c>
+      <c r="E202" t="s">
         <v>949</v>
       </c>
-      <c r="B202" t="s">
-        <v>950</v>
-      </c>
-      <c r="C202" t="s">
-        <v>951</v>
-      </c>
-      <c r="D202" t="s">
-        <v>952</v>
-      </c>
-      <c r="E202" t="s">
-        <v>953</v>
-      </c>
       <c r="F202" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H202">
         <f t="shared" si="15"/>
@@ -10865,19 +10868,19 @@
         <v>371</v>
       </c>
       <c r="B203" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="C203" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
       <c r="D203" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="E203" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="F203" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H203">
         <f t="shared" si="15"/>
@@ -10894,22 +10897,22 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>954</v>
+      </c>
+      <c r="B204" t="s">
+        <v>955</v>
+      </c>
+      <c r="C204" t="s">
+        <v>956</v>
+      </c>
+      <c r="D204" t="s">
+        <v>957</v>
+      </c>
+      <c r="E204" t="s">
         <v>958</v>
       </c>
-      <c r="B204" t="s">
-        <v>959</v>
-      </c>
-      <c r="C204" t="s">
-        <v>960</v>
-      </c>
-      <c r="D204" t="s">
-        <v>961</v>
-      </c>
-      <c r="E204" t="s">
-        <v>962</v>
-      </c>
       <c r="F204" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H204">
         <f t="shared" si="15"/>
@@ -10926,22 +10929,22 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>959</v>
+      </c>
+      <c r="B205" t="s">
+        <v>960</v>
+      </c>
+      <c r="C205" t="s">
+        <v>961</v>
+      </c>
+      <c r="D205" t="s">
+        <v>962</v>
+      </c>
+      <c r="E205" t="s">
         <v>963</v>
       </c>
-      <c r="B205" t="s">
-        <v>964</v>
-      </c>
-      <c r="C205" t="s">
-        <v>965</v>
-      </c>
-      <c r="D205" t="s">
-        <v>966</v>
-      </c>
-      <c r="E205" t="s">
-        <v>967</v>
-      </c>
       <c r="F205" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H205">
         <f t="shared" si="15"/>
@@ -10958,22 +10961,22 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
       <c r="B206" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="C206" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
       <c r="D206" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
       <c r="E206" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
       <c r="F206" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H206">
         <f t="shared" si="15"/>
@@ -10990,22 +10993,22 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
       <c r="B207" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
       <c r="C207" t="s">
         <v>392</v>
       </c>
       <c r="D207" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="E207" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
       <c r="F207" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H207">
         <f t="shared" si="15"/>
@@ -11022,22 +11025,22 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>972</v>
+      </c>
+      <c r="B208" t="s">
+        <v>973</v>
+      </c>
+      <c r="C208" t="s">
+        <v>974</v>
+      </c>
+      <c r="D208" t="s">
+        <v>975</v>
+      </c>
+      <c r="E208" t="s">
         <v>976</v>
       </c>
-      <c r="B208" t="s">
-        <v>977</v>
-      </c>
-      <c r="C208" t="s">
-        <v>978</v>
-      </c>
-      <c r="D208" t="s">
-        <v>979</v>
-      </c>
-      <c r="E208" t="s">
-        <v>980</v>
-      </c>
       <c r="F208" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H208">
         <f t="shared" si="15"/>
@@ -11054,22 +11057,22 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="B209" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
       <c r="C209" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
       <c r="D209" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
       <c r="E209" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
       <c r="F209" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H209">
         <f t="shared" si="15"/>
@@ -11086,22 +11089,22 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
       <c r="B210" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
       <c r="C210" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="D210" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="E210" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="F210" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H210">
         <f t="shared" si="15"/>
@@ -11118,22 +11121,22 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="B211" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
       <c r="C211" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="D211" t="s">
         <v>456</v>
       </c>
       <c r="E211" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="F211" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H211">
         <f t="shared" si="15"/>
@@ -11150,22 +11153,22 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="B212" t="s">
         <v>78</v>
       </c>
       <c r="C212" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
       <c r="D212" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="E212" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="F212" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H212">
         <f t="shared" si="15"/>
@@ -11182,22 +11185,22 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>993</v>
+      </c>
+      <c r="B213" t="s">
+        <v>994</v>
+      </c>
+      <c r="C213" t="s">
+        <v>995</v>
+      </c>
+      <c r="D213" t="s">
+        <v>996</v>
+      </c>
+      <c r="E213" t="s">
         <v>997</v>
       </c>
-      <c r="B213" t="s">
-        <v>998</v>
-      </c>
-      <c r="C213" t="s">
-        <v>999</v>
-      </c>
-      <c r="D213" t="s">
-        <v>1000</v>
-      </c>
-      <c r="E213" t="s">
-        <v>1001</v>
-      </c>
       <c r="F213" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H213">
         <f t="shared" si="15"/>
@@ -11214,22 +11217,22 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
+        <v>998</v>
+      </c>
+      <c r="B214" t="s">
+        <v>999</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D214" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E214" t="s">
         <v>1002</v>
       </c>
-      <c r="B214" t="s">
-        <v>1003</v>
-      </c>
-      <c r="C214" t="s">
-        <v>1004</v>
-      </c>
-      <c r="D214" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E214" t="s">
-        <v>1006</v>
-      </c>
       <c r="F214" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H214">
         <f t="shared" si="15"/>
@@ -11246,22 +11249,22 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B215" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
       <c r="C215" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
       <c r="D215" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="E215" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
       <c r="F215" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H215">
         <f t="shared" si="15"/>
@@ -11278,22 +11281,22 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B216" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E216" t="s">
         <v>1011</v>
       </c>
-      <c r="B216" t="s">
-        <v>1012</v>
-      </c>
-      <c r="C216" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D216" t="s">
-        <v>1014</v>
-      </c>
-      <c r="E216" t="s">
-        <v>1015</v>
-      </c>
       <c r="F216" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H216">
         <f t="shared" si="15"/>
@@ -11310,22 +11313,22 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
       <c r="B217" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
       <c r="C217" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="D217" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
       <c r="E217" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
       <c r="F217" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H217">
         <f t="shared" si="15"/>
@@ -11342,22 +11345,22 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="B218" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
       <c r="C218" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
       <c r="D218" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="E218" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
       <c r="F218" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H218">
         <f t="shared" si="15"/>
@@ -11377,19 +11380,19 @@
         <v>64</v>
       </c>
       <c r="B219" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C219" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
       <c r="D219" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
       <c r="E219" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
       <c r="F219" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H219">
         <f t="shared" si="15"/>
@@ -11406,22 +11409,22 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B220" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C220" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D220" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E220" t="s">
         <v>1030</v>
       </c>
-      <c r="B220" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C220" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D220" t="s">
-        <v>1033</v>
-      </c>
-      <c r="E220" t="s">
-        <v>1034</v>
-      </c>
       <c r="F220" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="H220">
         <f t="shared" si="15"/>
@@ -11438,22 +11441,22 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B221" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C221" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D221" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E221" t="s">
         <v>1035</v>
       </c>
-      <c r="B221" t="s">
-        <v>1036</v>
-      </c>
-      <c r="C221" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D221" t="s">
-        <v>1038</v>
-      </c>
-      <c r="E221" t="s">
-        <v>1039</v>
-      </c>
       <c r="F221" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H221">
         <f t="shared" si="15"/>
@@ -11473,19 +11476,19 @@
         <v>14</v>
       </c>
       <c r="B222" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="C222" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
       <c r="D222" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="E222" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="F222" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="H222">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
Timer stopping and Share message and words
</commit_message>
<xml_diff>
--- a/code/shabdakala/resource/sbwords.xlsx
+++ b/code/shabdakala/resource/sbwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/shabdak_github/sbbd/shabdakala/code/shabdakala/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61C43C-072A-4245-A288-61F46AAE511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619C52C7-88D2-EC41-9FAA-7CD2A3FC7DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9F74AEE5-EB85-4044-AC84-8761A591B5C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1045">
   <si>
     <t>word0</t>
   </si>
@@ -1463,24 +1463,12 @@
     <t>फुले</t>
   </si>
   <si>
-    <t>लागु</t>
-  </si>
-  <si>
     <t>जुन्या मराठी चित्रपटातल्या अभिनेत्यांची आडनावे</t>
   </si>
   <si>
-    <t>स्क्रीन</t>
-  </si>
-  <si>
     <t>खिडकी</t>
   </si>
   <si>
-    <t>भिंगं</t>
-  </si>
-  <si>
-    <t>बाटली</t>
-  </si>
-  <si>
     <t>काचेच्या वस्तु</t>
   </si>
   <si>
@@ -1502,15 +1490,9 @@
     <t>तिरंगा</t>
   </si>
   <si>
-    <t>फडकणे</t>
-  </si>
-  <si>
     <t>स्तंभ</t>
   </si>
   <si>
-    <t>वंदना</t>
-  </si>
-  <si>
     <t>झेंड्या बाबत</t>
   </si>
   <si>
@@ -3171,6 +3153,21 @@
   </si>
   <si>
     <t>अडीच</t>
+  </si>
+  <si>
+    <t>लागू</t>
+  </si>
+  <si>
+    <t>दौत</t>
+  </si>
+  <si>
+    <t>पेला</t>
+  </si>
+  <si>
+    <t>फडकवणे</t>
+  </si>
+  <si>
+    <t>मानवंदना</t>
   </si>
 </sst>
 </file>
@@ -4097,8 +4094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1707B-2FB7-B84C-9F84-E9F074F3056C}">
   <dimension ref="A1:L222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4186,7 +4183,7 @@
       </c>
       <c r="L2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45651</v>
+        <v>45652</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -4981,7 +4978,7 @@
         <v>370</v>
       </c>
       <c r="F25" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>185</v>
@@ -5086,7 +5083,7 @@
         <v>426</v>
       </c>
       <c r="F28" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>432</v>
@@ -5211,22 +5208,22 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="B32" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C32" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="D32" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="E32" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="F32" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H32">
         <f t="shared" si="7"/>
@@ -5243,22 +5240,22 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="B33" t="s">
         <v>371</v>
       </c>
       <c r="C33" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
       </c>
       <c r="E33" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="F33" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H33">
         <f t="shared" si="7"/>
@@ -5275,22 +5272,22 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="B34" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="C34" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
       </c>
       <c r="E34" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="F34" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H34">
         <f t="shared" si="7"/>
@@ -5354,7 +5351,7 @@
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>339</v>
@@ -5389,7 +5386,7 @@
         <v>111</v>
       </c>
       <c r="E37" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>85</v>
@@ -5412,22 +5409,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="B38" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
       <c r="C38" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="D38" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="E38" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="F38" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H38">
         <f t="shared" si="7"/>
@@ -5444,22 +5441,22 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="B39" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="E39" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="F39" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H39">
         <f t="shared" si="7"/>
@@ -5546,22 +5543,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="B42" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C42" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="D42" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="E42" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="F42" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H42">
         <f t="shared" si="7"/>
@@ -5578,22 +5575,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B43" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="C43" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="D43" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="E43" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="F43" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H43">
         <f t="shared" si="7"/>
@@ -5625,7 +5622,7 @@
         <v>378</v>
       </c>
       <c r="F44" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>275</v>
@@ -5680,22 +5677,22 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B46" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C46" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="D46" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="E46" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="F46" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H46">
         <f t="shared" si="7"/>
@@ -5715,19 +5712,19 @@
         <v>228</v>
       </c>
       <c r="B47" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="C47" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="D47" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="E47" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F47" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H47">
         <f t="shared" si="7"/>
@@ -5744,22 +5741,22 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="B48" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C48" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="D48" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="E48" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="F48" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H48">
         <f t="shared" si="7"/>
@@ -5826,7 +5823,7 @@
         <v>416</v>
       </c>
       <c r="F50" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>275</v>
@@ -5852,7 +5849,7 @@
         <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="D51" t="s">
         <v>121</v>
@@ -5881,7 +5878,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="B52" t="s">
         <v>36</v>
@@ -5954,7 +5951,7 @@
         <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="C54" t="s">
         <v>213</v>
@@ -6001,7 +5998,7 @@
         <v>433</v>
       </c>
       <c r="F55" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>275</v>
@@ -6024,19 +6021,19 @@
         <v>233</v>
       </c>
       <c r="B56" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C56" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="D56" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="E56" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F56" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H56">
         <f t="shared" si="7"/>
@@ -6059,7 +6056,7 @@
         <v>232</v>
       </c>
       <c r="C57" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="D57" t="s">
         <v>234</v>
@@ -6088,19 +6085,19 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="B58" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C58" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="D58" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="E58" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="F58" t="s">
         <v>444</v>
@@ -6132,10 +6129,10 @@
         <v>467</v>
       </c>
       <c r="E59" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="F59" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H59">
         <f t="shared" si="7"/>
@@ -6152,22 +6149,22 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="B60" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="C60" t="s">
         <v>468</v>
       </c>
       <c r="D60" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="E60" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="F60" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H60">
         <f t="shared" ref="H60:H123" si="9">INT(J60/3)</f>
@@ -6184,7 +6181,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
       <c r="B61" t="s">
         <v>469</v>
@@ -6199,7 +6196,7 @@
         <v>472</v>
       </c>
       <c r="F61" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H61">
         <f t="shared" si="9"/>
@@ -6216,22 +6213,22 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
       <c r="B62" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="C62" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="D62" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="E62" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="F62" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H62">
         <f t="shared" si="9"/>
@@ -6248,19 +6245,19 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="B63" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="C63" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="D63" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="E63" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>444</v>
@@ -6296,7 +6293,7 @@
         <v>375</v>
       </c>
       <c r="F64" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>275</v>
@@ -6436,7 +6433,7 @@
         <v>421</v>
       </c>
       <c r="F68" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>275</v>
@@ -6471,7 +6468,7 @@
         <v>408</v>
       </c>
       <c r="F69" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>431</v>
@@ -6503,10 +6500,10 @@
         <v>461</v>
       </c>
       <c r="E70" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="F70" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H70">
         <f t="shared" si="9"/>
@@ -6561,19 +6558,19 @@
         <v>213</v>
       </c>
       <c r="B72" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="C72" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="D72" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="E72" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="F72" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H72">
         <f t="shared" si="9"/>
@@ -6590,22 +6587,22 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="B73" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="C73" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="D73" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="E73" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="F73" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H73">
         <f t="shared" si="9"/>
@@ -6622,22 +6619,22 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="B74" t="s">
-        <v>840</v>
+        <v>834</v>
       </c>
       <c r="C74" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
       <c r="D74" t="s">
-        <v>842</v>
+        <v>836</v>
       </c>
       <c r="E74" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="F74" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H74">
         <f t="shared" si="9"/>
@@ -6669,7 +6666,7 @@
         <v>427</v>
       </c>
       <c r="F75" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>275</v>
@@ -6794,22 +6791,22 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B79" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C79" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="D79" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="E79" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="F79" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H79">
         <f t="shared" si="9"/>
@@ -6826,22 +6823,22 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B80" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C80" t="s">
         <v>302</v>
       </c>
       <c r="D80" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="E80" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F80" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H80">
         <f t="shared" si="9"/>
@@ -6896,13 +6893,13 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="C82" t="s">
         <v>282</v>
       </c>
       <c r="D82" t="s">
-        <v>1040</v>
+        <v>1034</v>
       </c>
       <c r="E82" t="s">
         <v>316</v>
@@ -6934,7 +6931,7 @@
         <v>457</v>
       </c>
       <c r="C83" t="s">
-        <v>1042</v>
+        <v>1036</v>
       </c>
       <c r="D83" t="s">
         <v>458</v>
@@ -6943,7 +6940,7 @@
         <v>459</v>
       </c>
       <c r="F83" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H83">
         <f t="shared" si="9"/>
@@ -6960,22 +6957,22 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1045</v>
+        <v>1039</v>
       </c>
       <c r="B84" t="s">
-        <v>1044</v>
+        <v>1038</v>
       </c>
       <c r="C84" t="s">
-        <v>1041</v>
+        <v>1035</v>
       </c>
       <c r="D84" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
       <c r="E84" t="s">
-        <v>1039</v>
+        <v>1033</v>
       </c>
       <c r="F84" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H84">
         <f t="shared" si="9"/>
@@ -7007,7 +7004,7 @@
         <v>391</v>
       </c>
       <c r="F85" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>428</v>
@@ -7071,13 +7068,13 @@
         <v>475</v>
       </c>
       <c r="D87" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E87" t="s">
         <v>476</v>
       </c>
-      <c r="E87" t="s">
-        <v>477</v>
-      </c>
       <c r="F87" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H87">
         <f t="shared" si="9"/>
@@ -7094,22 +7091,22 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B88" t="s">
+        <v>477</v>
+      </c>
+      <c r="C88" t="s">
+        <v>675</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E88" t="s">
         <v>478</v>
       </c>
-      <c r="B88" t="s">
-        <v>479</v>
-      </c>
-      <c r="C88" t="s">
-        <v>480</v>
-      </c>
-      <c r="D88" t="s">
-        <v>481</v>
-      </c>
-      <c r="E88" t="s">
-        <v>482</v>
-      </c>
       <c r="F88" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H88">
         <f t="shared" si="9"/>
@@ -7196,22 +7193,22 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B91" t="s">
-        <v>489</v>
+        <v>1043</v>
       </c>
       <c r="C91" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D91" t="s">
-        <v>491</v>
+        <v>1044</v>
       </c>
       <c r="E91" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="F91" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H91">
         <f t="shared" si="9"/>
@@ -7228,22 +7225,22 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B92" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="C92" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="D92" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="E92" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F92" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H92">
         <f t="shared" si="9"/>
@@ -7260,22 +7257,22 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="B93" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C93" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="D93" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="E93" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="F93" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H93">
         <f t="shared" si="9"/>
@@ -7397,22 +7394,22 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="B97" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="C97" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="D97" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="E97" t="s">
         <v>162</v>
       </c>
       <c r="F97" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H97">
         <f t="shared" si="9"/>
@@ -7432,19 +7429,19 @@
         <v>162</v>
       </c>
       <c r="B98" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C98" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="D98" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="E98" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="F98" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H98">
         <f t="shared" si="9"/>
@@ -7461,22 +7458,22 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="B99" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="C99" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="D99" t="s">
         <v>151</v>
       </c>
       <c r="E99" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="F99" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H99">
         <f t="shared" si="9"/>
@@ -7508,7 +7505,7 @@
         <v>397</v>
       </c>
       <c r="F100" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>275</v>
@@ -7601,7 +7598,7 @@
         <v>411</v>
       </c>
       <c r="B103" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C103" t="s">
         <v>410</v>
@@ -7610,10 +7607,10 @@
         <v>412</v>
       </c>
       <c r="E103" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="F103" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H103">
         <f t="shared" si="9"/>
@@ -7630,22 +7627,22 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="B104" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="C104" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="D104" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E104" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="F104" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H104">
         <f t="shared" si="9"/>
@@ -7668,16 +7665,16 @@
         <v>392</v>
       </c>
       <c r="C105" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="D105" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="E105" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="F105" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H105">
         <f t="shared" si="9"/>
@@ -7694,22 +7691,22 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="B106" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="C106" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D106" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="E106" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="F106" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H106">
         <f t="shared" si="9"/>
@@ -7726,22 +7723,22 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="B107" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="C107" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="D107" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="E107" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="F107" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H107">
         <f t="shared" si="9"/>
@@ -7898,22 +7895,22 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="B112" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="C112" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="D112" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="E112" t="s">
+        <v>601</v>
+      </c>
+      <c r="F112" t="s">
         <v>607</v>
-      </c>
-      <c r="F112" t="s">
-        <v>613</v>
       </c>
       <c r="H112">
         <f t="shared" si="9"/>
@@ -7930,22 +7927,22 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="B113" t="s">
         <v>463</v>
       </c>
       <c r="C113" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="D113" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E113" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="F113" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H113">
         <f t="shared" si="9"/>
@@ -7962,22 +7959,22 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="B114" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="C114" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="D114" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="E114" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="F114" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H114">
         <f t="shared" si="9"/>
@@ -8009,7 +8006,7 @@
         <v>424</v>
       </c>
       <c r="F115" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>87</v>
@@ -8029,22 +8026,22 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B116" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="C116" t="s">
         <v>412</v>
       </c>
       <c r="D116" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="E116" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="F116" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H116">
         <f t="shared" si="9"/>
@@ -8061,22 +8058,22 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="B117" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C117" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="D117" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="E117" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="F117" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H117">
         <f t="shared" si="9"/>
@@ -8093,22 +8090,22 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="B118" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C118" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="D118" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="E118" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="F118" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H118">
         <f t="shared" si="9"/>
@@ -8230,22 +8227,22 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="B122" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="C122" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="D122" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="E122" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="F122" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H122">
         <f t="shared" si="9"/>
@@ -8297,7 +8294,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="B124" t="s">
         <v>425</v>
@@ -8312,7 +8309,7 @@
         <v>430</v>
       </c>
       <c r="F124" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>429</v>
@@ -8402,22 +8399,22 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="B127" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="C127" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="D127" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="E127" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="F127" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H127">
         <f t="shared" si="12"/>
@@ -8749,22 +8746,22 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B137" t="s">
         <v>232</v>
       </c>
       <c r="C137" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="D137" t="s">
         <v>231</v>
       </c>
       <c r="E137" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="F137" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H137">
         <f t="shared" si="12"/>
@@ -8793,7 +8790,7 @@
         <v>43</v>
       </c>
       <c r="E138" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>339</v>
@@ -8816,22 +8813,22 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B139" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
       <c r="C139" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="D139" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
       <c r="E139" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="F139" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139">
@@ -8849,22 +8846,22 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B140" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="C140" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="D140" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="E140" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="F140" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H140">
         <f t="shared" si="12"/>
@@ -8881,22 +8878,22 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="B141" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="C141" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="D141" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="E141" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="F141" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H141">
         <f t="shared" si="12"/>
@@ -8913,22 +8910,22 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="B142" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="C142" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="D142" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="E142" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
       <c r="F142" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H142">
         <f t="shared" si="12"/>
@@ -8945,22 +8942,22 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="B143" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="C143" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="D143" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="E143" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="F143" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H143">
         <f t="shared" si="12"/>
@@ -8977,22 +8974,22 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>685</v>
+        <v>679</v>
       </c>
       <c r="B144" t="s">
         <v>228</v>
       </c>
       <c r="C144" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="D144" t="s">
-        <v>687</v>
+        <v>681</v>
       </c>
       <c r="E144" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="F144" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H144">
         <f t="shared" si="12"/>
@@ -9009,22 +9006,22 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>689</v>
+        <v>683</v>
       </c>
       <c r="B145" t="s">
-        <v>690</v>
+        <v>684</v>
       </c>
       <c r="C145" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="D145" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="E145" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="F145" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H145">
         <f t="shared" si="12"/>
@@ -9041,22 +9038,22 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="B146" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="C146" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="D146" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="E146" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="F146" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H146">
         <f t="shared" si="12"/>
@@ -9073,22 +9070,22 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="B147" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="C147" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
       <c r="D147" t="s">
-        <v>701</v>
+        <v>695</v>
       </c>
       <c r="E147" t="s">
-        <v>702</v>
+        <v>696</v>
       </c>
       <c r="F147" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H147">
         <f t="shared" si="12"/>
@@ -9105,22 +9102,22 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>703</v>
+        <v>697</v>
       </c>
       <c r="B148" t="s">
-        <v>704</v>
+        <v>698</v>
       </c>
       <c r="C148" t="s">
-        <v>705</v>
+        <v>699</v>
       </c>
       <c r="D148" t="s">
-        <v>706</v>
+        <v>700</v>
       </c>
       <c r="E148" t="s">
-        <v>707</v>
+        <v>701</v>
       </c>
       <c r="F148" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H148">
         <f t="shared" si="12"/>
@@ -9137,22 +9134,22 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>708</v>
+        <v>702</v>
       </c>
       <c r="B149" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="C149" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="D149" t="s">
-        <v>711</v>
+        <v>705</v>
       </c>
       <c r="E149" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="F149" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H149">
         <f t="shared" si="12"/>
@@ -9169,22 +9166,22 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="B150" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="C150" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="D150" t="s">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="E150" t="s">
-        <v>717</v>
+        <v>711</v>
       </c>
       <c r="F150" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H150">
         <f t="shared" si="12"/>
@@ -9201,22 +9198,22 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>718</v>
+        <v>712</v>
       </c>
       <c r="B151" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
       <c r="C151" t="s">
-        <v>720</v>
+        <v>714</v>
       </c>
       <c r="D151" t="s">
-        <v>721</v>
+        <v>715</v>
       </c>
       <c r="E151" t="s">
-        <v>722</v>
+        <v>716</v>
       </c>
       <c r="F151" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H151">
         <f t="shared" si="12"/>
@@ -9233,22 +9230,22 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>723</v>
+        <v>717</v>
       </c>
       <c r="B152" t="s">
-        <v>724</v>
+        <v>718</v>
       </c>
       <c r="C152" t="s">
-        <v>725</v>
+        <v>719</v>
       </c>
       <c r="D152" t="s">
-        <v>726</v>
+        <v>720</v>
       </c>
       <c r="E152" t="s">
-        <v>727</v>
+        <v>721</v>
       </c>
       <c r="F152" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H152">
         <f t="shared" si="12"/>
@@ -9265,22 +9262,22 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="B153" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="C153" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="D153" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="E153" t="s">
         <v>246</v>
       </c>
       <c r="F153" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H153">
         <f t="shared" si="12"/>
@@ -9297,22 +9294,22 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="B154" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="C154" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="D154" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="E154" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="F154" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H154">
         <f t="shared" si="12"/>
@@ -9329,22 +9326,22 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="B155" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="C155" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="D155" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="E155" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="F155" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H155">
         <f t="shared" si="12"/>
@@ -9361,22 +9358,22 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="B156" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="C156" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="D156" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="E156" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="F156" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H156">
         <f t="shared" si="12"/>
@@ -9393,22 +9390,22 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="B157" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="C157" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="D157" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="E157" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="F157" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H157">
         <f t="shared" si="12"/>
@@ -9425,22 +9422,22 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="B158" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="C158" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="D158" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="E158" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="F158" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H158">
         <f t="shared" si="12"/>
@@ -9457,22 +9454,22 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B159" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C159" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="D159" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="E159" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="F159" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H159">
         <f t="shared" si="12"/>
@@ -9489,22 +9486,22 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="B160" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="C160" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="D160" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="E160" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="F160" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H160">
         <f t="shared" si="12"/>
@@ -9521,22 +9518,22 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="B161" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="C161" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="D161" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="E161" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="F161" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H161">
         <f t="shared" si="12"/>
@@ -9553,22 +9550,22 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B162" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="C162" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="D162" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="E162" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="F162" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H162">
         <f t="shared" si="12"/>
@@ -9585,22 +9582,22 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="B163" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="C163" t="s">
         <v>291</v>
       </c>
       <c r="D163" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="E163" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="F163" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H163">
         <f t="shared" si="12"/>
@@ -9617,22 +9614,22 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="B164" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="C164" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="D164" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="E164" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="F164" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H164">
         <f t="shared" si="12"/>
@@ -9649,22 +9646,22 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B165" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="C165" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
       <c r="D165" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="E165" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
       <c r="F165" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H165">
         <f t="shared" si="12"/>
@@ -9681,22 +9678,22 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="B166" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
       <c r="C166" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
       <c r="D166" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
       <c r="E166" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
       <c r="F166" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H166">
         <f t="shared" si="12"/>
@@ -9713,22 +9710,22 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
       <c r="B167" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="C167" t="s">
-        <v>790</v>
+        <v>784</v>
       </c>
       <c r="D167" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="E167" t="s">
-        <v>792</v>
+        <v>786</v>
       </c>
       <c r="F167" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H167">
         <f t="shared" si="12"/>
@@ -9745,22 +9742,22 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="B168" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="C168" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="D168" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="E168" t="s">
-        <v>797</v>
+        <v>791</v>
       </c>
       <c r="F168" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H168">
         <f t="shared" si="12"/>
@@ -9777,22 +9774,22 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>798</v>
+        <v>792</v>
       </c>
       <c r="B169" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C169" t="s">
-        <v>799</v>
+        <v>793</v>
       </c>
       <c r="D169" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="E169" t="s">
-        <v>801</v>
+        <v>795</v>
       </c>
       <c r="F169" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H169">
         <f t="shared" si="12"/>
@@ -9809,22 +9806,22 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>802</v>
+        <v>796</v>
       </c>
       <c r="B170" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="C170" t="s">
-        <v>804</v>
+        <v>798</v>
       </c>
       <c r="D170" t="s">
-        <v>805</v>
+        <v>799</v>
       </c>
       <c r="E170" t="s">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="F170" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H170">
         <f t="shared" si="12"/>
@@ -9841,22 +9838,22 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>807</v>
+        <v>801</v>
       </c>
       <c r="B171" t="s">
-        <v>808</v>
+        <v>802</v>
       </c>
       <c r="C171" t="s">
-        <v>809</v>
+        <v>803</v>
       </c>
       <c r="D171" t="s">
-        <v>810</v>
+        <v>804</v>
       </c>
       <c r="E171" t="s">
-        <v>811</v>
+        <v>805</v>
       </c>
       <c r="F171" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H171">
         <f t="shared" si="12"/>
@@ -9876,19 +9873,19 @@
         <v>404</v>
       </c>
       <c r="B172" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="C172" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="D172" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="E172" t="s">
         <v>103</v>
       </c>
       <c r="F172" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H172">
         <f t="shared" si="12"/>
@@ -9905,22 +9902,22 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="B173" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="C173" t="s">
-        <v>817</v>
+        <v>811</v>
       </c>
       <c r="D173" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="E173" t="s">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="F173" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H173">
         <f t="shared" si="12"/>
@@ -9937,22 +9934,22 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>820</v>
+        <v>814</v>
       </c>
       <c r="B174" t="s">
-        <v>821</v>
+        <v>815</v>
       </c>
       <c r="C174" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="D174" t="s">
-        <v>823</v>
+        <v>817</v>
       </c>
       <c r="E174" t="s">
-        <v>824</v>
+        <v>818</v>
       </c>
       <c r="F174" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H174">
         <f t="shared" si="12"/>
@@ -9969,22 +9966,22 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>825</v>
+        <v>819</v>
       </c>
       <c r="B175" t="s">
-        <v>826</v>
+        <v>820</v>
       </c>
       <c r="C175" t="s">
-        <v>827</v>
+        <v>821</v>
       </c>
       <c r="D175" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
       <c r="E175" t="s">
-        <v>829</v>
+        <v>823</v>
       </c>
       <c r="F175" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H175">
         <f t="shared" si="12"/>
@@ -10001,22 +9998,22 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>830</v>
+        <v>824</v>
       </c>
       <c r="B176" t="s">
         <v>299</v>
       </c>
       <c r="C176" t="s">
-        <v>831</v>
+        <v>825</v>
       </c>
       <c r="D176" t="s">
-        <v>832</v>
+        <v>826</v>
       </c>
       <c r="E176" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
       <c r="F176" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H176">
         <f t="shared" si="12"/>
@@ -10033,22 +10030,22 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="B177" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="C177" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
       <c r="D177" t="s">
-        <v>837</v>
+        <v>831</v>
       </c>
       <c r="E177" t="s">
-        <v>838</v>
+        <v>832</v>
       </c>
       <c r="F177" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H177">
         <f t="shared" si="12"/>
@@ -10065,22 +10062,22 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>844</v>
+        <v>838</v>
       </c>
       <c r="B178" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C178" t="s">
-        <v>845</v>
+        <v>839</v>
       </c>
       <c r="D178" t="s">
-        <v>846</v>
+        <v>840</v>
       </c>
       <c r="E178" t="s">
-        <v>847</v>
+        <v>841</v>
       </c>
       <c r="F178" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H178">
         <f t="shared" si="12"/>
@@ -10097,22 +10094,22 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>848</v>
+        <v>842</v>
       </c>
       <c r="B179" t="s">
-        <v>849</v>
+        <v>843</v>
       </c>
       <c r="C179" t="s">
-        <v>850</v>
+        <v>844</v>
       </c>
       <c r="D179" t="s">
-        <v>851</v>
+        <v>845</v>
       </c>
       <c r="E179" t="s">
-        <v>852</v>
+        <v>846</v>
       </c>
       <c r="F179" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H179">
         <f t="shared" si="12"/>
@@ -10129,22 +10126,22 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>853</v>
+        <v>847</v>
       </c>
       <c r="B180" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="C180" t="s">
-        <v>855</v>
+        <v>849</v>
       </c>
       <c r="D180" t="s">
-        <v>856</v>
+        <v>850</v>
       </c>
       <c r="E180" t="s">
-        <v>857</v>
+        <v>851</v>
       </c>
       <c r="F180" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H180">
         <f t="shared" si="12"/>
@@ -10161,22 +10158,22 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>858</v>
+        <v>852</v>
       </c>
       <c r="B181" t="s">
-        <v>859</v>
+        <v>853</v>
       </c>
       <c r="C181" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="D181" t="s">
-        <v>861</v>
+        <v>855</v>
       </c>
       <c r="E181" t="s">
-        <v>862</v>
+        <v>856</v>
       </c>
       <c r="F181" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H181">
         <f t="shared" si="12"/>
@@ -10193,22 +10190,22 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B182" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C182" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="D182" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="E182" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="F182" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H182">
         <f t="shared" si="12"/>
@@ -10225,22 +10222,22 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>863</v>
+        <v>857</v>
       </c>
       <c r="B183" t="s">
-        <v>864</v>
+        <v>858</v>
       </c>
       <c r="C183" t="s">
-        <v>865</v>
+        <v>859</v>
       </c>
       <c r="D183" t="s">
-        <v>866</v>
+        <v>860</v>
       </c>
       <c r="E183" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="F183" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H183">
         <f t="shared" si="12"/>
@@ -10257,22 +10254,22 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="B184" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="C184" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="D184" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="E184" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="F184" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H184">
         <f t="shared" si="12"/>
@@ -10289,22 +10286,22 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="B185" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
       <c r="C185" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="D185" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
       <c r="E185" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="F185" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H185">
         <f t="shared" si="12"/>
@@ -10321,22 +10318,22 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="B186" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="C186" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="D186" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="E186" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="F186" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H186">
         <f t="shared" si="12"/>
@@ -10353,22 +10350,22 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="B187" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="C187" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="D187" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="E187" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
       <c r="F187" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H187">
         <f t="shared" si="12"/>
@@ -10385,22 +10382,22 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
       <c r="B188" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="C188" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="D188" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="E188" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="F188" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H188">
         <f t="shared" ref="H188:H222" si="15">INT(J188/3)</f>
@@ -10417,22 +10414,22 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="B189" t="s">
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="D189" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="E189" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
       <c r="F189" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H189">
         <f t="shared" si="15"/>
@@ -10449,22 +10446,22 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="B190" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
       <c r="C190" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="D190" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="E190" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="F190" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H190">
         <f t="shared" si="15"/>
@@ -10481,22 +10478,22 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>686</v>
+        <v>680</v>
       </c>
       <c r="B191" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="C191" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D191" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="E191" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="F191" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H191">
         <f t="shared" si="15"/>
@@ -10513,22 +10510,22 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="B192" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="C192" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="D192" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="E192" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="F192" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H192">
         <f t="shared" si="15"/>
@@ -10545,22 +10542,22 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
       <c r="B193" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="C193" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="D193" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="E193" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="F193" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H193">
         <f t="shared" si="15"/>
@@ -10577,22 +10574,22 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="B194" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="C194" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="D194" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="E194" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="F194" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H194">
         <f t="shared" si="15"/>
@@ -10609,22 +10606,22 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
       <c r="B195" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="C195" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="D195" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="E195" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
       <c r="F195" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H195">
         <f t="shared" si="15"/>
@@ -10641,22 +10638,22 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="B196" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="C196" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="D196" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="E196" t="s">
-        <v>923</v>
+        <v>917</v>
       </c>
       <c r="F196" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H196">
         <f t="shared" si="15"/>
@@ -10673,22 +10670,22 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>924</v>
+        <v>918</v>
       </c>
       <c r="B197" t="s">
-        <v>925</v>
+        <v>919</v>
       </c>
       <c r="C197" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
       <c r="D197" t="s">
-        <v>927</v>
+        <v>921</v>
       </c>
       <c r="E197" t="s">
-        <v>928</v>
+        <v>922</v>
       </c>
       <c r="F197" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H197">
         <f t="shared" si="15"/>
@@ -10705,22 +10702,22 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="B198" t="s">
-        <v>929</v>
+        <v>923</v>
       </c>
       <c r="C198" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
       <c r="D198" t="s">
-        <v>931</v>
+        <v>925</v>
       </c>
       <c r="E198" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="F198" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H198">
         <f t="shared" si="15"/>
@@ -10737,22 +10734,22 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>818</v>
+        <v>812</v>
       </c>
       <c r="B199" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C199" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="D199" t="s">
-        <v>933</v>
+        <v>927</v>
       </c>
       <c r="E199" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="F199" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H199">
         <f t="shared" si="15"/>
@@ -10769,22 +10766,22 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="B200" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="C200" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="D200" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="E200" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="F200" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H200">
         <f t="shared" si="15"/>
@@ -10801,22 +10798,22 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
       <c r="B201" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="C201" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="D201" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="E201" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
       <c r="F201" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H201">
         <f t="shared" si="15"/>
@@ -10833,22 +10830,22 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
       <c r="B202" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="C202" t="s">
-        <v>947</v>
+        <v>941</v>
       </c>
       <c r="D202" t="s">
-        <v>948</v>
+        <v>942</v>
       </c>
       <c r="E202" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
       <c r="F202" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H202">
         <f t="shared" si="15"/>
@@ -10868,19 +10865,19 @@
         <v>371</v>
       </c>
       <c r="B203" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="C203" t="s">
-        <v>951</v>
+        <v>945</v>
       </c>
       <c r="D203" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="E203" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="F203" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H203">
         <f t="shared" si="15"/>
@@ -10897,22 +10894,22 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="B204" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="C204" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
       <c r="D204" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
       <c r="E204" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
       <c r="F204" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H204">
         <f t="shared" si="15"/>
@@ -10929,22 +10926,22 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
       <c r="B205" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="C205" t="s">
-        <v>961</v>
+        <v>955</v>
       </c>
       <c r="D205" t="s">
-        <v>962</v>
+        <v>956</v>
       </c>
       <c r="E205" t="s">
-        <v>963</v>
+        <v>957</v>
       </c>
       <c r="F205" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H205">
         <f t="shared" si="15"/>
@@ -10961,22 +10958,22 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>964</v>
+        <v>958</v>
       </c>
       <c r="B206" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="C206" t="s">
-        <v>965</v>
+        <v>959</v>
       </c>
       <c r="D206" t="s">
-        <v>966</v>
+        <v>960</v>
       </c>
       <c r="E206" t="s">
-        <v>967</v>
+        <v>961</v>
       </c>
       <c r="F206" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H206">
         <f t="shared" si="15"/>
@@ -10993,22 +10990,22 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
       <c r="B207" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="C207" t="s">
         <v>392</v>
       </c>
       <c r="D207" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E207" t="s">
-        <v>971</v>
+        <v>965</v>
       </c>
       <c r="F207" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H207">
         <f t="shared" si="15"/>
@@ -11025,22 +11022,22 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>972</v>
+        <v>966</v>
       </c>
       <c r="B208" t="s">
-        <v>973</v>
+        <v>967</v>
       </c>
       <c r="C208" t="s">
-        <v>974</v>
+        <v>968</v>
       </c>
       <c r="D208" t="s">
-        <v>975</v>
+        <v>969</v>
       </c>
       <c r="E208" t="s">
-        <v>976</v>
+        <v>970</v>
       </c>
       <c r="F208" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H208">
         <f t="shared" si="15"/>
@@ -11057,22 +11054,22 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="B209" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="C209" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
       <c r="D209" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="E209" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="F209" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H209">
         <f t="shared" si="15"/>
@@ -11089,22 +11086,22 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>981</v>
+        <v>975</v>
       </c>
       <c r="B210" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
       <c r="C210" t="s">
-        <v>983</v>
+        <v>977</v>
       </c>
       <c r="D210" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="E210" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
       <c r="F210" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H210">
         <f t="shared" si="15"/>
@@ -11121,22 +11118,22 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>985</v>
+        <v>979</v>
       </c>
       <c r="B211" t="s">
-        <v>986</v>
+        <v>980</v>
       </c>
       <c r="C211" t="s">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="D211" t="s">
         <v>456</v>
       </c>
       <c r="E211" t="s">
-        <v>988</v>
+        <v>982</v>
       </c>
       <c r="F211" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H211">
         <f t="shared" si="15"/>
@@ -11153,22 +11150,22 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>989</v>
+        <v>983</v>
       </c>
       <c r="B212" t="s">
         <v>78</v>
       </c>
       <c r="C212" t="s">
-        <v>990</v>
+        <v>984</v>
       </c>
       <c r="D212" t="s">
-        <v>991</v>
+        <v>985</v>
       </c>
       <c r="E212" t="s">
-        <v>992</v>
+        <v>986</v>
       </c>
       <c r="F212" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H212">
         <f t="shared" si="15"/>
@@ -11185,22 +11182,22 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>993</v>
+        <v>987</v>
       </c>
       <c r="B213" t="s">
-        <v>994</v>
+        <v>988</v>
       </c>
       <c r="C213" t="s">
-        <v>995</v>
+        <v>989</v>
       </c>
       <c r="D213" t="s">
-        <v>996</v>
+        <v>990</v>
       </c>
       <c r="E213" t="s">
-        <v>997</v>
+        <v>991</v>
       </c>
       <c r="F213" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H213">
         <f t="shared" si="15"/>
@@ -11217,22 +11214,22 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>998</v>
+        <v>992</v>
       </c>
       <c r="B214" t="s">
-        <v>999</v>
+        <v>993</v>
       </c>
       <c r="C214" t="s">
-        <v>1000</v>
+        <v>994</v>
       </c>
       <c r="D214" t="s">
-        <v>1001</v>
+        <v>995</v>
       </c>
       <c r="E214" t="s">
-        <v>1002</v>
+        <v>996</v>
       </c>
       <c r="F214" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H214">
         <f t="shared" si="15"/>
@@ -11249,22 +11246,22 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="B215" t="s">
-        <v>1003</v>
+        <v>997</v>
       </c>
       <c r="C215" t="s">
-        <v>1004</v>
+        <v>998</v>
       </c>
       <c r="D215" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="E215" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="F215" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H215">
         <f t="shared" si="15"/>
@@ -11281,22 +11278,22 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="B216" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="C216" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="D216" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="E216" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="F216" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H216">
         <f t="shared" si="15"/>
@@ -11313,22 +11310,22 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="B217" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="C217" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="D217" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
       <c r="E217" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="F217" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H217">
         <f t="shared" si="15"/>
@@ -11345,22 +11342,22 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="B218" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="C218" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
       <c r="D218" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="E218" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="F218" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H218">
         <f t="shared" si="15"/>
@@ -11383,16 +11380,16 @@
         <v>475</v>
       </c>
       <c r="C219" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
       <c r="D219" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
       <c r="E219" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="F219" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H219">
         <f t="shared" si="15"/>
@@ -11409,22 +11406,22 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
       <c r="B220" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="C220" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
       <c r="D220" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
       <c r="E220" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
       <c r="F220" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="H220">
         <f t="shared" si="15"/>
@@ -11441,22 +11438,22 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
       <c r="B221" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
       <c r="C221" t="s">
-        <v>1033</v>
+        <v>1027</v>
       </c>
       <c r="D221" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="E221" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="F221" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H221">
         <f t="shared" si="15"/>
@@ -11476,19 +11473,19 @@
         <v>14</v>
       </c>
       <c r="B222" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
       <c r="C222" t="s">
-        <v>1037</v>
+        <v>1031</v>
       </c>
       <c r="D222" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="E222" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="F222" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="H222">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
Reduce share size and words corrections
</commit_message>
<xml_diff>
--- a/code/shabdakala/resource/sbwords.xlsx
+++ b/code/shabdakala/resource/sbwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/shabdak_github/sbbd/shabdakala/code/shabdakala/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842A0073-2CA2-FD4D-9C42-11B47A289C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3499A6A4-2688-7741-AFA2-D63617950E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9F74AEE5-EB85-4044-AC84-8761A591B5C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="1048">
   <si>
     <t>word0</t>
   </si>
@@ -1700,18 +1700,12 @@
     <t>तरस</t>
   </si>
   <si>
-    <t>आफ्रिकेतले प्राणी</t>
-  </si>
-  <si>
     <t>मगर</t>
   </si>
   <si>
     <t>कासव</t>
   </si>
   <si>
-    <t>हिप्पो</t>
-  </si>
-  <si>
     <t>बेडूक</t>
   </si>
   <si>
@@ -1802,9 +1796,6 @@
     <t>दिवाळी</t>
   </si>
   <si>
-    <t>चातुर्दशी</t>
-  </si>
-  <si>
     <t>बिज</t>
   </si>
   <si>
@@ -1814,9 +1805,6 @@
     <t>पूजन</t>
   </si>
   <si>
-    <t>दिवाळीच्या दिवसांचे दुसरे शब्द</t>
-  </si>
-  <si>
     <t>सकाळ</t>
   </si>
   <si>
@@ -1889,9 +1877,6 @@
     <t>उभयचर प्राणी</t>
   </si>
   <si>
-    <t>रामायणातील प्राणी</t>
-  </si>
-  <si>
     <t>खोडी</t>
   </si>
   <si>
@@ -2243,9 +2228,6 @@
     <t>मॅराथॉन</t>
   </si>
   <si>
-    <t>26 (post this after Jan 1 !!)</t>
-  </si>
-  <si>
     <t>ॲटलास</t>
   </si>
   <si>
@@ -2375,9 +2357,6 @@
     <t>बांधवगड</t>
   </si>
   <si>
-    <t>काॅर्बेट</t>
-  </si>
-  <si>
     <t>पेरियार</t>
   </si>
   <si>
@@ -3165,6 +3144,39 @@
   </si>
   <si>
     <t>टायटन</t>
+  </si>
+  <si>
+    <t>गिधाड</t>
+  </si>
+  <si>
+    <t>रामायणात उल्लेख असलेले  प्राणी</t>
+  </si>
+  <si>
+    <t>पाणघोडा</t>
+  </si>
+  <si>
+    <t>आफ्रिकेत आढळणारे प्राणी</t>
+  </si>
+  <si>
+    <t>केदार</t>
+  </si>
+  <si>
+    <t>मासळी</t>
+  </si>
+  <si>
+    <t>चतुर्दशी</t>
+  </si>
+  <si>
+    <t>दिवाळीच्या दिवसांचे दुसरे शब्द प्रत्यय</t>
+  </si>
+  <si>
+    <t xml:space="preserve">संख्या लपलेले शब्द  </t>
+  </si>
+  <si>
+    <t>कॉर्बेट</t>
+  </si>
+  <si>
+    <t xml:space="preserve">२६ (सव्वीस)  - चित्रपट, वर्ष, मैल वगैरे </t>
   </si>
 </sst>
 </file>
@@ -4091,15 +4103,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1707B-2FB7-B84C-9F84-E9F074F3056C}">
   <dimension ref="A1:L222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
@@ -4180,7 +4192,7 @@
       </c>
       <c r="L2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45653</v>
+        <v>45662</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -4975,7 +4987,7 @@
         <v>369</v>
       </c>
       <c r="F25" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>185</v>
@@ -5080,7 +5092,7 @@
         <v>425</v>
       </c>
       <c r="F28" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>431</v>
@@ -5220,7 +5232,7 @@
         <v>503</v>
       </c>
       <c r="F32" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H32">
         <f t="shared" si="7"/>
@@ -5243,7 +5255,7 @@
         <v>370</v>
       </c>
       <c r="C33" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D33" t="s">
         <v>228</v>
@@ -5252,7 +5264,7 @@
         <v>505</v>
       </c>
       <c r="F33" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H33">
         <f t="shared" si="7"/>
@@ -5272,10 +5284,10 @@
         <v>506</v>
       </c>
       <c r="B34" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="C34" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D34" t="s">
         <v>48</v>
@@ -5284,7 +5296,7 @@
         <v>507</v>
       </c>
       <c r="F34" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H34">
         <f t="shared" si="7"/>
@@ -5348,7 +5360,7 @@
         <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>338</v>
@@ -5383,7 +5395,7 @@
         <v>111</v>
       </c>
       <c r="E37" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>85</v>
@@ -5406,13 +5418,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="B38" t="s">
         <v>496</v>
       </c>
       <c r="C38" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D38" t="s">
         <v>497</v>
@@ -5421,7 +5433,7 @@
         <v>498</v>
       </c>
       <c r="F38" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H38">
         <f t="shared" si="7"/>
@@ -5450,10 +5462,10 @@
         <v>510</v>
       </c>
       <c r="E39" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="F39" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H39">
         <f t="shared" si="7"/>
@@ -5540,22 +5552,22 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>565</v>
+      </c>
+      <c r="B42" t="s">
+        <v>566</v>
+      </c>
+      <c r="C42" t="s">
+        <v>619</v>
+      </c>
+      <c r="D42" t="s">
         <v>567</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E42" t="s">
         <v>568</v>
       </c>
-      <c r="C42" t="s">
-        <v>624</v>
-      </c>
-      <c r="D42" t="s">
-        <v>569</v>
-      </c>
-      <c r="E42" t="s">
-        <v>570</v>
-      </c>
       <c r="F42" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H42">
         <f t="shared" si="7"/>
@@ -5572,22 +5584,22 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>577</v>
+      </c>
+      <c r="B43" t="s">
+        <v>578</v>
+      </c>
+      <c r="C43" t="s">
         <v>579</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>580</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
         <v>581</v>
       </c>
-      <c r="D43" t="s">
-        <v>582</v>
-      </c>
-      <c r="E43" t="s">
-        <v>583</v>
-      </c>
       <c r="F43" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H43">
         <f t="shared" si="7"/>
@@ -5619,7 +5631,7 @@
         <v>377</v>
       </c>
       <c r="F44" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>275</v>
@@ -5683,13 +5695,13 @@
         <v>517</v>
       </c>
       <c r="D46" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="E46" t="s">
         <v>518</v>
       </c>
       <c r="F46" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H46">
         <f t="shared" si="7"/>
@@ -5721,7 +5733,7 @@
         <v>522</v>
       </c>
       <c r="F47" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H47">
         <f t="shared" si="7"/>
@@ -5753,7 +5765,7 @@
         <v>527</v>
       </c>
       <c r="F48" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H48">
         <f t="shared" si="7"/>
@@ -5820,7 +5832,7 @@
         <v>415</v>
       </c>
       <c r="F50" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>275</v>
@@ -5846,7 +5858,7 @@
         <v>120</v>
       </c>
       <c r="C51" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="D51" t="s">
         <v>121</v>
@@ -5875,7 +5887,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="B52" t="s">
         <v>36</v>
@@ -5948,7 +5960,7 @@
         <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="C54" t="s">
         <v>213</v>
@@ -5995,7 +6007,7 @@
         <v>432</v>
       </c>
       <c r="F55" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>275</v>
@@ -6018,19 +6030,19 @@
         <v>233</v>
       </c>
       <c r="B56" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="C56" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D56" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E56" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="F56" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H56">
         <f t="shared" si="7"/>
@@ -6053,7 +6065,7 @@
         <v>232</v>
       </c>
       <c r="C57" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D57" t="s">
         <v>234</v>
@@ -6082,19 +6094,19 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="B58" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="C58" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="D58" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="E58" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="F58" t="s">
         <v>443</v>
@@ -6126,10 +6138,10 @@
         <v>466</v>
       </c>
       <c r="E59" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="F59" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H59">
         <f t="shared" si="7"/>
@@ -6146,22 +6158,22 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="B60" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="C60" t="s">
         <v>467</v>
       </c>
       <c r="D60" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="E60" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="F60" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H60">
         <f t="shared" ref="H60:H123" si="9">INT(J60/3)</f>
@@ -6178,7 +6190,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="B61" t="s">
         <v>468</v>
@@ -6193,7 +6205,7 @@
         <v>471</v>
       </c>
       <c r="F61" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H61">
         <f t="shared" si="9"/>
@@ -6210,22 +6222,22 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1014</v>
+        <v>1007</v>
       </c>
       <c r="B62" t="s">
-        <v>1015</v>
+        <v>1008</v>
       </c>
       <c r="C62" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="D62" t="s">
-        <v>1016</v>
+        <v>1009</v>
       </c>
       <c r="E62" t="s">
         <v>497</v>
       </c>
       <c r="F62" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H62">
         <f t="shared" si="9"/>
@@ -6242,19 +6254,19 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B63" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="C63" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="D63" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="E63" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>443</v>
@@ -6290,7 +6302,7 @@
         <v>374</v>
       </c>
       <c r="F64" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>275</v>
@@ -6430,7 +6442,7 @@
         <v>420</v>
       </c>
       <c r="F68" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>275</v>
@@ -6465,7 +6477,7 @@
         <v>407</v>
       </c>
       <c r="F69" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>430</v>
@@ -6497,10 +6509,10 @@
         <v>460</v>
       </c>
       <c r="E70" t="s">
-        <v>1030</v>
+        <v>1023</v>
       </c>
       <c r="F70" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H70">
         <f t="shared" si="9"/>
@@ -6555,19 +6567,19 @@
         <v>213</v>
       </c>
       <c r="B72" t="s">
+        <v>569</v>
+      </c>
+      <c r="C72" t="s">
+        <v>570</v>
+      </c>
+      <c r="D72" t="s">
         <v>571</v>
       </c>
-      <c r="C72" t="s">
-        <v>572</v>
-      </c>
-      <c r="D72" t="s">
-        <v>573</v>
-      </c>
       <c r="E72" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="F72" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H72">
         <f t="shared" si="9"/>
@@ -6584,22 +6596,22 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>572</v>
+      </c>
+      <c r="B73" t="s">
+        <v>573</v>
+      </c>
+      <c r="C73" t="s">
         <v>574</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>575</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" t="s">
         <v>576</v>
       </c>
-      <c r="D73" t="s">
-        <v>577</v>
-      </c>
-      <c r="E73" t="s">
-        <v>578</v>
-      </c>
       <c r="F73" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H73">
         <f t="shared" si="9"/>
@@ -6616,22 +6628,22 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>830</v>
+        <v>823</v>
       </c>
       <c r="B74" t="s">
-        <v>831</v>
+        <v>824</v>
       </c>
       <c r="C74" t="s">
-        <v>832</v>
+        <v>825</v>
       </c>
       <c r="D74" t="s">
-        <v>833</v>
+        <v>826</v>
       </c>
       <c r="E74" t="s">
-        <v>834</v>
+        <v>827</v>
       </c>
       <c r="F74" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H74">
         <f t="shared" si="9"/>
@@ -6663,7 +6675,7 @@
         <v>426</v>
       </c>
       <c r="F75" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G75" s="1" t="s">
         <v>275</v>
@@ -6794,16 +6806,16 @@
         <v>479</v>
       </c>
       <c r="C79" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D79" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E79" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="F79" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H79">
         <f t="shared" si="9"/>
@@ -6829,13 +6841,13 @@
         <v>301</v>
       </c>
       <c r="D80" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="E80" t="s">
         <v>482</v>
       </c>
       <c r="F80" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H80">
         <f t="shared" si="9"/>
@@ -6890,13 +6902,13 @@
         <v>48</v>
       </c>
       <c r="B82" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="C82" t="s">
         <v>282</v>
       </c>
       <c r="D82" t="s">
-        <v>1031</v>
+        <v>1024</v>
       </c>
       <c r="E82" t="s">
         <v>315</v>
@@ -6928,7 +6940,7 @@
         <v>456</v>
       </c>
       <c r="C83" t="s">
-        <v>1033</v>
+        <v>1026</v>
       </c>
       <c r="D83" t="s">
         <v>457</v>
@@ -6937,7 +6949,7 @@
         <v>458</v>
       </c>
       <c r="F83" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H83">
         <f t="shared" si="9"/>
@@ -6954,22 +6966,22 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1036</v>
+        <v>1029</v>
       </c>
       <c r="B84" t="s">
-        <v>1035</v>
+        <v>1028</v>
       </c>
       <c r="C84" t="s">
-        <v>1032</v>
+        <v>1025</v>
       </c>
       <c r="D84" t="s">
-        <v>1034</v>
+        <v>1027</v>
       </c>
       <c r="E84" t="s">
-        <v>1030</v>
+        <v>1023</v>
       </c>
       <c r="F84" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H84">
         <f t="shared" si="9"/>
@@ -7001,7 +7013,7 @@
         <v>390</v>
       </c>
       <c r="F85" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>427</v>
@@ -7065,13 +7077,13 @@
         <v>474</v>
       </c>
       <c r="D87" t="s">
-        <v>1037</v>
+        <v>1030</v>
       </c>
       <c r="E87" t="s">
         <v>475</v>
       </c>
       <c r="F87" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H87">
         <f t="shared" si="9"/>
@@ -7088,22 +7100,22 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1039</v>
+        <v>1032</v>
       </c>
       <c r="B88" t="s">
         <v>476</v>
       </c>
       <c r="C88" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="D88" t="s">
-        <v>1038</v>
+        <v>1031</v>
       </c>
       <c r="E88" t="s">
         <v>477</v>
       </c>
       <c r="F88" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H88">
         <f t="shared" si="9"/>
@@ -7193,19 +7205,19 @@
         <v>483</v>
       </c>
       <c r="B91" t="s">
-        <v>1040</v>
+        <v>1033</v>
       </c>
       <c r="C91" t="s">
         <v>484</v>
       </c>
       <c r="D91" t="s">
-        <v>1041</v>
+        <v>1034</v>
       </c>
       <c r="E91" t="s">
         <v>485</v>
       </c>
       <c r="F91" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H91">
         <f t="shared" si="9"/>
@@ -7237,7 +7249,7 @@
         <v>490</v>
       </c>
       <c r="F92" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H92">
         <f t="shared" si="9"/>
@@ -7269,7 +7281,7 @@
         <v>495</v>
       </c>
       <c r="F93" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H93">
         <f t="shared" si="9"/>
@@ -7391,10 +7403,10 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B97" t="s">
-        <v>1042</v>
+        <v>1035</v>
       </c>
       <c r="C97" t="s">
         <v>535</v>
@@ -7406,7 +7418,7 @@
         <v>162</v>
       </c>
       <c r="F97" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H97">
         <f t="shared" si="9"/>
@@ -7429,16 +7441,16 @@
         <v>516</v>
       </c>
       <c r="C98" t="s">
+        <v>559</v>
+      </c>
+      <c r="D98" t="s">
+        <v>560</v>
+      </c>
+      <c r="E98" t="s">
         <v>561</v>
       </c>
-      <c r="D98" t="s">
-        <v>562</v>
-      </c>
-      <c r="E98" t="s">
-        <v>563</v>
-      </c>
       <c r="F98" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H98">
         <f t="shared" si="9"/>
@@ -7455,22 +7467,22 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B99" t="s">
-        <v>1043</v>
+        <v>1036</v>
       </c>
       <c r="C99" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D99" t="s">
         <v>151</v>
       </c>
       <c r="E99" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F99" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H99">
         <f t="shared" si="9"/>
@@ -7502,7 +7514,7 @@
         <v>396</v>
       </c>
       <c r="F100" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>275</v>
@@ -7607,7 +7619,7 @@
         <v>529</v>
       </c>
       <c r="F103" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H103">
         <f t="shared" si="9"/>
@@ -7639,7 +7651,7 @@
         <v>534</v>
       </c>
       <c r="F104" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H104">
         <f t="shared" si="9"/>
@@ -7671,7 +7683,7 @@
         <v>537</v>
       </c>
       <c r="F105" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H105">
         <f t="shared" si="9"/>
@@ -7703,7 +7715,7 @@
         <v>542</v>
       </c>
       <c r="F106" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H106">
         <f t="shared" si="9"/>
@@ -7735,7 +7747,7 @@
         <v>547</v>
       </c>
       <c r="F107" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H107">
         <f t="shared" si="9"/>
@@ -7892,22 +7904,22 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>590</v>
+      </c>
+      <c r="B112" t="s">
+        <v>591</v>
+      </c>
+      <c r="C112" t="s">
+        <v>592</v>
+      </c>
+      <c r="D112" t="s">
+        <v>593</v>
+      </c>
+      <c r="E112" t="s">
         <v>594</v>
       </c>
-      <c r="B112" t="s">
-        <v>595</v>
-      </c>
-      <c r="C112" t="s">
-        <v>596</v>
-      </c>
-      <c r="D112" t="s">
-        <v>597</v>
-      </c>
-      <c r="E112" t="s">
-        <v>598</v>
-      </c>
       <c r="F112" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H112">
         <f t="shared" si="9"/>
@@ -7939,7 +7951,7 @@
         <v>514</v>
       </c>
       <c r="F113" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H113">
         <f t="shared" si="9"/>
@@ -7956,22 +7968,22 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
+        <v>595</v>
+      </c>
+      <c r="B114" t="s">
+        <v>596</v>
+      </c>
+      <c r="C114" t="s">
+        <v>597</v>
+      </c>
+      <c r="D114" t="s">
+        <v>598</v>
+      </c>
+      <c r="E114" t="s">
         <v>599</v>
       </c>
-      <c r="B114" t="s">
+      <c r="F114" t="s">
         <v>600</v>
-      </c>
-      <c r="C114" t="s">
-        <v>601</v>
-      </c>
-      <c r="D114" t="s">
-        <v>602</v>
-      </c>
-      <c r="E114" t="s">
-        <v>603</v>
-      </c>
-      <c r="F114" t="s">
-        <v>604</v>
       </c>
       <c r="H114">
         <f t="shared" si="9"/>
@@ -8003,7 +8015,7 @@
         <v>423</v>
       </c>
       <c r="F115" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>87</v>
@@ -8029,16 +8041,16 @@
         <v>549</v>
       </c>
       <c r="C116" t="s">
-        <v>411</v>
+        <v>1037</v>
       </c>
       <c r="D116" t="s">
         <v>550</v>
       </c>
       <c r="E116" t="s">
-        <v>618</v>
+        <v>1038</v>
       </c>
       <c r="F116" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H116">
         <f t="shared" si="9"/>
@@ -8067,10 +8079,10 @@
         <v>554</v>
       </c>
       <c r="E117" t="s">
-        <v>555</v>
+        <v>1040</v>
       </c>
       <c r="F117" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H117">
         <f t="shared" si="9"/>
@@ -8087,22 +8099,22 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
+        <v>555</v>
+      </c>
+      <c r="B118" t="s">
         <v>556</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D118" t="s">
         <v>557</v>
       </c>
-      <c r="C118" t="s">
-        <v>558</v>
-      </c>
-      <c r="D118" t="s">
-        <v>559</v>
-      </c>
       <c r="E118" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="F118" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H118">
         <f t="shared" si="9"/>
@@ -8224,22 +8236,22 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
+        <v>582</v>
+      </c>
+      <c r="B122" t="s">
+        <v>583</v>
+      </c>
+      <c r="C122" t="s">
         <v>584</v>
       </c>
-      <c r="B122" t="s">
+      <c r="D122" t="s">
         <v>585</v>
       </c>
-      <c r="C122" t="s">
+      <c r="E122" t="s">
         <v>586</v>
       </c>
-      <c r="D122" t="s">
-        <v>587</v>
-      </c>
-      <c r="E122" t="s">
-        <v>588</v>
-      </c>
       <c r="F122" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H122">
         <f t="shared" si="9"/>
@@ -8291,7 +8303,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>625</v>
+        <v>1041</v>
       </c>
       <c r="B124" t="s">
         <v>424</v>
@@ -8306,7 +8318,7 @@
         <v>429</v>
       </c>
       <c r="F124" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>428</v>
@@ -8370,7 +8382,7 @@
         <v>242</v>
       </c>
       <c r="D126" t="s">
-        <v>243</v>
+        <v>1042</v>
       </c>
       <c r="E126" t="s">
         <v>244</v>
@@ -8396,22 +8408,22 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B127" t="s">
+        <v>587</v>
+      </c>
+      <c r="C127" t="s">
+        <v>588</v>
+      </c>
+      <c r="D127" t="s">
         <v>589</v>
       </c>
-      <c r="B127" t="s">
-        <v>590</v>
-      </c>
-      <c r="C127" t="s">
-        <v>591</v>
-      </c>
-      <c r="D127" t="s">
-        <v>592</v>
-      </c>
       <c r="E127" t="s">
-        <v>593</v>
+        <v>1044</v>
       </c>
       <c r="F127" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H127">
         <f t="shared" si="12"/>
@@ -8743,22 +8755,22 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B137" t="s">
         <v>232</v>
       </c>
       <c r="C137" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D137" t="s">
         <v>231</v>
       </c>
       <c r="E137" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F137" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H137">
         <f t="shared" si="12"/>
@@ -8787,7 +8799,7 @@
         <v>43</v>
       </c>
       <c r="E138" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>338</v>
@@ -8810,22 +8822,22 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="B139" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="C139" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="D139" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="E139" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
       <c r="F139" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="G139" s="1"/>
       <c r="H139">
@@ -8843,22 +8855,22 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="B140" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="C140" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="D140" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="E140" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="F140" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H140">
         <f t="shared" si="12"/>
@@ -8875,22 +8887,22 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="B141" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="C141" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="D141" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="E141" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="F141" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H141">
         <f t="shared" si="12"/>
@@ -8907,22 +8919,22 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="B142" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
       <c r="C142" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
       <c r="D142" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
       <c r="E142" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="F142" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H142">
         <f t="shared" si="12"/>
@@ -8939,22 +8951,22 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
       <c r="B143" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
       <c r="C143" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="D143" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="E143" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="F143" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H143">
         <f t="shared" si="12"/>
@@ -8971,22 +8983,22 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="B144" t="s">
         <v>228</v>
       </c>
       <c r="C144" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="D144" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
       <c r="E144" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="F144" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H144">
         <f t="shared" si="12"/>
@@ -9003,22 +9015,22 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="B145" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="C145" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="D145" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="E145" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="F145" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H145">
         <f t="shared" si="12"/>
@@ -9035,22 +9047,22 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="B146" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="C146" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="D146" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="E146" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="F146" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H146">
         <f t="shared" si="12"/>
@@ -9067,22 +9079,22 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="B147" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="C147" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="D147" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
       <c r="E147" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="F147" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H147">
         <f t="shared" si="12"/>
@@ -9099,22 +9111,22 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="B148" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="C148" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="D148" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="E148" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="F148" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H148">
         <f t="shared" si="12"/>
@@ -9131,22 +9143,22 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="B149" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="C149" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="D149" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="E149" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="F149" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H149">
         <f t="shared" si="12"/>
@@ -9163,22 +9175,22 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="B150" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="C150" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="D150" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="E150" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="F150" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H150">
         <f t="shared" si="12"/>
@@ -9195,22 +9207,22 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="B151" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="C151" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="D151" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="E151" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="F151" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H151">
         <f t="shared" si="12"/>
@@ -9227,22 +9239,22 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="B152" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="C152" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="D152" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="E152" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="F152" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H152">
         <f t="shared" si="12"/>
@@ -9259,22 +9271,22 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="B153" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="C153" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="D153" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="E153" t="s">
         <v>246</v>
       </c>
       <c r="F153" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H153">
         <f t="shared" si="12"/>
@@ -9291,22 +9303,22 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="B154" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="C154" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D154" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="E154" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="F154" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H154">
         <f t="shared" si="12"/>
@@ -9323,22 +9335,22 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="B155" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="C155" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="D155" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="E155" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="F155" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H155">
         <f t="shared" si="12"/>
@@ -9355,22 +9367,22 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="B156" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="C156" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="D156" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="E156" t="s">
-        <v>736</v>
+        <v>1047</v>
       </c>
       <c r="F156" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H156">
         <f t="shared" si="12"/>
@@ -9387,22 +9399,22 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="B157" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="C157" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="D157" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="E157" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="F157" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H157">
         <f t="shared" si="12"/>
@@ -9419,22 +9431,22 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="B158" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="C158" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="D158" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="E158" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="F158" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H158">
         <f t="shared" si="12"/>
@@ -9451,22 +9463,22 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="B159" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="C159" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="D159" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="E159" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="F159" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H159">
         <f t="shared" si="12"/>
@@ -9483,22 +9495,22 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="B160" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="C160" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="D160" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="E160" t="s">
-        <v>755</v>
+        <v>749</v>
       </c>
       <c r="F160" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H160">
         <f t="shared" si="12"/>
@@ -9515,22 +9527,22 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B161" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="C161" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="D161" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="E161" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="F161" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H161">
         <f t="shared" si="12"/>
@@ -9547,22 +9559,22 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="B162" t="s">
-        <v>762</v>
+        <v>756</v>
       </c>
       <c r="C162" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="D162" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
       <c r="E162" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="F162" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H162">
         <f t="shared" si="12"/>
@@ -9579,22 +9591,22 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
       <c r="B163" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="C163" t="s">
         <v>291</v>
       </c>
       <c r="D163" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
       <c r="E163" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="F163" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H163">
         <f t="shared" si="12"/>
@@ -9611,22 +9623,22 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="B164" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="C164" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="D164" t="s">
-        <v>754</v>
+        <v>748</v>
       </c>
       <c r="E164" t="s">
-        <v>755</v>
+        <v>1045</v>
       </c>
       <c r="F164" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H164">
         <f t="shared" si="12"/>
@@ -9643,22 +9655,22 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
       <c r="B165" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="C165" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="D165" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
       <c r="E165" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="F165" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H165">
         <f t="shared" si="12"/>
@@ -9678,19 +9690,19 @@
         <v>536</v>
       </c>
       <c r="B166" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
       <c r="C166" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
       <c r="D166" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
       <c r="E166" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
       <c r="F166" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H166">
         <f t="shared" si="12"/>
@@ -9707,22 +9719,22 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
       <c r="B167" t="s">
-        <v>780</v>
+        <v>1046</v>
       </c>
       <c r="C167" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
       <c r="D167" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
       <c r="E167" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="F167" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H167">
         <f t="shared" si="12"/>
@@ -9739,22 +9751,22 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="B168" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="C168" t="s">
-        <v>786</v>
+        <v>779</v>
       </c>
       <c r="D168" t="s">
-        <v>787</v>
+        <v>780</v>
       </c>
       <c r="E168" t="s">
-        <v>788</v>
+        <v>781</v>
       </c>
       <c r="F168" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H168">
         <f t="shared" si="12"/>
@@ -9771,22 +9783,22 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>789</v>
+        <v>782</v>
       </c>
       <c r="B169" t="s">
         <v>512</v>
       </c>
       <c r="C169" t="s">
-        <v>790</v>
+        <v>783</v>
       </c>
       <c r="D169" t="s">
-        <v>791</v>
+        <v>784</v>
       </c>
       <c r="E169" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="F169" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H169">
         <f t="shared" si="12"/>
@@ -9803,22 +9815,22 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>793</v>
+        <v>786</v>
       </c>
       <c r="B170" t="s">
-        <v>794</v>
+        <v>787</v>
       </c>
       <c r="C170" t="s">
-        <v>795</v>
+        <v>788</v>
       </c>
       <c r="D170" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="E170" t="s">
-        <v>797</v>
+        <v>790</v>
       </c>
       <c r="F170" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H170">
         <f t="shared" si="12"/>
@@ -9835,22 +9847,22 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>798</v>
+        <v>791</v>
       </c>
       <c r="B171" t="s">
-        <v>799</v>
+        <v>792</v>
       </c>
       <c r="C171" t="s">
-        <v>800</v>
+        <v>793</v>
       </c>
       <c r="D171" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
       <c r="E171" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="F171" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H171">
         <f t="shared" si="12"/>
@@ -9870,19 +9882,19 @@
         <v>403</v>
       </c>
       <c r="B172" t="s">
-        <v>803</v>
+        <v>796</v>
       </c>
       <c r="C172" t="s">
-        <v>804</v>
+        <v>797</v>
       </c>
       <c r="D172" t="s">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="E172" t="s">
         <v>103</v>
       </c>
       <c r="F172" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H172">
         <f t="shared" si="12"/>
@@ -9899,22 +9911,22 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>806</v>
+        <v>799</v>
       </c>
       <c r="B173" t="s">
-        <v>807</v>
+        <v>800</v>
       </c>
       <c r="C173" t="s">
-        <v>808</v>
+        <v>801</v>
       </c>
       <c r="D173" t="s">
-        <v>809</v>
+        <v>802</v>
       </c>
       <c r="E173" t="s">
-        <v>810</v>
+        <v>803</v>
       </c>
       <c r="F173" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H173">
         <f t="shared" si="12"/>
@@ -9931,22 +9943,22 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>811</v>
+        <v>804</v>
       </c>
       <c r="B174" t="s">
-        <v>812</v>
+        <v>805</v>
       </c>
       <c r="C174" t="s">
-        <v>813</v>
+        <v>806</v>
       </c>
       <c r="D174" t="s">
-        <v>814</v>
+        <v>807</v>
       </c>
       <c r="E174" t="s">
-        <v>815</v>
+        <v>808</v>
       </c>
       <c r="F174" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H174">
         <f t="shared" si="12"/>
@@ -9963,22 +9975,22 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>816</v>
+        <v>809</v>
       </c>
       <c r="B175" t="s">
-        <v>817</v>
+        <v>810</v>
       </c>
       <c r="C175" t="s">
-        <v>818</v>
+        <v>811</v>
       </c>
       <c r="D175" t="s">
-        <v>819</v>
+        <v>812</v>
       </c>
       <c r="E175" t="s">
-        <v>820</v>
+        <v>813</v>
       </c>
       <c r="F175" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H175">
         <f t="shared" si="12"/>
@@ -9995,22 +10007,22 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>821</v>
+        <v>814</v>
       </c>
       <c r="B176" t="s">
         <v>299</v>
       </c>
       <c r="C176" t="s">
-        <v>822</v>
+        <v>815</v>
       </c>
       <c r="D176" t="s">
-        <v>823</v>
+        <v>816</v>
       </c>
       <c r="E176" t="s">
-        <v>824</v>
+        <v>817</v>
       </c>
       <c r="F176" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H176">
         <f t="shared" si="12"/>
@@ -10027,22 +10039,22 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>825</v>
+        <v>818</v>
       </c>
       <c r="B177" t="s">
-        <v>826</v>
+        <v>819</v>
       </c>
       <c r="C177" t="s">
-        <v>827</v>
+        <v>820</v>
       </c>
       <c r="D177" t="s">
-        <v>828</v>
+        <v>821</v>
       </c>
       <c r="E177" t="s">
-        <v>829</v>
+        <v>822</v>
       </c>
       <c r="F177" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H177">
         <f t="shared" si="12"/>
@@ -10059,22 +10071,22 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>835</v>
+        <v>828</v>
       </c>
       <c r="B178" t="s">
         <v>516</v>
       </c>
       <c r="C178" t="s">
-        <v>836</v>
+        <v>829</v>
       </c>
       <c r="D178" t="s">
-        <v>837</v>
+        <v>830</v>
       </c>
       <c r="E178" t="s">
-        <v>838</v>
+        <v>831</v>
       </c>
       <c r="F178" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H178">
         <f t="shared" si="12"/>
@@ -10091,22 +10103,22 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>839</v>
+        <v>832</v>
       </c>
       <c r="B179" t="s">
-        <v>840</v>
+        <v>833</v>
       </c>
       <c r="C179" t="s">
-        <v>841</v>
+        <v>834</v>
       </c>
       <c r="D179" t="s">
-        <v>842</v>
+        <v>835</v>
       </c>
       <c r="E179" t="s">
-        <v>843</v>
+        <v>836</v>
       </c>
       <c r="F179" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H179">
         <f t="shared" si="12"/>
@@ -10123,22 +10135,22 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>844</v>
+        <v>837</v>
       </c>
       <c r="B180" t="s">
-        <v>845</v>
+        <v>838</v>
       </c>
       <c r="C180" t="s">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="D180" t="s">
-        <v>847</v>
+        <v>840</v>
       </c>
       <c r="E180" t="s">
-        <v>848</v>
+        <v>841</v>
       </c>
       <c r="F180" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H180">
         <f t="shared" si="12"/>
@@ -10155,22 +10167,22 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>849</v>
+        <v>842</v>
       </c>
       <c r="B181" t="s">
-        <v>850</v>
+        <v>843</v>
       </c>
       <c r="C181" t="s">
-        <v>851</v>
+        <v>844</v>
       </c>
       <c r="D181" t="s">
-        <v>852</v>
+        <v>845</v>
       </c>
       <c r="E181" t="s">
-        <v>853</v>
+        <v>846</v>
       </c>
       <c r="F181" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H181">
         <f t="shared" si="12"/>
@@ -10187,22 +10199,22 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="B182" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="C182" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="D182" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="E182" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="F182" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H182">
         <f t="shared" si="12"/>
@@ -10219,22 +10231,22 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>854</v>
+        <v>847</v>
       </c>
       <c r="B183" t="s">
-        <v>855</v>
+        <v>848</v>
       </c>
       <c r="C183" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="D183" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="E183" t="s">
-        <v>858</v>
+        <v>851</v>
       </c>
       <c r="F183" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H183">
         <f t="shared" si="12"/>
@@ -10251,22 +10263,22 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>859</v>
+        <v>852</v>
       </c>
       <c r="B184" t="s">
-        <v>860</v>
+        <v>853</v>
       </c>
       <c r="C184" t="s">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="D184" t="s">
-        <v>862</v>
+        <v>855</v>
       </c>
       <c r="E184" t="s">
-        <v>863</v>
+        <v>856</v>
       </c>
       <c r="F184" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H184">
         <f t="shared" si="12"/>
@@ -10283,22 +10295,22 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>864</v>
+        <v>857</v>
       </c>
       <c r="B185" t="s">
-        <v>865</v>
+        <v>858</v>
       </c>
       <c r="C185" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="D185" t="s">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="E185" t="s">
-        <v>868</v>
+        <v>861</v>
       </c>
       <c r="F185" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H185">
         <f t="shared" si="12"/>
@@ -10315,22 +10327,22 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>869</v>
+        <v>862</v>
       </c>
       <c r="B186" t="s">
-        <v>870</v>
+        <v>863</v>
       </c>
       <c r="C186" t="s">
-        <v>871</v>
+        <v>864</v>
       </c>
       <c r="D186" t="s">
-        <v>872</v>
+        <v>865</v>
       </c>
       <c r="E186" t="s">
-        <v>873</v>
+        <v>866</v>
       </c>
       <c r="F186" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H186">
         <f t="shared" si="12"/>
@@ -10347,22 +10359,22 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>874</v>
+        <v>867</v>
       </c>
       <c r="B187" t="s">
-        <v>875</v>
+        <v>868</v>
       </c>
       <c r="C187" t="s">
-        <v>876</v>
+        <v>869</v>
       </c>
       <c r="D187" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="E187" t="s">
-        <v>878</v>
+        <v>871</v>
       </c>
       <c r="F187" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H187">
         <f t="shared" si="12"/>
@@ -10379,22 +10391,22 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>879</v>
+        <v>872</v>
       </c>
       <c r="B188" t="s">
-        <v>880</v>
+        <v>873</v>
       </c>
       <c r="C188" t="s">
-        <v>881</v>
+        <v>874</v>
       </c>
       <c r="D188" t="s">
-        <v>882</v>
+        <v>875</v>
       </c>
       <c r="E188" t="s">
-        <v>883</v>
+        <v>876</v>
       </c>
       <c r="F188" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H188">
         <f t="shared" ref="H188:H222" si="15">INT(J188/3)</f>
@@ -10411,22 +10423,22 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>884</v>
+        <v>877</v>
       </c>
       <c r="B189" t="s">
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>885</v>
+        <v>878</v>
       </c>
       <c r="D189" t="s">
-        <v>886</v>
+        <v>879</v>
       </c>
       <c r="E189" t="s">
-        <v>887</v>
+        <v>880</v>
       </c>
       <c r="F189" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H189">
         <f t="shared" si="15"/>
@@ -10443,22 +10455,22 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>888</v>
+        <v>881</v>
       </c>
       <c r="B190" t="s">
-        <v>889</v>
+        <v>882</v>
       </c>
       <c r="C190" t="s">
-        <v>890</v>
+        <v>883</v>
       </c>
       <c r="D190" t="s">
-        <v>891</v>
+        <v>884</v>
       </c>
       <c r="E190" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="F190" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H190">
         <f t="shared" si="15"/>
@@ -10475,22 +10487,22 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="B191" t="s">
-        <v>893</v>
+        <v>886</v>
       </c>
       <c r="C191" t="s">
         <v>543</v>
       </c>
       <c r="D191" t="s">
-        <v>894</v>
+        <v>887</v>
       </c>
       <c r="E191" t="s">
-        <v>895</v>
+        <v>888</v>
       </c>
       <c r="F191" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H191">
         <f t="shared" si="15"/>
@@ -10507,22 +10519,22 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="B192" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="C192" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="D192" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="E192" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="F192" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H192">
         <f t="shared" si="15"/>
@@ -10539,22 +10551,22 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>896</v>
+        <v>889</v>
       </c>
       <c r="B193" t="s">
-        <v>897</v>
+        <v>890</v>
       </c>
       <c r="C193" t="s">
-        <v>898</v>
+        <v>891</v>
       </c>
       <c r="D193" t="s">
-        <v>899</v>
+        <v>892</v>
       </c>
       <c r="E193" t="s">
-        <v>900</v>
+        <v>893</v>
       </c>
       <c r="F193" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H193">
         <f t="shared" si="15"/>
@@ -10571,22 +10583,22 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>901</v>
+        <v>894</v>
       </c>
       <c r="B194" t="s">
-        <v>902</v>
+        <v>895</v>
       </c>
       <c r="C194" t="s">
-        <v>903</v>
+        <v>896</v>
       </c>
       <c r="D194" t="s">
-        <v>904</v>
+        <v>897</v>
       </c>
       <c r="E194" t="s">
-        <v>905</v>
+        <v>898</v>
       </c>
       <c r="F194" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H194">
         <f t="shared" si="15"/>
@@ -10603,22 +10615,22 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>906</v>
+        <v>899</v>
       </c>
       <c r="B195" t="s">
-        <v>892</v>
+        <v>885</v>
       </c>
       <c r="C195" t="s">
-        <v>907</v>
+        <v>900</v>
       </c>
       <c r="D195" t="s">
-        <v>908</v>
+        <v>901</v>
       </c>
       <c r="E195" t="s">
-        <v>909</v>
+        <v>902</v>
       </c>
       <c r="F195" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H195">
         <f t="shared" si="15"/>
@@ -10635,22 +10647,22 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>910</v>
+        <v>903</v>
       </c>
       <c r="B196" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="C196" t="s">
-        <v>912</v>
+        <v>905</v>
       </c>
       <c r="D196" t="s">
-        <v>913</v>
+        <v>906</v>
       </c>
       <c r="E196" t="s">
-        <v>914</v>
+        <v>907</v>
       </c>
       <c r="F196" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H196">
         <f t="shared" si="15"/>
@@ -10667,22 +10679,22 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>915</v>
+        <v>908</v>
       </c>
       <c r="B197" t="s">
-        <v>916</v>
+        <v>909</v>
       </c>
       <c r="C197" t="s">
-        <v>917</v>
+        <v>910</v>
       </c>
       <c r="D197" t="s">
-        <v>918</v>
+        <v>911</v>
       </c>
       <c r="E197" t="s">
-        <v>919</v>
+        <v>912</v>
       </c>
       <c r="F197" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H197">
         <f t="shared" si="15"/>
@@ -10699,22 +10711,22 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>866</v>
+        <v>859</v>
       </c>
       <c r="B198" t="s">
-        <v>920</v>
+        <v>913</v>
       </c>
       <c r="C198" t="s">
-        <v>921</v>
+        <v>914</v>
       </c>
       <c r="D198" t="s">
-        <v>922</v>
+        <v>915</v>
       </c>
       <c r="E198" t="s">
-        <v>923</v>
+        <v>916</v>
       </c>
       <c r="F198" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H198">
         <f t="shared" si="15"/>
@@ -10731,7 +10743,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>809</v>
+        <v>802</v>
       </c>
       <c r="B199" t="s">
         <v>480</v>
@@ -10740,13 +10752,13 @@
         <v>487</v>
       </c>
       <c r="D199" t="s">
-        <v>924</v>
+        <v>917</v>
       </c>
       <c r="E199" t="s">
-        <v>925</v>
+        <v>918</v>
       </c>
       <c r="F199" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H199">
         <f t="shared" si="15"/>
@@ -10763,22 +10775,22 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>926</v>
+        <v>919</v>
       </c>
       <c r="B200" t="s">
-        <v>927</v>
+        <v>920</v>
       </c>
       <c r="C200" t="s">
-        <v>928</v>
+        <v>921</v>
       </c>
       <c r="D200" t="s">
-        <v>929</v>
+        <v>922</v>
       </c>
       <c r="E200" t="s">
-        <v>930</v>
+        <v>923</v>
       </c>
       <c r="F200" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H200">
         <f t="shared" si="15"/>
@@ -10795,22 +10807,22 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>931</v>
+        <v>924</v>
       </c>
       <c r="B201" t="s">
-        <v>932</v>
+        <v>925</v>
       </c>
       <c r="C201" t="s">
-        <v>933</v>
+        <v>926</v>
       </c>
       <c r="D201" t="s">
-        <v>934</v>
+        <v>927</v>
       </c>
       <c r="E201" t="s">
-        <v>935</v>
+        <v>928</v>
       </c>
       <c r="F201" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H201">
         <f t="shared" si="15"/>
@@ -10827,22 +10839,22 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>936</v>
+        <v>929</v>
       </c>
       <c r="B202" t="s">
-        <v>937</v>
+        <v>930</v>
       </c>
       <c r="C202" t="s">
-        <v>938</v>
+        <v>931</v>
       </c>
       <c r="D202" t="s">
-        <v>939</v>
+        <v>932</v>
       </c>
       <c r="E202" t="s">
-        <v>940</v>
+        <v>933</v>
       </c>
       <c r="F202" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H202">
         <f t="shared" si="15"/>
@@ -10862,19 +10874,19 @@
         <v>370</v>
       </c>
       <c r="B203" t="s">
-        <v>941</v>
+        <v>934</v>
       </c>
       <c r="C203" t="s">
-        <v>942</v>
+        <v>935</v>
       </c>
       <c r="D203" t="s">
-        <v>943</v>
+        <v>936</v>
       </c>
       <c r="E203" t="s">
-        <v>944</v>
+        <v>937</v>
       </c>
       <c r="F203" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H203">
         <f t="shared" si="15"/>
@@ -10891,22 +10903,22 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>945</v>
+        <v>938</v>
       </c>
       <c r="B204" t="s">
-        <v>946</v>
+        <v>939</v>
       </c>
       <c r="C204" t="s">
-        <v>947</v>
+        <v>940</v>
       </c>
       <c r="D204" t="s">
-        <v>948</v>
+        <v>941</v>
       </c>
       <c r="E204" t="s">
-        <v>949</v>
+        <v>942</v>
       </c>
       <c r="F204" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H204">
         <f t="shared" si="15"/>
@@ -10923,22 +10935,22 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>950</v>
+        <v>943</v>
       </c>
       <c r="B205" t="s">
-        <v>951</v>
+        <v>944</v>
       </c>
       <c r="C205" t="s">
-        <v>952</v>
+        <v>945</v>
       </c>
       <c r="D205" t="s">
-        <v>953</v>
+        <v>946</v>
       </c>
       <c r="E205" t="s">
-        <v>954</v>
+        <v>947</v>
       </c>
       <c r="F205" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H205">
         <f t="shared" si="15"/>
@@ -10955,22 +10967,22 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>955</v>
+        <v>948</v>
       </c>
       <c r="B206" t="s">
-        <v>912</v>
+        <v>905</v>
       </c>
       <c r="C206" t="s">
-        <v>956</v>
+        <v>949</v>
       </c>
       <c r="D206" t="s">
-        <v>957</v>
+        <v>950</v>
       </c>
       <c r="E206" t="s">
-        <v>958</v>
+        <v>951</v>
       </c>
       <c r="F206" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H206">
         <f t="shared" si="15"/>
@@ -10987,22 +10999,22 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>959</v>
+        <v>952</v>
       </c>
       <c r="B207" t="s">
-        <v>960</v>
+        <v>953</v>
       </c>
       <c r="C207" t="s">
         <v>391</v>
       </c>
       <c r="D207" t="s">
-        <v>961</v>
+        <v>954</v>
       </c>
       <c r="E207" t="s">
-        <v>962</v>
+        <v>955</v>
       </c>
       <c r="F207" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H207">
         <f t="shared" si="15"/>
@@ -11019,22 +11031,22 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>963</v>
+        <v>956</v>
       </c>
       <c r="B208" t="s">
-        <v>964</v>
+        <v>957</v>
       </c>
       <c r="C208" t="s">
-        <v>965</v>
+        <v>958</v>
       </c>
       <c r="D208" t="s">
-        <v>966</v>
+        <v>959</v>
       </c>
       <c r="E208" t="s">
-        <v>967</v>
+        <v>960</v>
       </c>
       <c r="F208" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H208">
         <f t="shared" si="15"/>
@@ -11051,22 +11063,22 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="B209" t="s">
-        <v>968</v>
+        <v>961</v>
       </c>
       <c r="C209" t="s">
-        <v>969</v>
+        <v>962</v>
       </c>
       <c r="D209" t="s">
-        <v>970</v>
+        <v>963</v>
       </c>
       <c r="E209" t="s">
-        <v>971</v>
+        <v>964</v>
       </c>
       <c r="F209" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H209">
         <f t="shared" si="15"/>
@@ -11083,22 +11095,22 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>972</v>
+        <v>965</v>
       </c>
       <c r="B210" t="s">
-        <v>973</v>
+        <v>966</v>
       </c>
       <c r="C210" t="s">
-        <v>974</v>
+        <v>967</v>
       </c>
       <c r="D210" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="E210" t="s">
-        <v>975</v>
+        <v>968</v>
       </c>
       <c r="F210" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H210">
         <f t="shared" si="15"/>
@@ -11115,22 +11127,22 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>976</v>
+        <v>969</v>
       </c>
       <c r="B211" t="s">
-        <v>977</v>
+        <v>970</v>
       </c>
       <c r="C211" t="s">
-        <v>978</v>
+        <v>971</v>
       </c>
       <c r="D211" t="s">
         <v>455</v>
       </c>
       <c r="E211" t="s">
-        <v>979</v>
+        <v>972</v>
       </c>
       <c r="F211" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H211">
         <f t="shared" si="15"/>
@@ -11147,22 +11159,22 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>980</v>
+        <v>973</v>
       </c>
       <c r="B212" t="s">
         <v>78</v>
       </c>
       <c r="C212" t="s">
-        <v>981</v>
+        <v>974</v>
       </c>
       <c r="D212" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
       <c r="E212" t="s">
-        <v>983</v>
+        <v>976</v>
       </c>
       <c r="F212" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H212">
         <f t="shared" si="15"/>
@@ -11179,22 +11191,22 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>984</v>
+        <v>977</v>
       </c>
       <c r="B213" t="s">
-        <v>985</v>
+        <v>978</v>
       </c>
       <c r="C213" t="s">
-        <v>986</v>
+        <v>979</v>
       </c>
       <c r="D213" t="s">
-        <v>987</v>
+        <v>980</v>
       </c>
       <c r="E213" t="s">
-        <v>988</v>
+        <v>981</v>
       </c>
       <c r="F213" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H213">
         <f t="shared" si="15"/>
@@ -11211,22 +11223,22 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>989</v>
+        <v>982</v>
       </c>
       <c r="B214" t="s">
-        <v>990</v>
+        <v>983</v>
       </c>
       <c r="C214" t="s">
-        <v>991</v>
+        <v>984</v>
       </c>
       <c r="D214" t="s">
-        <v>992</v>
+        <v>985</v>
       </c>
       <c r="E214" t="s">
-        <v>993</v>
+        <v>986</v>
       </c>
       <c r="F214" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H214">
         <f t="shared" si="15"/>
@@ -11246,19 +11258,19 @@
         <v>548</v>
       </c>
       <c r="B215" t="s">
-        <v>994</v>
+        <v>987</v>
       </c>
       <c r="C215" t="s">
-        <v>995</v>
+        <v>988</v>
       </c>
       <c r="D215" t="s">
-        <v>996</v>
+        <v>989</v>
       </c>
       <c r="E215" t="s">
-        <v>997</v>
+        <v>990</v>
       </c>
       <c r="F215" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H215">
         <f t="shared" si="15"/>
@@ -11275,22 +11287,22 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>998</v>
+        <v>991</v>
       </c>
       <c r="B216" t="s">
-        <v>999</v>
+        <v>992</v>
       </c>
       <c r="C216" t="s">
-        <v>1000</v>
+        <v>993</v>
       </c>
       <c r="D216" t="s">
-        <v>1001</v>
+        <v>994</v>
       </c>
       <c r="E216" t="s">
-        <v>1002</v>
+        <v>995</v>
       </c>
       <c r="F216" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H216">
         <f t="shared" si="15"/>
@@ -11307,22 +11319,22 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>1003</v>
+        <v>996</v>
       </c>
       <c r="B217" t="s">
-        <v>1004</v>
+        <v>997</v>
       </c>
       <c r="C217" t="s">
-        <v>943</v>
+        <v>936</v>
       </c>
       <c r="D217" t="s">
-        <v>1005</v>
+        <v>998</v>
       </c>
       <c r="E217" t="s">
-        <v>1006</v>
+        <v>999</v>
       </c>
       <c r="F217" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H217">
         <f t="shared" si="15"/>
@@ -11339,22 +11351,22 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="B218" t="s">
-        <v>1007</v>
+        <v>1000</v>
       </c>
       <c r="C218" t="s">
-        <v>1008</v>
+        <v>1001</v>
       </c>
       <c r="D218" t="s">
-        <v>1009</v>
+        <v>1002</v>
       </c>
       <c r="E218" t="s">
-        <v>1010</v>
+        <v>1003</v>
       </c>
       <c r="F218" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H218">
         <f t="shared" si="15"/>
@@ -11377,16 +11389,16 @@
         <v>474</v>
       </c>
       <c r="C219" t="s">
-        <v>1011</v>
+        <v>1004</v>
       </c>
       <c r="D219" t="s">
-        <v>1012</v>
+        <v>1005</v>
       </c>
       <c r="E219" t="s">
-        <v>1013</v>
+        <v>1006</v>
       </c>
       <c r="F219" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H219">
         <f t="shared" si="15"/>
@@ -11403,22 +11415,22 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>1017</v>
+        <v>1010</v>
       </c>
       <c r="B220" t="s">
-        <v>1018</v>
+        <v>1011</v>
       </c>
       <c r="C220" t="s">
-        <v>1019</v>
+        <v>1012</v>
       </c>
       <c r="D220" t="s">
-        <v>1020</v>
+        <v>1013</v>
       </c>
       <c r="E220" t="s">
-        <v>1021</v>
+        <v>1014</v>
       </c>
       <c r="F220" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="H220">
         <f t="shared" si="15"/>
@@ -11435,22 +11447,22 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>1022</v>
+        <v>1015</v>
       </c>
       <c r="B221" t="s">
-        <v>1023</v>
+        <v>1016</v>
       </c>
       <c r="C221" t="s">
-        <v>1024</v>
+        <v>1017</v>
       </c>
       <c r="D221" t="s">
-        <v>1025</v>
+        <v>1018</v>
       </c>
       <c r="E221" t="s">
-        <v>1026</v>
+        <v>1019</v>
       </c>
       <c r="F221" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H221">
         <f t="shared" si="15"/>
@@ -11470,19 +11482,19 @@
         <v>14</v>
       </c>
       <c r="B222" t="s">
-        <v>1027</v>
+        <v>1020</v>
       </c>
       <c r="C222" t="s">
-        <v>1028</v>
+        <v>1021</v>
       </c>
       <c r="D222" t="s">
-        <v>1029</v>
+        <v>1022</v>
       </c>
       <c r="E222" t="s">
-        <v>805</v>
+        <v>798</v>
       </c>
       <c r="F222" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="H222">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
Words change and beautification
</commit_message>
<xml_diff>
--- a/code/shabdakala/resource/sbwords.xlsx
+++ b/code/shabdakala/resource/sbwords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishinene/shabdak_github/sbbd/shabdakala/code/shabdakala/resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A02FFC8-7902-B641-88C4-0305D3BAD410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC6C803-E0AA-064D-BE6F-5BFC83609483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{9F74AEE5-EB85-4044-AC84-8761A591B5C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2666" uniqueCount="2005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2666" uniqueCount="2003">
   <si>
     <t>word0</t>
   </si>
@@ -4226,24 +4226,12 @@
     <t>बाॅन्ड</t>
   </si>
   <si>
-    <t>ओरिजिन</t>
-  </si>
-  <si>
-    <t>सेंच्युरी</t>
-  </si>
-  <si>
-    <t xml:space="preserve">शून्य शून्य </t>
-  </si>
-  <si>
     <t>बाॅयलर</t>
   </si>
   <si>
     <t>कट</t>
   </si>
   <si>
-    <t>रॅप</t>
-  </si>
-  <si>
     <t>टेक</t>
   </si>
   <si>
@@ -4280,51 +4268,6 @@
     <t>भारतीय उत्पत्तीचे इंग्लिश शब्द</t>
   </si>
   <si>
-    <t xml:space="preserve">ब्रेड </t>
-  </si>
-  <si>
-    <t>काठी</t>
-  </si>
-  <si>
-    <t xml:space="preserve">क्रिम </t>
-  </si>
-  <si>
-    <t xml:space="preserve">स्प्रिंग </t>
-  </si>
-  <si>
-    <t>--- रोल</t>
-  </si>
-  <si>
-    <t>युतू</t>
-  </si>
-  <si>
-    <t>प्रग्यान</t>
-  </si>
-  <si>
-    <t>बग्गी</t>
-  </si>
-  <si>
-    <t>लुनोखोड</t>
-  </si>
-  <si>
-    <t>चंद्रावर चालवलेल्या वहान/रोव्हर्र ची नावे</t>
-  </si>
-  <si>
-    <t>मरिया</t>
-  </si>
-  <si>
-    <t>कटेना</t>
-  </si>
-  <si>
-    <t>व्हालिस</t>
-  </si>
-  <si>
-    <t>माॅन्स</t>
-  </si>
-  <si>
-    <t>चंद्रावरची भौगोलिक वैशिष्ट्ये</t>
-  </si>
-  <si>
     <t>प्राण</t>
   </si>
   <si>
@@ -6048,6 +5991,57 @@
   </si>
   <si>
     <t xml:space="preserve">ऑक्सिजन (O2) </t>
+  </si>
+  <si>
+    <t>जेम्स बॉण्ड</t>
+  </si>
+  <si>
+    <t>शतक</t>
+  </si>
+  <si>
+    <t>मूळ बिंदू (origin)</t>
+  </si>
+  <si>
+    <t>शून्य शून्य (दोन शून्यांचा समावेश)</t>
+  </si>
+  <si>
+    <t>पॅक उप</t>
+  </si>
+  <si>
+    <t>पेज</t>
+  </si>
+  <si>
+    <t>खड्ग</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- पूर नावाची भारतातील प्रसिद्ध गावे </t>
+  </si>
+  <si>
+    <t>इन्दु</t>
+  </si>
+  <si>
+    <t>मृगांक</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> सुधांशु</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> सोम</t>
+  </si>
+  <si>
+    <t xml:space="preserve">चंद्राची काही नावे </t>
+  </si>
+  <si>
+    <t>ओहोटी</t>
+  </si>
+  <si>
+    <t>ग्रहण</t>
+  </si>
+  <si>
+    <t>अपोलो</t>
+  </si>
+  <si>
+    <t xml:space="preserve">चंद्र कारणीभूत असणाऱ्या काही गोष्टी  </t>
   </si>
 </sst>
 </file>
@@ -6974,8 +6968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA1707B-2FB7-B84C-9F84-E9F074F3056C}">
   <dimension ref="A1:L429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C279" sqref="C279"/>
+    <sheetView tabSelected="1" topLeftCell="A279" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F302" sqref="F302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7063,7 +7057,7 @@
       </c>
       <c r="L2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45716</v>
+        <v>45720</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -13102,7 +13096,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>1772</v>
+        <v>1753</v>
       </c>
       <c r="B183" t="s">
         <v>833</v>
@@ -13166,7 +13160,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>1774</v>
+        <v>1755</v>
       </c>
       <c r="B185" t="s">
         <v>1047</v>
@@ -13178,7 +13172,7 @@
         <v>1049</v>
       </c>
       <c r="E185" t="s">
-        <v>1775</v>
+        <v>1756</v>
       </c>
       <c r="F185" t="s">
         <v>597</v>
@@ -13210,7 +13204,7 @@
         <v>1053</v>
       </c>
       <c r="E186" t="s">
-        <v>1773</v>
+        <v>1754</v>
       </c>
       <c r="F186" t="s">
         <v>597</v>
@@ -13274,7 +13268,7 @@
         <v>1061</v>
       </c>
       <c r="E188" t="s">
-        <v>1776</v>
+        <v>1757</v>
       </c>
       <c r="F188" t="s">
         <v>597</v>
@@ -13306,7 +13300,7 @@
         <v>1065</v>
       </c>
       <c r="E189" t="s">
-        <v>1777</v>
+        <v>1758</v>
       </c>
       <c r="F189" t="s">
         <v>597</v>
@@ -13338,7 +13332,7 @@
         <v>1069</v>
       </c>
       <c r="E190" t="s">
-        <v>1778</v>
+        <v>1759</v>
       </c>
       <c r="F190" t="s">
         <v>597</v>
@@ -13591,7 +13585,7 @@
         <v>1105</v>
       </c>
       <c r="D198" t="s">
-        <v>1808</v>
+        <v>1789</v>
       </c>
       <c r="E198" t="s">
         <v>1106</v>
@@ -13620,13 +13614,13 @@
         <v>1108</v>
       </c>
       <c r="C199" t="s">
-        <v>1809</v>
+        <v>1790</v>
       </c>
       <c r="D199" t="s">
         <v>1109</v>
       </c>
       <c r="E199" t="s">
-        <v>1810</v>
+        <v>1791</v>
       </c>
       <c r="F199" t="s">
         <v>597</v>
@@ -13722,7 +13716,7 @@
         <v>1121</v>
       </c>
       <c r="E202" t="s">
-        <v>1811</v>
+        <v>1792</v>
       </c>
       <c r="F202" t="s">
         <v>597</v>
@@ -13777,7 +13771,7 @@
         <v>1126</v>
       </c>
       <c r="B204" t="s">
-        <v>1818</v>
+        <v>1799</v>
       </c>
       <c r="C204" t="s">
         <v>778</v>
@@ -13844,10 +13838,10 @@
         <v>1135</v>
       </c>
       <c r="C206" t="s">
-        <v>1812</v>
+        <v>1793</v>
       </c>
       <c r="D206" t="s">
-        <v>1813</v>
+        <v>1794</v>
       </c>
       <c r="E206" t="s">
         <v>1136</v>
@@ -13876,10 +13870,10 @@
         <v>1138</v>
       </c>
       <c r="C207" t="s">
-        <v>1814</v>
+        <v>1795</v>
       </c>
       <c r="D207" t="s">
-        <v>1815</v>
+        <v>1796</v>
       </c>
       <c r="E207" t="s">
         <v>1139</v>
@@ -13902,19 +13896,19 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>1819</v>
+        <v>1800</v>
       </c>
       <c r="B208" t="s">
-        <v>1820</v>
+        <v>1801</v>
       </c>
       <c r="C208" t="s">
         <v>1140</v>
       </c>
       <c r="D208" t="s">
-        <v>1821</v>
+        <v>1802</v>
       </c>
       <c r="E208" t="s">
-        <v>1822</v>
+        <v>1803</v>
       </c>
       <c r="F208" t="s">
         <v>597</v>
@@ -13946,7 +13940,7 @@
         <v>1144</v>
       </c>
       <c r="E209" t="s">
-        <v>1779</v>
+        <v>1760</v>
       </c>
       <c r="F209" t="s">
         <v>597</v>
@@ -14001,13 +13995,13 @@
         <v>1150</v>
       </c>
       <c r="B211" t="s">
-        <v>1781</v>
+        <v>1762</v>
       </c>
       <c r="C211" t="s">
         <v>1151</v>
       </c>
       <c r="D211" t="s">
-        <v>1780</v>
+        <v>1761</v>
       </c>
       <c r="E211" t="s">
         <v>1152</v>
@@ -14138,7 +14132,7 @@
         <v>1170</v>
       </c>
       <c r="E215" t="s">
-        <v>1816</v>
+        <v>1797</v>
       </c>
       <c r="F215" t="s">
         <v>597</v>
@@ -14170,7 +14164,7 @@
         <v>1174</v>
       </c>
       <c r="E216" t="s">
-        <v>1817</v>
+        <v>1798</v>
       </c>
       <c r="F216" t="s">
         <v>597</v>
@@ -14222,7 +14216,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>1823</v>
+        <v>1804</v>
       </c>
       <c r="B218" t="s">
         <v>1179</v>
@@ -14263,7 +14257,7 @@
         <v>32</v>
       </c>
       <c r="D219" t="s">
-        <v>1824</v>
+        <v>1805</v>
       </c>
       <c r="E219" t="s">
         <v>1185</v>
@@ -14286,7 +14280,7 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>1825</v>
+        <v>1806</v>
       </c>
       <c r="B220" t="s">
         <v>1186</v>
@@ -14330,7 +14324,7 @@
         <v>1193</v>
       </c>
       <c r="E221" t="s">
-        <v>1782</v>
+        <v>1763</v>
       </c>
       <c r="F221" t="s">
         <v>597</v>
@@ -14356,10 +14350,10 @@
         <v>1195</v>
       </c>
       <c r="C222" t="s">
-        <v>1785</v>
+        <v>1766</v>
       </c>
       <c r="D222" t="s">
-        <v>1786</v>
+        <v>1767</v>
       </c>
       <c r="E222" t="s">
         <v>1196</v>
@@ -14382,7 +14376,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>1784</v>
+        <v>1765</v>
       </c>
       <c r="B223" t="s">
         <v>1197</v>
@@ -14394,7 +14388,7 @@
         <v>1198</v>
       </c>
       <c r="E223" t="s">
-        <v>1783</v>
+        <v>1764</v>
       </c>
       <c r="F223" t="s">
         <v>597</v>
@@ -14548,7 +14542,7 @@
         <v>1216</v>
       </c>
       <c r="C228" t="s">
-        <v>1826</v>
+        <v>1807</v>
       </c>
       <c r="D228" t="s">
         <v>1217</v>
@@ -14670,13 +14664,13 @@
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>1828</v>
+        <v>1809</v>
       </c>
       <c r="B232" t="s">
         <v>1234</v>
       </c>
       <c r="C232" t="s">
-        <v>1827</v>
+        <v>1808</v>
       </c>
       <c r="D232" t="s">
         <v>438</v>
@@ -14708,7 +14702,7 @@
         <v>1237</v>
       </c>
       <c r="C233" t="s">
-        <v>1829</v>
+        <v>1810</v>
       </c>
       <c r="D233" t="s">
         <v>1238</v>
@@ -14769,13 +14763,13 @@
         <v>1243</v>
       </c>
       <c r="B235" t="s">
-        <v>1832</v>
+        <v>1813</v>
       </c>
       <c r="C235" t="s">
-        <v>1830</v>
+        <v>1811</v>
       </c>
       <c r="D235" t="s">
-        <v>1831</v>
+        <v>1812</v>
       </c>
       <c r="E235" t="s">
         <v>1244</v>
@@ -14798,7 +14792,7 @@
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>1833</v>
+        <v>1814</v>
       </c>
       <c r="B236" t="s">
         <v>1245</v>
@@ -14830,7 +14824,7 @@
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>1834</v>
+        <v>1815</v>
       </c>
       <c r="B237" t="s">
         <v>1249</v>
@@ -14862,7 +14856,7 @@
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>1835</v>
+        <v>1816</v>
       </c>
       <c r="B238" t="s">
         <v>316</v>
@@ -15182,13 +15176,13 @@
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>1836</v>
+        <v>1817</v>
       </c>
       <c r="B248" t="s">
         <v>1296</v>
       </c>
       <c r="C248" t="s">
-        <v>1837</v>
+        <v>1818</v>
       </c>
       <c r="D248" t="s">
         <v>1297</v>
@@ -15214,7 +15208,7 @@
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>1838</v>
+        <v>1819</v>
       </c>
       <c r="B249" t="s">
         <v>1299</v>
@@ -15246,10 +15240,10 @@
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>1839</v>
+        <v>1820</v>
       </c>
       <c r="B250" t="s">
-        <v>1840</v>
+        <v>1821</v>
       </c>
       <c r="C250" t="s">
         <v>1302</v>
@@ -15374,7 +15368,7 @@
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>1841</v>
+        <v>1822</v>
       </c>
       <c r="B254" t="s">
         <v>1320</v>
@@ -15482,7 +15476,7 @@
         <v>1335</v>
       </c>
       <c r="E257" t="s">
-        <v>1844</v>
+        <v>1825</v>
       </c>
       <c r="F257" t="s">
         <v>597</v>
@@ -15508,7 +15502,7 @@
         <v>1337</v>
       </c>
       <c r="C258" t="s">
-        <v>1845</v>
+        <v>1826</v>
       </c>
       <c r="D258" t="s">
         <v>64</v>
@@ -15601,10 +15595,10 @@
         <v>1349</v>
       </c>
       <c r="B261" t="s">
-        <v>1842</v>
+        <v>1823</v>
       </c>
       <c r="C261" t="s">
-        <v>1843</v>
+        <v>1824</v>
       </c>
       <c r="D261" t="s">
         <v>1350</v>
@@ -15662,22 +15656,22 @@
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>1847</v>
+        <v>1828</v>
       </c>
       <c r="B263" t="s">
-        <v>1848</v>
+        <v>1829</v>
       </c>
       <c r="C263" t="s">
         <v>573</v>
       </c>
       <c r="D263" t="s">
-        <v>1849</v>
+        <v>1830</v>
       </c>
       <c r="E263" t="s">
-        <v>1850</v>
+        <v>1831</v>
       </c>
       <c r="F263" t="s">
-        <v>1851</v>
+        <v>1832</v>
       </c>
       <c r="H263">
         <f t="shared" si="25"/>
@@ -15694,22 +15688,22 @@
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>1852</v>
+        <v>1833</v>
       </c>
       <c r="B264" t="s">
-        <v>1522</v>
+        <v>1503</v>
       </c>
       <c r="C264" t="s">
-        <v>1853</v>
+        <v>1834</v>
       </c>
       <c r="D264" t="s">
-        <v>1854</v>
+        <v>1835</v>
       </c>
       <c r="E264" t="s">
-        <v>1855</v>
+        <v>1836</v>
       </c>
       <c r="F264" t="s">
-        <v>1856</v>
+        <v>1837</v>
       </c>
       <c r="H264">
         <f t="shared" si="25"/>
@@ -15726,22 +15720,22 @@
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>1857</v>
+        <v>1838</v>
       </c>
       <c r="B265" t="s">
-        <v>1858</v>
+        <v>1839</v>
       </c>
       <c r="C265" t="s">
-        <v>1859</v>
+        <v>1840</v>
       </c>
       <c r="D265" t="s">
-        <v>1860</v>
+        <v>1841</v>
       </c>
       <c r="E265" t="s">
-        <v>1861</v>
+        <v>1842</v>
       </c>
       <c r="F265" t="s">
-        <v>1862</v>
+        <v>1843</v>
       </c>
       <c r="H265">
         <f t="shared" si="25"/>
@@ -15758,22 +15752,22 @@
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>1867</v>
+        <v>1848</v>
       </c>
       <c r="B266" t="s">
-        <v>1868</v>
+        <v>1849</v>
       </c>
       <c r="C266" t="s">
-        <v>1869</v>
+        <v>1850</v>
       </c>
       <c r="D266" t="s">
-        <v>1870</v>
+        <v>1851</v>
       </c>
       <c r="E266" t="s">
-        <v>1871</v>
+        <v>1852</v>
       </c>
       <c r="F266" t="s">
-        <v>1872</v>
+        <v>1853</v>
       </c>
       <c r="H266">
         <f t="shared" si="25"/>
@@ -15790,22 +15784,22 @@
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>1873</v>
+        <v>1854</v>
       </c>
       <c r="B267" t="s">
-        <v>1874</v>
+        <v>1855</v>
       </c>
       <c r="C267" t="s">
-        <v>1875</v>
+        <v>1856</v>
       </c>
       <c r="D267" t="s">
-        <v>1876</v>
+        <v>1857</v>
       </c>
       <c r="E267" t="s">
-        <v>1877</v>
+        <v>1858</v>
       </c>
       <c r="F267" t="s">
-        <v>1886</v>
+        <v>1867</v>
       </c>
       <c r="H267">
         <f t="shared" si="25"/>
@@ -15834,7 +15828,7 @@
         <v>1360</v>
       </c>
       <c r="E268" t="s">
-        <v>1846</v>
+        <v>1827</v>
       </c>
       <c r="F268" t="s">
         <v>597</v>
@@ -15886,22 +15880,22 @@
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>1919</v>
+        <v>1900</v>
       </c>
       <c r="B270" t="s">
-        <v>1920</v>
+        <v>1901</v>
       </c>
       <c r="C270" t="s">
-        <v>1921</v>
+        <v>1902</v>
       </c>
       <c r="D270" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="E270" t="s">
-        <v>1922</v>
+        <v>1903</v>
       </c>
       <c r="F270" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="H270">
         <f t="shared" si="25"/>
@@ -15918,22 +15912,22 @@
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>1928</v>
+        <v>1909</v>
       </c>
       <c r="B271" t="s">
         <v>71</v>
       </c>
       <c r="C271" t="s">
-        <v>1929</v>
+        <v>1910</v>
       </c>
       <c r="D271" t="s">
-        <v>1930</v>
+        <v>1911</v>
       </c>
       <c r="E271" t="s">
-        <v>1931</v>
+        <v>1912</v>
       </c>
       <c r="F271" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="H271">
         <f t="shared" si="25"/>
@@ -15982,22 +15976,22 @@
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>1902</v>
+        <v>1883</v>
       </c>
       <c r="B273" t="s">
-        <v>1903</v>
+        <v>1884</v>
       </c>
       <c r="C273" t="s">
-        <v>1904</v>
+        <v>1885</v>
       </c>
       <c r="D273" t="s">
-        <v>1905</v>
+        <v>1886</v>
       </c>
       <c r="E273" t="s">
-        <v>1906</v>
+        <v>1887</v>
       </c>
       <c r="F273" t="s">
-        <v>1907</v>
+        <v>1888</v>
       </c>
       <c r="H273">
         <f t="shared" si="25"/>
@@ -16014,22 +16008,22 @@
     </row>
     <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>1923</v>
+        <v>1904</v>
       </c>
       <c r="B274" t="s">
-        <v>1924</v>
+        <v>1905</v>
       </c>
       <c r="C274" t="s">
-        <v>1925</v>
+        <v>1906</v>
       </c>
       <c r="D274" t="s">
-        <v>1926</v>
+        <v>1907</v>
       </c>
       <c r="E274" t="s">
-        <v>1927</v>
+        <v>1908</v>
       </c>
       <c r="F274" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="H274">
         <f t="shared" si="25"/>
@@ -16055,7 +16049,7 @@
         <v>1371</v>
       </c>
       <c r="D275" t="s">
-        <v>1998</v>
+        <v>1979</v>
       </c>
       <c r="E275" t="s">
         <v>1373</v>
@@ -16110,22 +16104,22 @@
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>1999</v>
+        <v>1980</v>
       </c>
       <c r="B277" t="s">
-        <v>1864</v>
+        <v>1845</v>
       </c>
       <c r="C277" t="s">
-        <v>1865</v>
+        <v>1846</v>
       </c>
       <c r="D277" t="s">
-        <v>1866</v>
+        <v>1847</v>
       </c>
       <c r="E277" t="s">
-        <v>1863</v>
+        <v>1844</v>
       </c>
       <c r="F277" t="s">
-        <v>1862</v>
+        <v>1843</v>
       </c>
       <c r="H277">
         <f t="shared" si="25"/>
@@ -16145,7 +16139,7 @@
         <v>406</v>
       </c>
       <c r="B278" t="s">
-        <v>2000</v>
+        <v>1981</v>
       </c>
       <c r="C278" t="s">
         <v>1377</v>
@@ -16180,7 +16174,7 @@
         <v>1380</v>
       </c>
       <c r="C279" t="s">
-        <v>2004</v>
+        <v>1985</v>
       </c>
       <c r="D279" t="s">
         <v>1381</v>
@@ -16206,22 +16200,22 @@
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>1878</v>
+        <v>1859</v>
       </c>
       <c r="B280" t="s">
-        <v>1879</v>
+        <v>1860</v>
       </c>
       <c r="C280" t="s">
         <v>73</v>
       </c>
       <c r="D280" t="s">
-        <v>1880</v>
+        <v>1861</v>
       </c>
       <c r="E280" t="s">
-        <v>1881</v>
+        <v>1862</v>
       </c>
       <c r="F280" t="s">
-        <v>1886</v>
+        <v>1867</v>
       </c>
       <c r="H280">
         <f t="shared" si="25"/>
@@ -16241,16 +16235,16 @@
         <v>925</v>
       </c>
       <c r="B281" t="s">
-        <v>2003</v>
+        <v>1984</v>
       </c>
       <c r="C281" t="s">
-        <v>2002</v>
+        <v>1983</v>
       </c>
       <c r="D281" t="s">
         <v>1383</v>
       </c>
       <c r="E281" t="s">
-        <v>2001</v>
+        <v>1982</v>
       </c>
       <c r="F281" t="s">
         <v>597</v>
@@ -16302,22 +16296,22 @@
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>1908</v>
+        <v>1889</v>
       </c>
       <c r="B283" t="s">
-        <v>1909</v>
+        <v>1890</v>
       </c>
       <c r="C283" t="s">
-        <v>1910</v>
+        <v>1891</v>
       </c>
       <c r="D283" t="s">
-        <v>1911</v>
+        <v>1892</v>
       </c>
       <c r="E283" t="s">
-        <v>1912</v>
+        <v>1893</v>
       </c>
       <c r="F283" t="s">
-        <v>1907</v>
+        <v>1888</v>
       </c>
       <c r="H283">
         <f t="shared" ref="H283:H346" si="27">INT(J283/3)</f>
@@ -16343,13 +16337,13 @@
         <v>547</v>
       </c>
       <c r="D284" t="s">
-        <v>1933</v>
+        <v>1914</v>
       </c>
       <c r="E284" t="s">
-        <v>1934</v>
+        <v>1915</v>
       </c>
       <c r="F284" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="H284">
         <f t="shared" si="27"/>
@@ -16366,22 +16360,22 @@
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>1935</v>
+        <v>1916</v>
       </c>
       <c r="B285" t="s">
-        <v>1936</v>
+        <v>1917</v>
       </c>
       <c r="C285" t="s">
-        <v>1937</v>
+        <v>1918</v>
       </c>
       <c r="D285" t="s">
         <v>1390</v>
       </c>
       <c r="E285" t="s">
-        <v>1938</v>
+        <v>1919</v>
       </c>
       <c r="F285" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="H285">
         <f t="shared" si="27"/>
@@ -16398,22 +16392,22 @@
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>1939</v>
+        <v>1920</v>
       </c>
       <c r="B286" t="s">
-        <v>1940</v>
+        <v>1921</v>
       </c>
       <c r="C286" t="s">
-        <v>1774</v>
+        <v>1755</v>
       </c>
       <c r="D286" t="s">
         <v>1279</v>
       </c>
       <c r="E286" t="s">
-        <v>1941</v>
+        <v>1922</v>
       </c>
       <c r="F286" t="s">
-        <v>1932</v>
+        <v>1913</v>
       </c>
       <c r="H286">
         <f t="shared" si="27"/>
@@ -16462,22 +16456,22 @@
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>1892</v>
+        <v>1873</v>
       </c>
       <c r="B288" t="s">
-        <v>1890</v>
+        <v>1871</v>
       </c>
       <c r="C288" t="s">
-        <v>1897</v>
+        <v>1878</v>
       </c>
       <c r="D288" t="s">
-        <v>1889</v>
+        <v>1870</v>
       </c>
       <c r="E288" t="s">
-        <v>1899</v>
+        <v>1880</v>
       </c>
       <c r="F288" t="s">
-        <v>1901</v>
+        <v>1882</v>
       </c>
       <c r="H288">
         <f t="shared" si="27"/>
@@ -16497,7 +16491,7 @@
         <v>1392</v>
       </c>
       <c r="B289" t="s">
-        <v>1523</v>
+        <v>1504</v>
       </c>
       <c r="C289" t="s">
         <v>1393</v>
@@ -16526,22 +16520,22 @@
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>1919</v>
+        <v>1900</v>
       </c>
       <c r="B290" t="s">
-        <v>1920</v>
+        <v>1901</v>
       </c>
       <c r="C290" t="s">
-        <v>1921</v>
+        <v>1902</v>
       </c>
       <c r="D290" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="E290" t="s">
-        <v>1922</v>
+        <v>1903</v>
       </c>
       <c r="F290" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H290">
         <f t="shared" si="27"/>
@@ -16561,19 +16555,19 @@
         <v>438</v>
       </c>
       <c r="B291" t="s">
-        <v>1943</v>
+        <v>1924</v>
       </c>
       <c r="C291" t="s">
-        <v>1944</v>
+        <v>1925</v>
       </c>
       <c r="D291" t="s">
-        <v>1945</v>
+        <v>1926</v>
       </c>
       <c r="E291" t="s">
-        <v>1946</v>
+        <v>1927</v>
       </c>
       <c r="F291" t="s">
-        <v>1947</v>
+        <v>1928</v>
       </c>
       <c r="H291">
         <f t="shared" si="27"/>
@@ -16593,16 +16587,16 @@
         <v>1395</v>
       </c>
       <c r="B292" t="s">
-        <v>1396</v>
+        <v>1986</v>
       </c>
       <c r="C292" t="s">
-        <v>1397</v>
+        <v>1988</v>
       </c>
       <c r="D292" t="s">
-        <v>1398</v>
+        <v>1987</v>
       </c>
       <c r="E292" t="s">
-        <v>1399</v>
+        <v>1989</v>
       </c>
       <c r="F292" t="s">
         <v>597</v>
@@ -16625,19 +16619,19 @@
         <v>1016</v>
       </c>
       <c r="B293" t="s">
-        <v>1882</v>
+        <v>1863</v>
       </c>
       <c r="C293" t="s">
-        <v>1883</v>
+        <v>1864</v>
       </c>
       <c r="D293" t="s">
-        <v>1884</v>
+        <v>1865</v>
       </c>
       <c r="E293" t="s">
-        <v>1885</v>
+        <v>1866</v>
       </c>
       <c r="F293" t="s">
-        <v>1886</v>
+        <v>1867</v>
       </c>
       <c r="H293">
         <f t="shared" si="27"/>
@@ -16654,19 +16648,19 @@
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B294" t="s">
+        <v>1990</v>
+      </c>
+      <c r="C294" t="s">
+        <v>1399</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1400</v>
+      </c>
+      <c r="E294" t="s">
         <v>1401</v>
-      </c>
-      <c r="B294" t="s">
-        <v>1402</v>
-      </c>
-      <c r="C294" t="s">
-        <v>1403</v>
-      </c>
-      <c r="D294" t="s">
-        <v>1404</v>
-      </c>
-      <c r="E294" t="s">
-        <v>1405</v>
       </c>
       <c r="F294" t="s">
         <v>597</v>
@@ -16686,22 +16680,22 @@
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>1893</v>
+        <v>1874</v>
       </c>
       <c r="B295" t="s">
         <v>1249</v>
       </c>
       <c r="C295" t="s">
-        <v>1894</v>
+        <v>1875</v>
       </c>
       <c r="D295" t="s">
-        <v>1888</v>
+        <v>1869</v>
       </c>
       <c r="E295" t="s">
-        <v>1898</v>
+        <v>1879</v>
       </c>
       <c r="F295" t="s">
-        <v>1901</v>
+        <v>1882</v>
       </c>
       <c r="H295">
         <f t="shared" si="27"/>
@@ -16718,19 +16712,19 @@
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D296" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E296" t="s">
         <v>1406</v>
-      </c>
-      <c r="B296" t="s">
-        <v>1407</v>
-      </c>
-      <c r="C296" t="s">
-        <v>1408</v>
-      </c>
-      <c r="D296" t="s">
-        <v>1409</v>
-      </c>
-      <c r="E296" t="s">
-        <v>1410</v>
       </c>
       <c r="F296" t="s">
         <v>597</v>
@@ -16750,19 +16744,19 @@
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>1415</v>
+        <v>1393</v>
       </c>
       <c r="B297" t="s">
-        <v>1416</v>
+        <v>1615</v>
       </c>
       <c r="C297" t="s">
-        <v>1417</v>
+        <v>1065</v>
       </c>
       <c r="D297" t="s">
-        <v>1418</v>
+        <v>1992</v>
       </c>
       <c r="E297" t="s">
-        <v>1419</v>
+        <v>1993</v>
       </c>
       <c r="F297" t="s">
         <v>597</v>
@@ -16782,22 +16776,22 @@
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>1913</v>
+        <v>1894</v>
       </c>
       <c r="B298" t="s">
-        <v>1914</v>
+        <v>1895</v>
       </c>
       <c r="C298" t="s">
-        <v>1915</v>
+        <v>1896</v>
       </c>
       <c r="D298" t="s">
-        <v>1916</v>
+        <v>1897</v>
       </c>
       <c r="E298" t="s">
-        <v>1917</v>
+        <v>1898</v>
       </c>
       <c r="F298" t="s">
-        <v>1918</v>
+        <v>1899</v>
       </c>
       <c r="H298">
         <f t="shared" si="27"/>
@@ -16814,22 +16808,22 @@
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>1420</v>
+        <v>1994</v>
       </c>
       <c r="B299" t="s">
-        <v>1421</v>
+        <v>1995</v>
       </c>
       <c r="C299" t="s">
-        <v>1422</v>
+        <v>1996</v>
       </c>
       <c r="D299" t="s">
-        <v>1423</v>
+        <v>1997</v>
       </c>
       <c r="E299" t="s">
-        <v>1424</v>
+        <v>1998</v>
       </c>
       <c r="F299" t="s">
-        <v>597</v>
+        <v>440</v>
       </c>
       <c r="H299">
         <f t="shared" si="27"/>
@@ -16846,22 +16840,22 @@
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>1887</v>
+        <v>1868</v>
       </c>
       <c r="B300" t="s">
-        <v>1891</v>
+        <v>1872</v>
       </c>
       <c r="C300" t="s">
-        <v>1896</v>
+        <v>1877</v>
       </c>
       <c r="D300" t="s">
-        <v>1895</v>
+        <v>1876</v>
       </c>
       <c r="E300" t="s">
-        <v>1900</v>
+        <v>1881</v>
       </c>
       <c r="F300" t="s">
-        <v>1901</v>
+        <v>1882</v>
       </c>
       <c r="H300">
         <f t="shared" si="27"/>
@@ -16872,28 +16866,28 @@
         <v>45724</v>
       </c>
       <c r="J300">
-        <f t="shared" si="18"/>
+        <f>J299+1</f>
         <v>298</v>
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>1425</v>
+        <v>133</v>
       </c>
       <c r="B301" t="s">
-        <v>1426</v>
+        <v>1999</v>
       </c>
       <c r="C301" t="s">
-        <v>1427</v>
+        <v>2000</v>
       </c>
       <c r="D301" t="s">
-        <v>1428</v>
+        <v>2001</v>
       </c>
       <c r="E301" t="s">
-        <v>1429</v>
+        <v>2002</v>
       </c>
       <c r="F301" t="s">
-        <v>597</v>
+        <v>440</v>
       </c>
       <c r="H301">
         <f t="shared" si="27"/>
@@ -16910,19 +16904,19 @@
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>1430</v>
+        <v>1411</v>
       </c>
       <c r="B302" t="s">
-        <v>1431</v>
+        <v>1412</v>
       </c>
       <c r="C302" t="s">
-        <v>1432</v>
+        <v>1413</v>
       </c>
       <c r="D302" t="s">
         <v>1157</v>
       </c>
       <c r="E302" t="s">
-        <v>1433</v>
+        <v>1414</v>
       </c>
       <c r="F302" t="s">
         <v>597</v>
@@ -16942,19 +16936,19 @@
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>1434</v>
+        <v>1415</v>
       </c>
       <c r="B303" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="C303" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="D303" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="E303" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="F303" t="s">
         <v>597</v>
@@ -16974,22 +16968,22 @@
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>1948</v>
+        <v>1929</v>
       </c>
       <c r="B304" t="s">
-        <v>1949</v>
+        <v>1930</v>
       </c>
       <c r="C304" t="s">
-        <v>1950</v>
+        <v>1931</v>
       </c>
       <c r="D304" t="s">
-        <v>1951</v>
+        <v>1932</v>
       </c>
       <c r="E304" t="s">
-        <v>1952</v>
+        <v>1933</v>
       </c>
       <c r="F304" t="s">
-        <v>1953</v>
+        <v>1934</v>
       </c>
       <c r="H304">
         <f t="shared" si="27"/>
@@ -17006,22 +17000,22 @@
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>1954</v>
+        <v>1935</v>
       </c>
       <c r="B305" t="s">
-        <v>1955</v>
+        <v>1936</v>
       </c>
       <c r="C305" t="s">
-        <v>1956</v>
+        <v>1937</v>
       </c>
       <c r="D305" t="s">
-        <v>1957</v>
+        <v>1938</v>
       </c>
       <c r="E305" t="s">
-        <v>1958</v>
+        <v>1939</v>
       </c>
       <c r="F305" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H305">
         <f t="shared" si="27"/>
@@ -17038,22 +17032,22 @@
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>1959</v>
+        <v>1940</v>
       </c>
       <c r="B306" t="s">
-        <v>1960</v>
+        <v>1941</v>
       </c>
       <c r="C306" t="s">
-        <v>1961</v>
+        <v>1942</v>
       </c>
       <c r="D306" t="s">
-        <v>1962</v>
+        <v>1943</v>
       </c>
       <c r="E306" t="s">
-        <v>1963</v>
+        <v>1944</v>
       </c>
       <c r="F306" t="s">
-        <v>1964</v>
+        <v>1945</v>
       </c>
       <c r="H306">
         <f t="shared" si="27"/>
@@ -17073,19 +17067,19 @@
         <v>31</v>
       </c>
       <c r="B307" t="s">
-        <v>1965</v>
+        <v>1946</v>
       </c>
       <c r="C307" t="s">
-        <v>1966</v>
+        <v>1947</v>
       </c>
       <c r="D307" t="s">
-        <v>1825</v>
+        <v>1806</v>
       </c>
       <c r="E307" t="s">
-        <v>1967</v>
+        <v>1948</v>
       </c>
       <c r="F307" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H307">
         <f t="shared" si="27"/>
@@ -17102,22 +17096,22 @@
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>1988</v>
+        <v>1969</v>
       </c>
       <c r="B308" t="s">
-        <v>1989</v>
+        <v>1970</v>
       </c>
       <c r="C308" t="s">
-        <v>1990</v>
+        <v>1971</v>
       </c>
       <c r="D308" t="s">
-        <v>1991</v>
+        <v>1972</v>
       </c>
       <c r="E308" t="s">
-        <v>1992</v>
+        <v>1973</v>
       </c>
       <c r="F308" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H308">
         <f t="shared" si="27"/>
@@ -17134,22 +17128,22 @@
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>1993</v>
+        <v>1974</v>
       </c>
       <c r="B309" t="s">
-        <v>1994</v>
+        <v>1975</v>
       </c>
       <c r="C309" t="s">
-        <v>1995</v>
+        <v>1976</v>
       </c>
       <c r="D309" t="s">
-        <v>1996</v>
+        <v>1977</v>
       </c>
       <c r="E309" t="s">
-        <v>1997</v>
+        <v>1978</v>
       </c>
       <c r="F309" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H309">
         <f t="shared" si="27"/>
@@ -17169,16 +17163,16 @@
         <v>533</v>
       </c>
       <c r="B310" t="s">
-        <v>1435</v>
+        <v>1416</v>
       </c>
       <c r="C310" t="s">
-        <v>1436</v>
+        <v>1417</v>
       </c>
       <c r="D310" t="s">
-        <v>1437</v>
+        <v>1418</v>
       </c>
       <c r="E310" t="s">
-        <v>1438</v>
+        <v>1419</v>
       </c>
       <c r="F310" t="s">
         <v>597</v>
@@ -17198,19 +17192,19 @@
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>1439</v>
+        <v>1420</v>
       </c>
       <c r="B311" t="s">
-        <v>1440</v>
+        <v>1421</v>
       </c>
       <c r="C311" t="s">
-        <v>1441</v>
+        <v>1422</v>
       </c>
       <c r="D311" t="s">
-        <v>1442</v>
+        <v>1423</v>
       </c>
       <c r="E311" t="s">
-        <v>1443</v>
+        <v>1424</v>
       </c>
       <c r="F311" t="s">
         <v>597</v>
@@ -17233,16 +17227,16 @@
         <v>208</v>
       </c>
       <c r="B312" t="s">
-        <v>1444</v>
+        <v>1425</v>
       </c>
       <c r="C312" t="s">
-        <v>1445</v>
+        <v>1426</v>
       </c>
       <c r="D312" t="s">
-        <v>1446</v>
+        <v>1427</v>
       </c>
       <c r="E312" t="s">
-        <v>1447</v>
+        <v>1428</v>
       </c>
       <c r="F312" t="s">
         <v>597</v>
@@ -17265,16 +17259,16 @@
         <v>210</v>
       </c>
       <c r="B313" t="s">
-        <v>1448</v>
+        <v>1429</v>
       </c>
       <c r="C313" t="s">
-        <v>1449</v>
+        <v>1430</v>
       </c>
       <c r="D313" t="s">
-        <v>1450</v>
+        <v>1431</v>
       </c>
       <c r="E313" t="s">
-        <v>1451</v>
+        <v>1432</v>
       </c>
       <c r="F313" t="s">
         <v>597</v>
@@ -17294,19 +17288,19 @@
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>1452</v>
+        <v>1433</v>
       </c>
       <c r="B314" t="s">
         <v>857</v>
       </c>
       <c r="C314" t="s">
-        <v>1453</v>
+        <v>1434</v>
       </c>
       <c r="D314" t="s">
-        <v>1454</v>
+        <v>1435</v>
       </c>
       <c r="E314" t="s">
-        <v>1455</v>
+        <v>1436</v>
       </c>
       <c r="F314" t="s">
         <v>597</v>
@@ -17326,22 +17320,22 @@
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>1978</v>
+        <v>1959</v>
       </c>
       <c r="B315" t="s">
-        <v>1979</v>
+        <v>1960</v>
       </c>
       <c r="C315" t="s">
-        <v>1980</v>
+        <v>1961</v>
       </c>
       <c r="D315" t="s">
-        <v>1981</v>
+        <v>1962</v>
       </c>
       <c r="E315" t="s">
-        <v>1982</v>
+        <v>1963</v>
       </c>
       <c r="F315" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H315">
         <f t="shared" si="27"/>
@@ -17358,19 +17352,19 @@
     </row>
     <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>1456</v>
+        <v>1437</v>
       </c>
       <c r="B316" t="s">
-        <v>1457</v>
+        <v>1438</v>
       </c>
       <c r="C316" t="s">
-        <v>1458</v>
+        <v>1439</v>
       </c>
       <c r="D316" t="s">
-        <v>1459</v>
+        <v>1440</v>
       </c>
       <c r="E316" t="s">
-        <v>1460</v>
+        <v>1441</v>
       </c>
       <c r="F316" t="s">
         <v>597</v>
@@ -17390,19 +17384,19 @@
     </row>
     <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>1461</v>
+        <v>1442</v>
       </c>
       <c r="B317" t="s">
-        <v>1462</v>
+        <v>1443</v>
       </c>
       <c r="C317" t="s">
         <v>1268</v>
       </c>
       <c r="D317" t="s">
-        <v>1463</v>
+        <v>1444</v>
       </c>
       <c r="E317" t="s">
-        <v>1464</v>
+        <v>1445</v>
       </c>
       <c r="F317" t="s">
         <v>597</v>
@@ -17422,19 +17416,19 @@
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>1465</v>
+        <v>1446</v>
       </c>
       <c r="B318" t="s">
-        <v>1466</v>
+        <v>1447</v>
       </c>
       <c r="C318" t="s">
-        <v>1467</v>
+        <v>1448</v>
       </c>
       <c r="D318" t="s">
-        <v>1468</v>
+        <v>1449</v>
       </c>
       <c r="E318" t="s">
-        <v>1469</v>
+        <v>1450</v>
       </c>
       <c r="F318" t="s">
         <v>597</v>
@@ -17454,19 +17448,19 @@
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>1470</v>
+        <v>1451</v>
       </c>
       <c r="B319" t="s">
-        <v>1471</v>
+        <v>1452</v>
       </c>
       <c r="C319" t="s">
-        <v>1472</v>
+        <v>1453</v>
       </c>
       <c r="D319" t="s">
-        <v>1473</v>
+        <v>1454</v>
       </c>
       <c r="E319" t="s">
-        <v>1474</v>
+        <v>1455</v>
       </c>
       <c r="F319" t="s">
         <v>597</v>
@@ -17486,19 +17480,19 @@
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>1475</v>
+        <v>1456</v>
       </c>
       <c r="B320" t="s">
-        <v>1476</v>
+        <v>1457</v>
       </c>
       <c r="C320" t="s">
-        <v>1477</v>
+        <v>1458</v>
       </c>
       <c r="D320" t="s">
-        <v>1478</v>
+        <v>1459</v>
       </c>
       <c r="E320" t="s">
-        <v>1479</v>
+        <v>1460</v>
       </c>
       <c r="F320" t="s">
         <v>597</v>
@@ -17518,19 +17512,19 @@
     </row>
     <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>1480</v>
+        <v>1461</v>
       </c>
       <c r="B321" t="s">
         <v>1279</v>
       </c>
       <c r="C321" t="s">
-        <v>1481</v>
+        <v>1462</v>
       </c>
       <c r="D321" t="s">
-        <v>1482</v>
+        <v>1463</v>
       </c>
       <c r="E321" t="s">
-        <v>1483</v>
+        <v>1464</v>
       </c>
       <c r="F321" t="s">
         <v>597</v>
@@ -17550,19 +17544,19 @@
     </row>
     <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>1484</v>
+        <v>1465</v>
       </c>
       <c r="B322" t="s">
-        <v>1485</v>
+        <v>1466</v>
       </c>
       <c r="C322" t="s">
-        <v>1486</v>
+        <v>1467</v>
       </c>
       <c r="D322" t="s">
-        <v>1487</v>
+        <v>1468</v>
       </c>
       <c r="E322" t="s">
-        <v>1488</v>
+        <v>1469</v>
       </c>
       <c r="F322" t="s">
         <v>597</v>
@@ -17582,19 +17576,19 @@
     </row>
     <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>1489</v>
+        <v>1470</v>
       </c>
       <c r="B323" t="s">
-        <v>1490</v>
+        <v>1471</v>
       </c>
       <c r="C323" t="s">
-        <v>1491</v>
+        <v>1472</v>
       </c>
       <c r="D323" t="s">
-        <v>1492</v>
+        <v>1473</v>
       </c>
       <c r="E323" t="s">
-        <v>1493</v>
+        <v>1474</v>
       </c>
       <c r="F323" t="s">
         <v>597</v>
@@ -17614,19 +17608,19 @@
     </row>
     <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>1494</v>
+        <v>1475</v>
       </c>
       <c r="B324" t="s">
-        <v>1495</v>
+        <v>1476</v>
       </c>
       <c r="C324" t="s">
-        <v>1496</v>
+        <v>1477</v>
       </c>
       <c r="D324" t="s">
-        <v>1497</v>
+        <v>1478</v>
       </c>
       <c r="E324" t="s">
-        <v>1498</v>
+        <v>1479</v>
       </c>
       <c r="F324" t="s">
         <v>597</v>
@@ -17646,19 +17640,19 @@
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>1499</v>
+        <v>1480</v>
       </c>
       <c r="B325" t="s">
-        <v>1500</v>
+        <v>1481</v>
       </c>
       <c r="C325" t="s">
-        <v>1501</v>
+        <v>1482</v>
       </c>
       <c r="D325" t="s">
-        <v>1502</v>
+        <v>1483</v>
       </c>
       <c r="E325" t="s">
-        <v>1503</v>
+        <v>1484</v>
       </c>
       <c r="F325" t="s">
         <v>597</v>
@@ -17678,19 +17672,19 @@
     </row>
     <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>1504</v>
+        <v>1485</v>
       </c>
       <c r="B326" t="s">
-        <v>1505</v>
+        <v>1486</v>
       </c>
       <c r="C326" t="s">
-        <v>1506</v>
+        <v>1487</v>
       </c>
       <c r="D326" t="s">
         <v>1111</v>
       </c>
       <c r="E326" t="s">
-        <v>1507</v>
+        <v>1488</v>
       </c>
       <c r="F326" t="s">
         <v>597</v>
@@ -17710,22 +17704,22 @@
     </row>
     <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>1973</v>
+        <v>1954</v>
       </c>
       <c r="B327" t="s">
-        <v>1974</v>
+        <v>1955</v>
       </c>
       <c r="C327" t="s">
-        <v>1975</v>
+        <v>1956</v>
       </c>
       <c r="D327" t="s">
-        <v>1976</v>
+        <v>1957</v>
       </c>
       <c r="E327" t="s">
-        <v>1977</v>
+        <v>1958</v>
       </c>
       <c r="F327" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H327">
         <f t="shared" si="27"/>
@@ -17742,22 +17736,22 @@
     </row>
     <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>1983</v>
+        <v>1964</v>
       </c>
       <c r="B328" t="s">
-        <v>1984</v>
+        <v>1965</v>
       </c>
       <c r="C328" t="s">
-        <v>1985</v>
+        <v>1966</v>
       </c>
       <c r="D328" t="s">
-        <v>1986</v>
+        <v>1967</v>
       </c>
       <c r="E328" t="s">
-        <v>1987</v>
+        <v>1968</v>
       </c>
       <c r="F328" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H328">
         <f t="shared" si="27"/>
@@ -17774,19 +17768,19 @@
     </row>
     <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>1508</v>
+        <v>1489</v>
       </c>
       <c r="B329" t="s">
         <v>1110</v>
       </c>
       <c r="C329" t="s">
-        <v>1509</v>
+        <v>1490</v>
       </c>
       <c r="D329" t="s">
-        <v>1510</v>
+        <v>1491</v>
       </c>
       <c r="E329" t="s">
-        <v>1511</v>
+        <v>1492</v>
       </c>
       <c r="F329" t="s">
         <v>597</v>
@@ -17806,19 +17800,19 @@
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>1512</v>
+        <v>1493</v>
       </c>
       <c r="B330" t="s">
         <v>218</v>
       </c>
       <c r="C330" t="s">
-        <v>1513</v>
+        <v>1494</v>
       </c>
       <c r="D330" t="s">
-        <v>1514</v>
+        <v>1495</v>
       </c>
       <c r="E330" t="s">
-        <v>1515</v>
+        <v>1496</v>
       </c>
       <c r="F330" t="s">
         <v>597</v>
@@ -17838,19 +17832,19 @@
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>1516</v>
+        <v>1497</v>
       </c>
       <c r="B331" t="s">
-        <v>1517</v>
+        <v>1498</v>
       </c>
       <c r="C331" t="s">
-        <v>1518</v>
+        <v>1499</v>
       </c>
       <c r="D331" t="s">
-        <v>1519</v>
+        <v>1500</v>
       </c>
       <c r="E331" t="s">
-        <v>1520</v>
+        <v>1501</v>
       </c>
       <c r="F331" t="s">
         <v>597</v>
@@ -17870,19 +17864,19 @@
     </row>
     <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>1521</v>
+        <v>1502</v>
       </c>
       <c r="B332" t="s">
-        <v>1522</v>
+        <v>1503</v>
       </c>
       <c r="C332" t="s">
-        <v>1523</v>
+        <v>1504</v>
       </c>
       <c r="D332" t="s">
-        <v>1524</v>
+        <v>1505</v>
       </c>
       <c r="E332" t="s">
-        <v>1525</v>
+        <v>1506</v>
       </c>
       <c r="F332" t="s">
         <v>597</v>
@@ -17902,19 +17896,19 @@
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>1526</v>
+        <v>1507</v>
       </c>
       <c r="B333" t="s">
         <v>973</v>
       </c>
       <c r="C333" t="s">
-        <v>1527</v>
+        <v>1508</v>
       </c>
       <c r="D333" t="s">
-        <v>1528</v>
+        <v>1509</v>
       </c>
       <c r="E333" t="s">
-        <v>1529</v>
+        <v>1510</v>
       </c>
       <c r="F333" t="s">
         <v>597</v>
@@ -17934,19 +17928,19 @@
     </row>
     <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>1530</v>
+        <v>1511</v>
       </c>
       <c r="B334" t="s">
-        <v>1531</v>
+        <v>1512</v>
       </c>
       <c r="C334" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="D334" t="s">
-        <v>1532</v>
+        <v>1513</v>
       </c>
       <c r="E334" t="s">
-        <v>1533</v>
+        <v>1514</v>
       </c>
       <c r="F334" t="s">
         <v>597</v>
@@ -17966,19 +17960,19 @@
     </row>
     <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>1534</v>
+        <v>1515</v>
       </c>
       <c r="B335" t="s">
-        <v>1535</v>
+        <v>1516</v>
       </c>
       <c r="C335" t="s">
-        <v>1536</v>
+        <v>1517</v>
       </c>
       <c r="D335" t="s">
-        <v>1537</v>
+        <v>1518</v>
       </c>
       <c r="E335" t="s">
-        <v>1538</v>
+        <v>1519</v>
       </c>
       <c r="F335" t="s">
         <v>597</v>
@@ -17998,19 +17992,19 @@
     </row>
     <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>1539</v>
+        <v>1520</v>
       </c>
       <c r="B336" t="s">
-        <v>1540</v>
+        <v>1521</v>
       </c>
       <c r="C336" t="s">
-        <v>1541</v>
+        <v>1522</v>
       </c>
       <c r="D336" t="s">
-        <v>1542</v>
+        <v>1523</v>
       </c>
       <c r="E336" t="s">
-        <v>1543</v>
+        <v>1524</v>
       </c>
       <c r="F336" t="s">
         <v>597</v>
@@ -18030,19 +18024,19 @@
     </row>
     <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>1544</v>
+        <v>1525</v>
       </c>
       <c r="B337" t="s">
-        <v>1545</v>
+        <v>1526</v>
       </c>
       <c r="C337" t="s">
-        <v>1546</v>
+        <v>1527</v>
       </c>
       <c r="D337" t="s">
-        <v>1547</v>
+        <v>1528</v>
       </c>
       <c r="E337" t="s">
-        <v>1548</v>
+        <v>1529</v>
       </c>
       <c r="F337" t="s">
         <v>597</v>
@@ -18062,19 +18056,19 @@
     </row>
     <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>1549</v>
+        <v>1530</v>
       </c>
       <c r="B338" t="s">
-        <v>1550</v>
+        <v>1531</v>
       </c>
       <c r="C338" t="s">
-        <v>1551</v>
+        <v>1532</v>
       </c>
       <c r="D338" t="s">
-        <v>1552</v>
+        <v>1533</v>
       </c>
       <c r="E338" t="s">
-        <v>1553</v>
+        <v>1534</v>
       </c>
       <c r="F338" t="s">
         <v>597</v>
@@ -18094,19 +18088,19 @@
     </row>
     <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>1554</v>
+        <v>1535</v>
       </c>
       <c r="B339" t="s">
-        <v>1555</v>
+        <v>1536</v>
       </c>
       <c r="C339" t="s">
-        <v>1556</v>
+        <v>1537</v>
       </c>
       <c r="D339" t="s">
-        <v>1557</v>
+        <v>1538</v>
       </c>
       <c r="E339" t="s">
-        <v>1558</v>
+        <v>1539</v>
       </c>
       <c r="F339" t="s">
         <v>597</v>
@@ -18129,16 +18123,16 @@
         <v>574</v>
       </c>
       <c r="B340" t="s">
-        <v>1559</v>
+        <v>1540</v>
       </c>
       <c r="C340" t="s">
-        <v>1560</v>
+        <v>1541</v>
       </c>
       <c r="D340" t="s">
-        <v>1561</v>
+        <v>1542</v>
       </c>
       <c r="E340" t="s">
-        <v>1562</v>
+        <v>1543</v>
       </c>
       <c r="F340" t="s">
         <v>597</v>
@@ -18158,19 +18152,19 @@
     </row>
     <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>1563</v>
+        <v>1544</v>
       </c>
       <c r="B341" t="s">
-        <v>1564</v>
+        <v>1545</v>
       </c>
       <c r="C341" t="s">
-        <v>1565</v>
+        <v>1546</v>
       </c>
       <c r="D341" t="s">
-        <v>1566</v>
+        <v>1547</v>
       </c>
       <c r="E341" t="s">
-        <v>1567</v>
+        <v>1548</v>
       </c>
       <c r="F341" t="s">
         <v>597</v>
@@ -18190,19 +18184,19 @@
     </row>
     <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>1568</v>
+        <v>1549</v>
       </c>
       <c r="B342" t="s">
-        <v>1569</v>
+        <v>1550</v>
       </c>
       <c r="C342" t="s">
-        <v>1570</v>
+        <v>1551</v>
       </c>
       <c r="D342" t="s">
-        <v>1571</v>
+        <v>1552</v>
       </c>
       <c r="E342" t="s">
-        <v>1572</v>
+        <v>1553</v>
       </c>
       <c r="F342" t="s">
         <v>597</v>
@@ -18222,19 +18216,19 @@
     </row>
     <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>1573</v>
+        <v>1554</v>
       </c>
       <c r="B343" t="s">
-        <v>1574</v>
+        <v>1555</v>
       </c>
       <c r="C343" t="s">
-        <v>1575</v>
+        <v>1556</v>
       </c>
       <c r="D343" t="s">
-        <v>1576</v>
+        <v>1557</v>
       </c>
       <c r="E343" t="s">
-        <v>1577</v>
+        <v>1558</v>
       </c>
       <c r="F343" t="s">
         <v>597</v>
@@ -18254,19 +18248,19 @@
     </row>
     <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>1578</v>
+        <v>1559</v>
       </c>
       <c r="B344" t="s">
         <v>676</v>
       </c>
       <c r="C344" t="s">
-        <v>1579</v>
+        <v>1560</v>
       </c>
       <c r="D344" t="s">
-        <v>1580</v>
+        <v>1561</v>
       </c>
       <c r="E344" t="s">
-        <v>1581</v>
+        <v>1562</v>
       </c>
       <c r="F344" t="s">
         <v>597</v>
@@ -18289,16 +18283,16 @@
         <v>779</v>
       </c>
       <c r="B345" t="s">
-        <v>1582</v>
+        <v>1563</v>
       </c>
       <c r="C345" t="s">
-        <v>1583</v>
+        <v>1564</v>
       </c>
       <c r="D345" t="s">
-        <v>1584</v>
+        <v>1565</v>
       </c>
       <c r="E345" t="s">
-        <v>1585</v>
+        <v>1566</v>
       </c>
       <c r="F345" t="s">
         <v>597</v>
@@ -18318,19 +18312,19 @@
     </row>
     <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>1586</v>
+        <v>1567</v>
       </c>
       <c r="B346" t="s">
-        <v>1587</v>
+        <v>1568</v>
       </c>
       <c r="C346" t="s">
-        <v>1588</v>
+        <v>1569</v>
       </c>
       <c r="D346" t="s">
-        <v>1589</v>
+        <v>1570</v>
       </c>
       <c r="E346" t="s">
-        <v>1590</v>
+        <v>1571</v>
       </c>
       <c r="F346" t="s">
         <v>597</v>
@@ -18350,16 +18344,16 @@
     </row>
     <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>1591</v>
+        <v>1572</v>
       </c>
       <c r="B347" t="s">
-        <v>1592</v>
+        <v>1573</v>
       </c>
       <c r="C347" t="s">
         <v>1396</v>
       </c>
       <c r="D347" t="s">
-        <v>1593</v>
+        <v>1574</v>
       </c>
       <c r="E347" t="s">
         <v>1060</v>
@@ -18382,19 +18376,19 @@
     </row>
     <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>1594</v>
+        <v>1575</v>
       </c>
       <c r="B348" t="s">
-        <v>1595</v>
+        <v>1576</v>
       </c>
       <c r="C348" t="s">
-        <v>1596</v>
+        <v>1577</v>
       </c>
       <c r="D348" t="s">
-        <v>1597</v>
+        <v>1578</v>
       </c>
       <c r="E348" t="s">
-        <v>1598</v>
+        <v>1579</v>
       </c>
       <c r="F348" t="s">
         <v>597</v>
@@ -18414,19 +18408,19 @@
     </row>
     <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>1599</v>
+        <v>1580</v>
       </c>
       <c r="B349" t="s">
-        <v>1600</v>
+        <v>1581</v>
       </c>
       <c r="C349" t="s">
-        <v>1601</v>
+        <v>1582</v>
       </c>
       <c r="D349" t="s">
-        <v>1602</v>
+        <v>1583</v>
       </c>
       <c r="E349" t="s">
-        <v>1603</v>
+        <v>1584</v>
       </c>
       <c r="F349" t="s">
         <v>597</v>
@@ -18446,22 +18440,22 @@
     </row>
     <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>1968</v>
+        <v>1949</v>
       </c>
       <c r="B350" t="s">
-        <v>1969</v>
+        <v>1950</v>
       </c>
       <c r="C350" t="s">
-        <v>1970</v>
+        <v>1951</v>
       </c>
       <c r="D350" t="s">
-        <v>1971</v>
+        <v>1952</v>
       </c>
       <c r="E350" t="s">
-        <v>1972</v>
+        <v>1953</v>
       </c>
       <c r="F350" t="s">
-        <v>1942</v>
+        <v>1923</v>
       </c>
       <c r="H350">
         <f t="shared" si="30"/>
@@ -18478,19 +18472,19 @@
     </row>
     <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>1604</v>
+        <v>1585</v>
       </c>
       <c r="B351" t="s">
-        <v>1605</v>
+        <v>1586</v>
       </c>
       <c r="C351" t="s">
-        <v>1606</v>
+        <v>1587</v>
       </c>
       <c r="D351" t="s">
-        <v>1607</v>
+        <v>1588</v>
       </c>
       <c r="E351" t="s">
-        <v>1608</v>
+        <v>1589</v>
       </c>
       <c r="F351" t="s">
         <v>597</v>
@@ -18510,19 +18504,19 @@
     </row>
     <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>1609</v>
+        <v>1590</v>
       </c>
       <c r="B352" t="s">
-        <v>1610</v>
+        <v>1591</v>
       </c>
       <c r="C352" t="s">
-        <v>1611</v>
+        <v>1592</v>
       </c>
       <c r="D352" t="s">
-        <v>1612</v>
+        <v>1593</v>
       </c>
       <c r="E352" t="s">
-        <v>1613</v>
+        <v>1594</v>
       </c>
       <c r="F352" t="s">
         <v>597</v>
@@ -18542,19 +18536,19 @@
     </row>
     <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>1614</v>
+        <v>1595</v>
       </c>
       <c r="B353" t="s">
         <v>1119</v>
       </c>
       <c r="C353" t="s">
-        <v>1615</v>
+        <v>1596</v>
       </c>
       <c r="D353" t="s">
-        <v>1616</v>
+        <v>1597</v>
       </c>
       <c r="E353" t="s">
-        <v>1617</v>
+        <v>1598</v>
       </c>
       <c r="F353" t="s">
         <v>597</v>
@@ -18574,19 +18568,19 @@
     </row>
     <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>1618</v>
+        <v>1599</v>
       </c>
       <c r="B354" t="s">
         <v>308</v>
       </c>
       <c r="C354" t="s">
-        <v>1619</v>
+        <v>1600</v>
       </c>
       <c r="D354" t="s">
-        <v>1620</v>
+        <v>1601</v>
       </c>
       <c r="E354" t="s">
-        <v>1621</v>
+        <v>1602</v>
       </c>
       <c r="F354" t="s">
         <v>597</v>
@@ -18606,19 +18600,19 @@
     </row>
     <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>1622</v>
+        <v>1603</v>
       </c>
       <c r="B355" t="s">
-        <v>1623</v>
+        <v>1604</v>
       </c>
       <c r="C355" t="s">
-        <v>1624</v>
+        <v>1605</v>
       </c>
       <c r="D355" t="s">
-        <v>1625</v>
+        <v>1606</v>
       </c>
       <c r="E355" t="s">
-        <v>1626</v>
+        <v>1607</v>
       </c>
       <c r="F355" t="s">
         <v>597</v>
@@ -18638,7 +18632,7 @@
     </row>
     <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>1627</v>
+        <v>1608</v>
       </c>
       <c r="B356" t="s">
         <v>1253</v>
@@ -18647,10 +18641,10 @@
         <v>367</v>
       </c>
       <c r="D356" t="s">
-        <v>1628</v>
+        <v>1609</v>
       </c>
       <c r="E356" t="s">
-        <v>1629</v>
+        <v>1610</v>
       </c>
       <c r="F356" t="s">
         <v>597</v>
@@ -18670,19 +18664,19 @@
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>1630</v>
+        <v>1611</v>
       </c>
       <c r="B357" t="s">
-        <v>1631</v>
+        <v>1612</v>
       </c>
       <c r="C357" t="s">
-        <v>1632</v>
+        <v>1613</v>
       </c>
       <c r="D357" t="s">
         <v>925</v>
       </c>
       <c r="E357" t="s">
-        <v>1633</v>
+        <v>1614</v>
       </c>
       <c r="F357" t="s">
         <v>597</v>
@@ -18702,19 +18696,19 @@
     </row>
     <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>1634</v>
+        <v>1615</v>
       </c>
       <c r="B358" t="s">
-        <v>1635</v>
+        <v>1616</v>
       </c>
       <c r="C358" t="s">
         <v>227</v>
       </c>
       <c r="D358" t="s">
-        <v>1636</v>
+        <v>1617</v>
       </c>
       <c r="E358" t="s">
-        <v>1637</v>
+        <v>1618</v>
       </c>
       <c r="F358" t="s">
         <v>597</v>
@@ -18734,16 +18728,16 @@
     </row>
     <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="B359" t="s">
-        <v>1638</v>
+        <v>1619</v>
       </c>
       <c r="C359" t="s">
-        <v>1639</v>
+        <v>1620</v>
       </c>
       <c r="E359" t="s">
-        <v>1640</v>
+        <v>1621</v>
       </c>
       <c r="F359" t="s">
         <v>597</v>
@@ -18763,19 +18757,19 @@
     </row>
     <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>1641</v>
+        <v>1622</v>
       </c>
       <c r="B360" t="s">
-        <v>1642</v>
+        <v>1623</v>
       </c>
       <c r="C360" t="s">
-        <v>1643</v>
+        <v>1624</v>
       </c>
       <c r="D360" t="s">
-        <v>1644</v>
+        <v>1625</v>
       </c>
       <c r="E360" t="s">
-        <v>1645</v>
+        <v>1626</v>
       </c>
       <c r="F360" t="s">
         <v>597</v>
@@ -18795,19 +18789,19 @@
     </row>
     <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>1646</v>
+        <v>1627</v>
       </c>
       <c r="B361" t="s">
-        <v>1647</v>
+        <v>1628</v>
       </c>
       <c r="C361" t="s">
         <v>228</v>
       </c>
       <c r="D361" t="s">
-        <v>1648</v>
+        <v>1629</v>
       </c>
       <c r="E361" t="s">
-        <v>1649</v>
+        <v>1630</v>
       </c>
       <c r="F361" t="s">
         <v>597</v>
@@ -18827,19 +18821,19 @@
     </row>
     <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>1650</v>
+        <v>1631</v>
       </c>
       <c r="B362" t="s">
-        <v>1651</v>
+        <v>1632</v>
       </c>
       <c r="C362" t="s">
-        <v>1652</v>
+        <v>1633</v>
       </c>
       <c r="D362" t="s">
-        <v>1653</v>
+        <v>1634</v>
       </c>
       <c r="E362" t="s">
-        <v>1654</v>
+        <v>1635</v>
       </c>
       <c r="F362" t="s">
         <v>597</v>
@@ -18859,19 +18853,19 @@
     </row>
     <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>1655</v>
+        <v>1636</v>
       </c>
       <c r="B363" t="s">
-        <v>1656</v>
+        <v>1637</v>
       </c>
       <c r="C363" t="s">
-        <v>1657</v>
+        <v>1638</v>
       </c>
       <c r="D363" t="s">
-        <v>1658</v>
+        <v>1639</v>
       </c>
       <c r="E363" t="s">
-        <v>1659</v>
+        <v>1640</v>
       </c>
       <c r="F363" t="s">
         <v>597</v>
@@ -18891,19 +18885,19 @@
     </row>
     <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>1660</v>
+        <v>1641</v>
       </c>
       <c r="B364" t="s">
-        <v>1661</v>
+        <v>1642</v>
       </c>
       <c r="C364" t="s">
         <v>689</v>
       </c>
       <c r="D364" t="s">
-        <v>1662</v>
+        <v>1643</v>
       </c>
       <c r="E364" t="s">
-        <v>1663</v>
+        <v>1644</v>
       </c>
       <c r="F364" t="s">
         <v>597</v>
@@ -18923,19 +18917,19 @@
     </row>
     <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>1664</v>
+        <v>1645</v>
       </c>
       <c r="B365" t="s">
-        <v>1665</v>
+        <v>1646</v>
       </c>
       <c r="C365" t="s">
-        <v>1666</v>
+        <v>1647</v>
       </c>
       <c r="D365" t="s">
-        <v>1667</v>
+        <v>1648</v>
       </c>
       <c r="E365" t="s">
-        <v>1668</v>
+        <v>1649</v>
       </c>
       <c r="F365" t="s">
         <v>597</v>
@@ -18955,19 +18949,19 @@
     </row>
     <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>1669</v>
+        <v>1650</v>
       </c>
       <c r="B366" t="s">
-        <v>1670</v>
+        <v>1651</v>
       </c>
       <c r="C366" t="s">
-        <v>1671</v>
+        <v>1652</v>
       </c>
       <c r="D366" t="s">
-        <v>1672</v>
+        <v>1653</v>
       </c>
       <c r="E366" t="s">
-        <v>1673</v>
+        <v>1654</v>
       </c>
       <c r="F366" t="s">
         <v>597</v>
@@ -18987,19 +18981,19 @@
     </row>
     <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>1674</v>
+        <v>1655</v>
       </c>
       <c r="B367" t="s">
-        <v>1675</v>
+        <v>1656</v>
       </c>
       <c r="C367" t="s">
-        <v>1676</v>
+        <v>1657</v>
       </c>
       <c r="D367" t="s">
-        <v>1677</v>
+        <v>1658</v>
       </c>
       <c r="E367" t="s">
-        <v>1678</v>
+        <v>1659</v>
       </c>
       <c r="F367" t="s">
         <v>597</v>
@@ -19019,16 +19013,16 @@
     </row>
     <row r="368" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>1679</v>
+        <v>1660</v>
       </c>
       <c r="B368" t="s">
-        <v>1680</v>
+        <v>1661</v>
       </c>
       <c r="C368" t="s">
-        <v>1681</v>
+        <v>1662</v>
       </c>
       <c r="D368" t="s">
-        <v>1682</v>
+        <v>1663</v>
       </c>
       <c r="E368" t="s">
         <v>777</v>
@@ -19051,19 +19045,19 @@
     </row>
     <row r="369" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>1683</v>
+        <v>1664</v>
       </c>
       <c r="B369" t="s">
-        <v>1684</v>
+        <v>1665</v>
       </c>
       <c r="C369" t="s">
-        <v>1685</v>
+        <v>1666</v>
       </c>
       <c r="D369" t="s">
-        <v>1686</v>
+        <v>1667</v>
       </c>
       <c r="E369" t="s">
-        <v>1687</v>
+        <v>1668</v>
       </c>
       <c r="F369" t="s">
         <v>597</v>
@@ -19083,19 +19077,19 @@
     </row>
     <row r="370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>1688</v>
+        <v>1669</v>
       </c>
       <c r="B370" t="s">
-        <v>1689</v>
+        <v>1670</v>
       </c>
       <c r="C370" t="s">
-        <v>1690</v>
+        <v>1671</v>
       </c>
       <c r="D370" t="s">
         <v>1372</v>
       </c>
       <c r="E370" t="s">
-        <v>1691</v>
+        <v>1672</v>
       </c>
       <c r="F370" t="s">
         <v>597</v>
@@ -19115,19 +19109,19 @@
     </row>
     <row r="371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>1692</v>
+        <v>1673</v>
       </c>
       <c r="B371" t="s">
-        <v>1693</v>
+        <v>1674</v>
       </c>
       <c r="C371" t="s">
-        <v>1694</v>
+        <v>1675</v>
       </c>
       <c r="D371" t="s">
-        <v>1695</v>
+        <v>1676</v>
       </c>
       <c r="E371" t="s">
-        <v>1696</v>
+        <v>1677</v>
       </c>
       <c r="F371" t="s">
         <v>597</v>
@@ -19147,19 +19141,19 @@
     </row>
     <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>1697</v>
+        <v>1678</v>
       </c>
       <c r="B372" t="s">
-        <v>1698</v>
+        <v>1679</v>
       </c>
       <c r="C372" t="s">
-        <v>1699</v>
+        <v>1680</v>
       </c>
       <c r="D372" t="s">
-        <v>1700</v>
+        <v>1681</v>
       </c>
       <c r="E372" t="s">
-        <v>1701</v>
+        <v>1682</v>
       </c>
       <c r="F372" t="s">
         <v>597</v>
@@ -19179,19 +19173,19 @@
     </row>
     <row r="373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>1702</v>
+        <v>1683</v>
       </c>
       <c r="B373" t="s">
-        <v>1703</v>
+        <v>1684</v>
       </c>
       <c r="C373" t="s">
-        <v>1704</v>
+        <v>1685</v>
       </c>
       <c r="D373" t="s">
-        <v>1705</v>
+        <v>1686</v>
       </c>
       <c r="E373" t="s">
-        <v>1706</v>
+        <v>1687</v>
       </c>
       <c r="F373" t="s">
         <v>597</v>
@@ -19211,19 +19205,19 @@
     </row>
     <row r="374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>1432</v>
+        <v>1413</v>
       </c>
       <c r="B374" t="s">
         <v>1370</v>
       </c>
       <c r="C374" t="s">
-        <v>1707</v>
+        <v>1688</v>
       </c>
       <c r="D374" t="s">
-        <v>1708</v>
+        <v>1689</v>
       </c>
       <c r="E374" t="s">
-        <v>1709</v>
+        <v>1690</v>
       </c>
       <c r="F374" t="s">
         <v>597</v>
@@ -19246,16 +19240,16 @@
         <v>228</v>
       </c>
       <c r="B375" t="s">
-        <v>1710</v>
+        <v>1691</v>
       </c>
       <c r="C375" t="s">
         <v>20</v>
       </c>
       <c r="D375" t="s">
-        <v>1711</v>
+        <v>1692</v>
       </c>
       <c r="E375" t="s">
-        <v>1712</v>
+        <v>1693</v>
       </c>
       <c r="F375" t="s">
         <v>597</v>
@@ -19275,19 +19269,19 @@
     </row>
     <row r="376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>1713</v>
+        <v>1694</v>
       </c>
       <c r="B376" t="s">
-        <v>1714</v>
+        <v>1695</v>
       </c>
       <c r="C376" t="s">
         <v>674</v>
       </c>
       <c r="D376" t="s">
-        <v>1715</v>
+        <v>1696</v>
       </c>
       <c r="E376" t="s">
-        <v>1716</v>
+        <v>1697</v>
       </c>
       <c r="F376" t="s">
         <v>597</v>
@@ -19307,19 +19301,19 @@
     </row>
     <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>1717</v>
+        <v>1698</v>
       </c>
       <c r="B377" t="s">
-        <v>1718</v>
+        <v>1699</v>
       </c>
       <c r="C377" t="s">
         <v>188</v>
       </c>
       <c r="D377" t="s">
-        <v>1719</v>
+        <v>1700</v>
       </c>
       <c r="E377" t="s">
-        <v>1720</v>
+        <v>1701</v>
       </c>
       <c r="F377" t="s">
         <v>597</v>
@@ -19345,13 +19339,13 @@
         <v>497</v>
       </c>
       <c r="C378" t="s">
-        <v>1721</v>
+        <v>1702</v>
       </c>
       <c r="D378" t="s">
-        <v>1722</v>
+        <v>1703</v>
       </c>
       <c r="E378" t="s">
-        <v>1723</v>
+        <v>1704</v>
       </c>
       <c r="F378" t="s">
         <v>597</v>
@@ -19371,19 +19365,19 @@
     </row>
     <row r="379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>1724</v>
+        <v>1705</v>
       </c>
       <c r="B379" t="s">
-        <v>1725</v>
+        <v>1706</v>
       </c>
       <c r="C379" t="s">
-        <v>1726</v>
+        <v>1707</v>
       </c>
       <c r="D379" t="s">
-        <v>1727</v>
+        <v>1708</v>
       </c>
       <c r="E379" t="s">
-        <v>1728</v>
+        <v>1709</v>
       </c>
       <c r="F379" t="s">
         <v>597</v>
@@ -19403,19 +19397,19 @@
     </row>
     <row r="380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>1729</v>
+        <v>1710</v>
       </c>
       <c r="B380" t="s">
-        <v>1730</v>
+        <v>1711</v>
       </c>
       <c r="C380" t="s">
-        <v>1731</v>
+        <v>1712</v>
       </c>
       <c r="D380" t="s">
-        <v>1732</v>
+        <v>1713</v>
       </c>
       <c r="E380" t="s">
-        <v>1733</v>
+        <v>1714</v>
       </c>
       <c r="F380" t="s">
         <v>597</v>
@@ -19435,19 +19429,19 @@
     </row>
     <row r="381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>1734</v>
+        <v>1715</v>
       </c>
       <c r="B381" t="s">
-        <v>1735</v>
+        <v>1716</v>
       </c>
       <c r="C381" t="s">
-        <v>1736</v>
+        <v>1717</v>
       </c>
       <c r="D381" t="s">
-        <v>1737</v>
+        <v>1718</v>
       </c>
       <c r="E381" t="s">
-        <v>1738</v>
+        <v>1719</v>
       </c>
       <c r="F381" t="s">
         <v>597</v>
@@ -19467,19 +19461,19 @@
     </row>
     <row r="382" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>1739</v>
+        <v>1720</v>
       </c>
       <c r="B382" t="s">
-        <v>1740</v>
+        <v>1721</v>
       </c>
       <c r="C382" t="s">
-        <v>1741</v>
+        <v>1722</v>
       </c>
       <c r="D382" t="s">
-        <v>1742</v>
+        <v>1723</v>
       </c>
       <c r="E382" t="s">
-        <v>1743</v>
+        <v>1724</v>
       </c>
       <c r="F382" t="s">
         <v>597</v>
@@ -19499,19 +19493,19 @@
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>1744</v>
+        <v>1725</v>
       </c>
       <c r="B383" t="s">
-        <v>1745</v>
+        <v>1726</v>
       </c>
       <c r="C383" t="s">
-        <v>1746</v>
+        <v>1727</v>
       </c>
       <c r="D383" t="s">
-        <v>1747</v>
+        <v>1728</v>
       </c>
       <c r="E383" t="s">
-        <v>1748</v>
+        <v>1729</v>
       </c>
       <c r="F383" t="s">
         <v>597</v>
@@ -19531,19 +19525,19 @@
     </row>
     <row r="384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>1749</v>
+        <v>1730</v>
       </c>
       <c r="B384" t="s">
-        <v>1750</v>
+        <v>1731</v>
       </c>
       <c r="C384" t="s">
-        <v>1751</v>
+        <v>1732</v>
       </c>
       <c r="D384" t="s">
-        <v>1752</v>
+        <v>1733</v>
       </c>
       <c r="E384" t="s">
-        <v>1753</v>
+        <v>1734</v>
       </c>
       <c r="F384" t="s">
         <v>597</v>
@@ -19563,19 +19557,19 @@
     </row>
     <row r="385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>1754</v>
+        <v>1735</v>
       </c>
       <c r="B385" t="s">
-        <v>1755</v>
+        <v>1736</v>
       </c>
       <c r="C385" t="s">
-        <v>1756</v>
+        <v>1737</v>
       </c>
       <c r="D385" t="s">
-        <v>1757</v>
+        <v>1738</v>
       </c>
       <c r="E385" t="s">
-        <v>1758</v>
+        <v>1739</v>
       </c>
       <c r="F385" t="s">
         <v>597</v>
@@ -19595,19 +19589,19 @@
     </row>
     <row r="386" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>1636</v>
+        <v>1617</v>
       </c>
       <c r="B386" t="s">
-        <v>1759</v>
+        <v>1740</v>
       </c>
       <c r="C386" t="s">
-        <v>1760</v>
+        <v>1741</v>
       </c>
       <c r="D386" t="s">
-        <v>1761</v>
+        <v>1742</v>
       </c>
       <c r="E386" t="s">
-        <v>1762</v>
+        <v>1743</v>
       </c>
       <c r="F386" t="s">
         <v>597</v>
@@ -19627,19 +19621,19 @@
     </row>
     <row r="387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>1763</v>
+        <v>1744</v>
       </c>
       <c r="B387" t="s">
-        <v>1764</v>
+        <v>1745</v>
       </c>
       <c r="C387" t="s">
-        <v>1765</v>
+        <v>1746</v>
       </c>
       <c r="D387" t="s">
-        <v>1766</v>
+        <v>1747</v>
       </c>
       <c r="E387" t="s">
-        <v>1767</v>
+        <v>1748</v>
       </c>
       <c r="F387" t="s">
         <v>597</v>
@@ -19659,19 +19653,19 @@
     </row>
     <row r="388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>1768</v>
+        <v>1749</v>
       </c>
       <c r="B388" t="s">
-        <v>1769</v>
+        <v>1750</v>
       </c>
       <c r="C388" t="s">
-        <v>1770</v>
+        <v>1751</v>
       </c>
       <c r="D388" t="s">
         <v>1124</v>
       </c>
       <c r="E388" t="s">
-        <v>1771</v>
+        <v>1752</v>
       </c>
       <c r="F388" t="s">
         <v>597</v>
@@ -20843,19 +20837,19 @@
     </row>
     <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>1787</v>
+        <v>1768</v>
       </c>
       <c r="B425" t="s">
-        <v>1788</v>
+        <v>1769</v>
       </c>
       <c r="C425" t="s">
-        <v>1789</v>
+        <v>1770</v>
       </c>
       <c r="D425" t="s">
-        <v>1790</v>
+        <v>1771</v>
       </c>
       <c r="E425" t="s">
-        <v>1605</v>
+        <v>1586</v>
       </c>
       <c r="F425" t="s">
         <v>597</v>
@@ -20875,19 +20869,19 @@
     </row>
     <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>1791</v>
+        <v>1772</v>
       </c>
       <c r="B426" t="s">
-        <v>1792</v>
+        <v>1773</v>
       </c>
       <c r="C426" t="s">
-        <v>1793</v>
+        <v>1774</v>
       </c>
       <c r="D426" t="s">
-        <v>1794</v>
+        <v>1775</v>
       </c>
       <c r="E426" t="s">
-        <v>1795</v>
+        <v>1776</v>
       </c>
       <c r="F426" t="s">
         <v>597</v>
@@ -20910,16 +20904,16 @@
         <v>577</v>
       </c>
       <c r="B427" t="s">
-        <v>1796</v>
+        <v>1777</v>
       </c>
       <c r="C427" t="s">
-        <v>1807</v>
+        <v>1788</v>
       </c>
       <c r="D427" t="s">
-        <v>1797</v>
+        <v>1778</v>
       </c>
       <c r="E427" t="s">
-        <v>1798</v>
+        <v>1779</v>
       </c>
       <c r="F427" t="s">
         <v>597</v>
@@ -20939,16 +20933,16 @@
     </row>
     <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>1799</v>
+        <v>1780</v>
       </c>
       <c r="B428" t="s">
-        <v>1800</v>
+        <v>1781</v>
       </c>
       <c r="C428" t="s">
-        <v>1801</v>
+        <v>1782</v>
       </c>
       <c r="D428" t="s">
-        <v>1802</v>
+        <v>1783</v>
       </c>
       <c r="E428" t="s">
         <v>210</v>
@@ -20974,16 +20968,16 @@
         <v>1353</v>
       </c>
       <c r="B429" t="s">
-        <v>1803</v>
+        <v>1784</v>
       </c>
       <c r="C429" t="s">
-        <v>1804</v>
+        <v>1785</v>
       </c>
       <c r="D429" t="s">
-        <v>1805</v>
+        <v>1786</v>
       </c>
       <c r="E429" t="s">
-        <v>1806</v>
+        <v>1787</v>
       </c>
       <c r="F429" t="s">
         <v>597</v>

</xml_diff>